<commit_message>
STATE 1 Scenario, Success Criteria Draft
STATE 1 Scenario, Success Criteria Draft
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SERVERMS30\usuarios$\secundaria\nicolas.philippe\Documents\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE13C17-622A-4C6F-8E12-B80AEC75E148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE8153E-864D-4195-9E44-738731C73DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7A099F99-E375-42D1-8638-50EE409111F1}"/>
   </bookViews>
@@ -36,37 +36,407 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
   <si>
+    <t>Planned Action</t>
+  </si>
+  <si>
+    <t>Planned Outcome</t>
+  </si>
+  <si>
     <t>Criterion</t>
   </si>
   <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>01/15/2025</t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>Criterion A: Planning</t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
+    <t>30 mn</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Discuss project goals and requirements with stakeholders</t>
+  </si>
+  <si>
+    <t>Interview to Discuss project goals and requirements with my uncle</t>
+  </si>
+  <si>
     <t>Duration</t>
   </si>
   <si>
     <t>Completion Date</t>
   </si>
   <si>
-    <t>Outcome</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Planned Date</t>
+    <t>Draft explaining the scenario</t>
+  </si>
+  <si>
+    <t>Meeting with my uncle to Review of the draft for scenario and criteria</t>
+  </si>
+  <si>
+    <t>Meeting with my uncle to validate of the  scenario and criteria</t>
+  </si>
+  <si>
+    <t>success criteria and scenario refinment</t>
+  </si>
+  <si>
+    <t>5 hours</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> success criteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (detailed above)</t>
+    </r>
+  </si>
+  <si>
+    <t>01/14/2025</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> success criteria </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>notes,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> functional solution </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>notes,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> notes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> success criteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> draft,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> functional solution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> draft, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> draft</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> success criteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> revised,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> functional solution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> revised, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> revised</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> success criteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> proposal,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> functional solution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> proposal, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> proposal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> success criteria draft </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">validated </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>,functional solution draft</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> validated, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>scenario draft</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> validated</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,16 +451,59 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -98,17 +511,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D9F25E-CBEA-4A45-8035-2BB081C2D9E7}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,36 +924,161 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" customWidth="1"/>
     <col min="3" max="3" width="58.5703125" customWidth="1"/>
-    <col min="4" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="50.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="E3" s="12">
+        <v>45839</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="13">
+        <v>45931</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13">
+        <v>45992</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" s="7" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" s="7" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
State 6 Implementation v1.0.1 - model - db mockup
State 6 Implementation v1.0.1 - model - db mockup
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="RVwEeOQSB5fKmoCyScIGp+h8/eELNMaHyveNNYHJtvM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="M52kuVW8mRZN8chrqIoPPkCVHra5SFvKktRC6XPmuMg="/>
     </ext>
   </extLst>
 </workbook>
@@ -1922,7 +1922,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1994,11 +1994,6 @@
       <sz val="11.0"/>
       <color rgb="FFC00000"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF156082"/>
-      <name val="Quattrocento Sans"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -2106,7 +2101,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2304,9 +2299,6 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -2327,7 +2319,7 @@
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -4083,47 +4075,47 @@
       <c r="D41" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="73"/>
+      <c r="E41" s="9"/>
       <c r="F41" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G41" s="74"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="75"/>
-      <c r="N41" s="75"/>
-      <c r="O41" s="75"/>
-      <c r="P41" s="75"/>
-      <c r="Q41" s="75"/>
-      <c r="R41" s="75"/>
-      <c r="S41" s="75"/>
-      <c r="T41" s="75"/>
-      <c r="U41" s="75"/>
-      <c r="V41" s="75"/>
-      <c r="W41" s="75"/>
-      <c r="X41" s="75"/>
-      <c r="Y41" s="75"/>
-      <c r="Z41" s="75"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="74"/>
+      <c r="L41" s="74"/>
+      <c r="M41" s="74"/>
+      <c r="N41" s="74"/>
+      <c r="O41" s="74"/>
+      <c r="P41" s="74"/>
+      <c r="Q41" s="74"/>
+      <c r="R41" s="74"/>
+      <c r="S41" s="74"/>
+      <c r="T41" s="74"/>
+      <c r="U41" s="74"/>
+      <c r="V41" s="74"/>
+      <c r="W41" s="74"/>
+      <c r="X41" s="74"/>
+      <c r="Y41" s="74"/>
+      <c r="Z41" s="74"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="76"/>
-      <c r="B42" s="76"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="78"/>
+      <c r="A42" s="75"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="77"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="76"/>
-      <c r="B43" s="76"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="78"/>
+      <c r="A43" s="75"/>
+      <c r="B43" s="75"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="77"/>
       <c r="G43" s="5"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -4178,26 +4170,26 @@
       <c r="F48" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G48" s="79"/>
-      <c r="H48" s="80"/>
-      <c r="I48" s="80"/>
-      <c r="J48" s="80"/>
-      <c r="K48" s="80"/>
-      <c r="L48" s="80"/>
-      <c r="M48" s="80"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="80"/>
-      <c r="P48" s="80"/>
-      <c r="Q48" s="80"/>
-      <c r="R48" s="80"/>
-      <c r="S48" s="80"/>
-      <c r="T48" s="80"/>
-      <c r="U48" s="80"/>
-      <c r="V48" s="80"/>
-      <c r="W48" s="80"/>
-      <c r="X48" s="80"/>
-      <c r="Y48" s="80"/>
-      <c r="Z48" s="80"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="79"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="79"/>
+      <c r="M48" s="79"/>
+      <c r="N48" s="79"/>
+      <c r="O48" s="79"/>
+      <c r="P48" s="79"/>
+      <c r="Q48" s="79"/>
+      <c r="R48" s="79"/>
+      <c r="S48" s="79"/>
+      <c r="T48" s="79"/>
+      <c r="U48" s="79"/>
+      <c r="V48" s="79"/>
+      <c r="W48" s="79"/>
+      <c r="X48" s="79"/>
+      <c r="Y48" s="79"/>
+      <c r="Z48" s="79"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="45" t="s">
@@ -4206,7 +4198,7 @@
       <c r="B49" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="C49" s="81" t="s">
+      <c r="C49" s="80" t="s">
         <v>146</v>
       </c>
       <c r="D49" s="45" t="s">
@@ -4216,26 +4208,26 @@
       <c r="F49" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G49" s="79"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="80"/>
-      <c r="J49" s="80"/>
-      <c r="K49" s="80"/>
-      <c r="L49" s="80"/>
-      <c r="M49" s="80"/>
-      <c r="N49" s="80"/>
-      <c r="O49" s="80"/>
-      <c r="P49" s="80"/>
-      <c r="Q49" s="80"/>
-      <c r="R49" s="80"/>
-      <c r="S49" s="80"/>
-      <c r="T49" s="80"/>
-      <c r="U49" s="80"/>
-      <c r="V49" s="80"/>
-      <c r="W49" s="80"/>
-      <c r="X49" s="80"/>
-      <c r="Y49" s="80"/>
-      <c r="Z49" s="80"/>
+      <c r="G49" s="78"/>
+      <c r="H49" s="79"/>
+      <c r="I49" s="79"/>
+      <c r="J49" s="79"/>
+      <c r="K49" s="79"/>
+      <c r="L49" s="79"/>
+      <c r="M49" s="79"/>
+      <c r="N49" s="79"/>
+      <c r="O49" s="79"/>
+      <c r="P49" s="79"/>
+      <c r="Q49" s="79"/>
+      <c r="R49" s="79"/>
+      <c r="S49" s="79"/>
+      <c r="T49" s="79"/>
+      <c r="U49" s="79"/>
+      <c r="V49" s="79"/>
+      <c r="W49" s="79"/>
+      <c r="X49" s="79"/>
+      <c r="Y49" s="79"/>
+      <c r="Z49" s="79"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="45" t="s">
@@ -4254,26 +4246,26 @@
       <c r="F50" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="G50" s="79"/>
-      <c r="H50" s="80"/>
-      <c r="I50" s="80"/>
-      <c r="J50" s="80"/>
-      <c r="K50" s="80"/>
-      <c r="L50" s="80"/>
-      <c r="M50" s="80"/>
-      <c r="N50" s="80"/>
-      <c r="O50" s="80"/>
-      <c r="P50" s="80"/>
-      <c r="Q50" s="80"/>
-      <c r="R50" s="80"/>
-      <c r="S50" s="80"/>
-      <c r="T50" s="80"/>
-      <c r="U50" s="80"/>
-      <c r="V50" s="80"/>
-      <c r="W50" s="80"/>
-      <c r="X50" s="80"/>
-      <c r="Y50" s="80"/>
-      <c r="Z50" s="80"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="79"/>
+      <c r="J50" s="79"/>
+      <c r="K50" s="79"/>
+      <c r="L50" s="79"/>
+      <c r="M50" s="79"/>
+      <c r="N50" s="79"/>
+      <c r="O50" s="79"/>
+      <c r="P50" s="79"/>
+      <c r="Q50" s="79"/>
+      <c r="R50" s="79"/>
+      <c r="S50" s="79"/>
+      <c r="T50" s="79"/>
+      <c r="U50" s="79"/>
+      <c r="V50" s="79"/>
+      <c r="W50" s="79"/>
+      <c r="X50" s="79"/>
+      <c r="Y50" s="79"/>
+      <c r="Z50" s="79"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="45" t="s">
@@ -4282,7 +4274,7 @@
       <c r="B51" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="C51" s="81" t="s">
+      <c r="C51" s="80" t="s">
         <v>154</v>
       </c>
       <c r="D51" s="45" t="s">
@@ -4292,26 +4284,26 @@
       <c r="F51" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G51" s="79"/>
-      <c r="H51" s="80"/>
-      <c r="I51" s="80"/>
-      <c r="J51" s="80"/>
-      <c r="K51" s="80"/>
-      <c r="L51" s="80"/>
-      <c r="M51" s="80"/>
-      <c r="N51" s="80"/>
-      <c r="O51" s="80"/>
-      <c r="P51" s="80"/>
-      <c r="Q51" s="80"/>
-      <c r="R51" s="80"/>
-      <c r="S51" s="80"/>
-      <c r="T51" s="80"/>
-      <c r="U51" s="80"/>
-      <c r="V51" s="80"/>
-      <c r="W51" s="80"/>
-      <c r="X51" s="80"/>
-      <c r="Y51" s="80"/>
-      <c r="Z51" s="80"/>
+      <c r="G51" s="78"/>
+      <c r="H51" s="79"/>
+      <c r="I51" s="79"/>
+      <c r="J51" s="79"/>
+      <c r="K51" s="79"/>
+      <c r="L51" s="79"/>
+      <c r="M51" s="79"/>
+      <c r="N51" s="79"/>
+      <c r="O51" s="79"/>
+      <c r="P51" s="79"/>
+      <c r="Q51" s="79"/>
+      <c r="R51" s="79"/>
+      <c r="S51" s="79"/>
+      <c r="T51" s="79"/>
+      <c r="U51" s="79"/>
+      <c r="V51" s="79"/>
+      <c r="W51" s="79"/>
+      <c r="X51" s="79"/>
+      <c r="Y51" s="79"/>
+      <c r="Z51" s="79"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="45" t="s">
@@ -4330,26 +4322,26 @@
       <c r="F52" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="G52" s="79"/>
-      <c r="H52" s="80"/>
-      <c r="I52" s="80"/>
-      <c r="J52" s="80"/>
-      <c r="K52" s="80"/>
-      <c r="L52" s="80"/>
-      <c r="M52" s="80"/>
-      <c r="N52" s="80"/>
-      <c r="O52" s="80"/>
-      <c r="P52" s="80"/>
-      <c r="Q52" s="80"/>
-      <c r="R52" s="80"/>
-      <c r="S52" s="80"/>
-      <c r="T52" s="80"/>
-      <c r="U52" s="80"/>
-      <c r="V52" s="80"/>
-      <c r="W52" s="80"/>
-      <c r="X52" s="80"/>
-      <c r="Y52" s="80"/>
-      <c r="Z52" s="80"/>
+      <c r="G52" s="78"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="79"/>
+      <c r="K52" s="79"/>
+      <c r="L52" s="79"/>
+      <c r="M52" s="79"/>
+      <c r="N52" s="79"/>
+      <c r="O52" s="79"/>
+      <c r="P52" s="79"/>
+      <c r="Q52" s="79"/>
+      <c r="R52" s="79"/>
+      <c r="S52" s="79"/>
+      <c r="T52" s="79"/>
+      <c r="U52" s="79"/>
+      <c r="V52" s="79"/>
+      <c r="W52" s="79"/>
+      <c r="X52" s="79"/>
+      <c r="Y52" s="79"/>
+      <c r="Z52" s="79"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="45" t="s">
@@ -4358,7 +4350,7 @@
       <c r="B53" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="81" t="s">
+      <c r="C53" s="80" t="s">
         <v>159</v>
       </c>
       <c r="D53" s="45" t="s">
@@ -4368,26 +4360,26 @@
       <c r="F53" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G53" s="79"/>
-      <c r="H53" s="80"/>
-      <c r="I53" s="80"/>
-      <c r="J53" s="80"/>
-      <c r="K53" s="80"/>
-      <c r="L53" s="80"/>
-      <c r="M53" s="80"/>
-      <c r="N53" s="80"/>
-      <c r="O53" s="80"/>
-      <c r="P53" s="80"/>
-      <c r="Q53" s="80"/>
-      <c r="R53" s="80"/>
-      <c r="S53" s="80"/>
-      <c r="T53" s="80"/>
-      <c r="U53" s="80"/>
-      <c r="V53" s="80"/>
-      <c r="W53" s="80"/>
-      <c r="X53" s="80"/>
-      <c r="Y53" s="80"/>
-      <c r="Z53" s="80"/>
+      <c r="G53" s="78"/>
+      <c r="H53" s="79"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="79"/>
+      <c r="K53" s="79"/>
+      <c r="L53" s="79"/>
+      <c r="M53" s="79"/>
+      <c r="N53" s="79"/>
+      <c r="O53" s="79"/>
+      <c r="P53" s="79"/>
+      <c r="Q53" s="79"/>
+      <c r="R53" s="79"/>
+      <c r="S53" s="79"/>
+      <c r="T53" s="79"/>
+      <c r="U53" s="79"/>
+      <c r="V53" s="79"/>
+      <c r="W53" s="79"/>
+      <c r="X53" s="79"/>
+      <c r="Y53" s="79"/>
+      <c r="Z53" s="79"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="45" t="s">
@@ -4406,26 +4398,26 @@
       <c r="F54" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="G54" s="79"/>
-      <c r="H54" s="80"/>
-      <c r="I54" s="80"/>
-      <c r="J54" s="80"/>
-      <c r="K54" s="80"/>
-      <c r="L54" s="80"/>
-      <c r="M54" s="80"/>
-      <c r="N54" s="80"/>
-      <c r="O54" s="80"/>
-      <c r="P54" s="80"/>
-      <c r="Q54" s="80"/>
-      <c r="R54" s="80"/>
-      <c r="S54" s="80"/>
-      <c r="T54" s="80"/>
-      <c r="U54" s="80"/>
-      <c r="V54" s="80"/>
-      <c r="W54" s="80"/>
-      <c r="X54" s="80"/>
-      <c r="Y54" s="80"/>
-      <c r="Z54" s="80"/>
+      <c r="G54" s="78"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="79"/>
+      <c r="J54" s="79"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="79"/>
+      <c r="N54" s="79"/>
+      <c r="O54" s="79"/>
+      <c r="P54" s="79"/>
+      <c r="Q54" s="79"/>
+      <c r="R54" s="79"/>
+      <c r="S54" s="79"/>
+      <c r="T54" s="79"/>
+      <c r="U54" s="79"/>
+      <c r="V54" s="79"/>
+      <c r="W54" s="79"/>
+      <c r="X54" s="79"/>
+      <c r="Y54" s="79"/>
+      <c r="Z54" s="79"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="45" t="s">
@@ -4434,7 +4426,7 @@
       <c r="B55" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="C55" s="82" t="s">
+      <c r="C55" s="81" t="s">
         <v>164</v>
       </c>
       <c r="D55" s="45" t="s">
@@ -4444,26 +4436,26 @@
       <c r="F55" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="G55" s="79"/>
-      <c r="H55" s="80"/>
-      <c r="I55" s="80"/>
-      <c r="J55" s="80"/>
-      <c r="K55" s="80"/>
-      <c r="L55" s="80"/>
-      <c r="M55" s="80"/>
-      <c r="N55" s="80"/>
-      <c r="O55" s="80"/>
-      <c r="P55" s="80"/>
-      <c r="Q55" s="80"/>
-      <c r="R55" s="80"/>
-      <c r="S55" s="80"/>
-      <c r="T55" s="80"/>
-      <c r="U55" s="80"/>
-      <c r="V55" s="80"/>
-      <c r="W55" s="80"/>
-      <c r="X55" s="80"/>
-      <c r="Y55" s="80"/>
-      <c r="Z55" s="80"/>
+      <c r="G55" s="78"/>
+      <c r="H55" s="79"/>
+      <c r="I55" s="79"/>
+      <c r="J55" s="79"/>
+      <c r="K55" s="79"/>
+      <c r="L55" s="79"/>
+      <c r="M55" s="79"/>
+      <c r="N55" s="79"/>
+      <c r="O55" s="79"/>
+      <c r="P55" s="79"/>
+      <c r="Q55" s="79"/>
+      <c r="R55" s="79"/>
+      <c r="S55" s="79"/>
+      <c r="T55" s="79"/>
+      <c r="U55" s="79"/>
+      <c r="V55" s="79"/>
+      <c r="W55" s="79"/>
+      <c r="X55" s="79"/>
+      <c r="Y55" s="79"/>
+      <c r="Z55" s="79"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="45" t="s">
@@ -4482,26 +4474,26 @@
       <c r="F56" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="G56" s="79"/>
-      <c r="H56" s="80"/>
-      <c r="I56" s="80"/>
-      <c r="J56" s="80"/>
-      <c r="K56" s="80"/>
-      <c r="L56" s="80"/>
-      <c r="M56" s="80"/>
-      <c r="N56" s="80"/>
-      <c r="O56" s="80"/>
-      <c r="P56" s="80"/>
-      <c r="Q56" s="80"/>
-      <c r="R56" s="80"/>
-      <c r="S56" s="80"/>
-      <c r="T56" s="80"/>
-      <c r="U56" s="80"/>
-      <c r="V56" s="80"/>
-      <c r="W56" s="80"/>
-      <c r="X56" s="80"/>
-      <c r="Y56" s="80"/>
-      <c r="Z56" s="80"/>
+      <c r="G56" s="78"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="79"/>
+      <c r="J56" s="79"/>
+      <c r="K56" s="79"/>
+      <c r="L56" s="79"/>
+      <c r="M56" s="79"/>
+      <c r="N56" s="79"/>
+      <c r="O56" s="79"/>
+      <c r="P56" s="79"/>
+      <c r="Q56" s="79"/>
+      <c r="R56" s="79"/>
+      <c r="S56" s="79"/>
+      <c r="T56" s="79"/>
+      <c r="U56" s="79"/>
+      <c r="V56" s="79"/>
+      <c r="W56" s="79"/>
+      <c r="X56" s="79"/>
+      <c r="Y56" s="79"/>
+      <c r="Z56" s="79"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="45" t="s">
@@ -4510,7 +4502,7 @@
       <c r="B57" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="C57" s="82" t="s">
+      <c r="C57" s="81" t="s">
         <v>168</v>
       </c>
       <c r="D57" s="45" t="s">
@@ -4520,26 +4512,26 @@
       <c r="F57" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="G57" s="79"/>
-      <c r="H57" s="80"/>
-      <c r="I57" s="80"/>
-      <c r="J57" s="80"/>
-      <c r="K57" s="80"/>
-      <c r="L57" s="80"/>
-      <c r="M57" s="80"/>
-      <c r="N57" s="80"/>
-      <c r="O57" s="80"/>
-      <c r="P57" s="80"/>
-      <c r="Q57" s="80"/>
-      <c r="R57" s="80"/>
-      <c r="S57" s="80"/>
-      <c r="T57" s="80"/>
-      <c r="U57" s="80"/>
-      <c r="V57" s="80"/>
-      <c r="W57" s="80"/>
-      <c r="X57" s="80"/>
-      <c r="Y57" s="80"/>
-      <c r="Z57" s="80"/>
+      <c r="G57" s="78"/>
+      <c r="H57" s="79"/>
+      <c r="I57" s="79"/>
+      <c r="J57" s="79"/>
+      <c r="K57" s="79"/>
+      <c r="L57" s="79"/>
+      <c r="M57" s="79"/>
+      <c r="N57" s="79"/>
+      <c r="O57" s="79"/>
+      <c r="P57" s="79"/>
+      <c r="Q57" s="79"/>
+      <c r="R57" s="79"/>
+      <c r="S57" s="79"/>
+      <c r="T57" s="79"/>
+      <c r="U57" s="79"/>
+      <c r="V57" s="79"/>
+      <c r="W57" s="79"/>
+      <c r="X57" s="79"/>
+      <c r="Y57" s="79"/>
+      <c r="Z57" s="79"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="45" t="s">
@@ -4558,26 +4550,26 @@
       <c r="F58" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="G58" s="79"/>
-      <c r="H58" s="80"/>
-      <c r="I58" s="80"/>
-      <c r="J58" s="80"/>
-      <c r="K58" s="80"/>
-      <c r="L58" s="80"/>
-      <c r="M58" s="80"/>
-      <c r="N58" s="80"/>
-      <c r="O58" s="80"/>
-      <c r="P58" s="80"/>
-      <c r="Q58" s="80"/>
-      <c r="R58" s="80"/>
-      <c r="S58" s="80"/>
-      <c r="T58" s="80"/>
-      <c r="U58" s="80"/>
-      <c r="V58" s="80"/>
-      <c r="W58" s="80"/>
-      <c r="X58" s="80"/>
-      <c r="Y58" s="80"/>
-      <c r="Z58" s="80"/>
+      <c r="G58" s="78"/>
+      <c r="H58" s="79"/>
+      <c r="I58" s="79"/>
+      <c r="J58" s="79"/>
+      <c r="K58" s="79"/>
+      <c r="L58" s="79"/>
+      <c r="M58" s="79"/>
+      <c r="N58" s="79"/>
+      <c r="O58" s="79"/>
+      <c r="P58" s="79"/>
+      <c r="Q58" s="79"/>
+      <c r="R58" s="79"/>
+      <c r="S58" s="79"/>
+      <c r="T58" s="79"/>
+      <c r="U58" s="79"/>
+      <c r="V58" s="79"/>
+      <c r="W58" s="79"/>
+      <c r="X58" s="79"/>
+      <c r="Y58" s="79"/>
+      <c r="Z58" s="79"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="45" t="s">
@@ -4596,26 +4588,26 @@
       <c r="F59" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="G59" s="79"/>
-      <c r="H59" s="80"/>
-      <c r="I59" s="80"/>
-      <c r="J59" s="80"/>
-      <c r="K59" s="80"/>
-      <c r="L59" s="80"/>
-      <c r="M59" s="80"/>
-      <c r="N59" s="80"/>
-      <c r="O59" s="80"/>
-      <c r="P59" s="80"/>
-      <c r="Q59" s="80"/>
-      <c r="R59" s="80"/>
-      <c r="S59" s="80"/>
-      <c r="T59" s="80"/>
-      <c r="U59" s="80"/>
-      <c r="V59" s="80"/>
-      <c r="W59" s="80"/>
-      <c r="X59" s="80"/>
-      <c r="Y59" s="80"/>
-      <c r="Z59" s="80"/>
+      <c r="G59" s="78"/>
+      <c r="H59" s="79"/>
+      <c r="I59" s="79"/>
+      <c r="J59" s="79"/>
+      <c r="K59" s="79"/>
+      <c r="L59" s="79"/>
+      <c r="M59" s="79"/>
+      <c r="N59" s="79"/>
+      <c r="O59" s="79"/>
+      <c r="P59" s="79"/>
+      <c r="Q59" s="79"/>
+      <c r="R59" s="79"/>
+      <c r="S59" s="79"/>
+      <c r="T59" s="79"/>
+      <c r="U59" s="79"/>
+      <c r="V59" s="79"/>
+      <c r="W59" s="79"/>
+      <c r="X59" s="79"/>
+      <c r="Y59" s="79"/>
+      <c r="Z59" s="79"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="4"/>
@@ -4657,7 +4649,7 @@
       <c r="B64" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="C64" s="81" t="s">
+      <c r="C64" s="80" t="s">
         <v>173</v>
       </c>
       <c r="D64" s="45" t="s">
@@ -4667,26 +4659,26 @@
       <c r="F64" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G64" s="79"/>
-      <c r="H64" s="80"/>
-      <c r="I64" s="80"/>
-      <c r="J64" s="80"/>
-      <c r="K64" s="80"/>
-      <c r="L64" s="80"/>
-      <c r="M64" s="80"/>
-      <c r="N64" s="80"/>
-      <c r="O64" s="80"/>
-      <c r="P64" s="80"/>
-      <c r="Q64" s="80"/>
-      <c r="R64" s="80"/>
-      <c r="S64" s="80"/>
-      <c r="T64" s="80"/>
-      <c r="U64" s="80"/>
-      <c r="V64" s="80"/>
-      <c r="W64" s="80"/>
-      <c r="X64" s="80"/>
-      <c r="Y64" s="80"/>
-      <c r="Z64" s="80"/>
+      <c r="G64" s="78"/>
+      <c r="H64" s="79"/>
+      <c r="I64" s="79"/>
+      <c r="J64" s="79"/>
+      <c r="K64" s="79"/>
+      <c r="L64" s="79"/>
+      <c r="M64" s="79"/>
+      <c r="N64" s="79"/>
+      <c r="O64" s="79"/>
+      <c r="P64" s="79"/>
+      <c r="Q64" s="79"/>
+      <c r="R64" s="79"/>
+      <c r="S64" s="79"/>
+      <c r="T64" s="79"/>
+      <c r="U64" s="79"/>
+      <c r="V64" s="79"/>
+      <c r="W64" s="79"/>
+      <c r="X64" s="79"/>
+      <c r="Y64" s="79"/>
+      <c r="Z64" s="79"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="45" t="s">
@@ -4695,7 +4687,7 @@
       <c r="B65" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="C65" s="81" t="s">
+      <c r="C65" s="80" t="s">
         <v>176</v>
       </c>
       <c r="D65" s="45" t="s">
@@ -4708,25 +4700,25 @@
       <c r="G65" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="H65" s="80"/>
-      <c r="I65" s="80"/>
-      <c r="J65" s="80"/>
-      <c r="K65" s="80"/>
-      <c r="L65" s="80"/>
-      <c r="M65" s="80"/>
-      <c r="N65" s="80"/>
-      <c r="O65" s="80"/>
-      <c r="P65" s="80"/>
-      <c r="Q65" s="80"/>
-      <c r="R65" s="80"/>
-      <c r="S65" s="80"/>
-      <c r="T65" s="80"/>
-      <c r="U65" s="80"/>
-      <c r="V65" s="80"/>
-      <c r="W65" s="80"/>
-      <c r="X65" s="80"/>
-      <c r="Y65" s="80"/>
-      <c r="Z65" s="80"/>
+      <c r="H65" s="79"/>
+      <c r="I65" s="79"/>
+      <c r="J65" s="79"/>
+      <c r="K65" s="79"/>
+      <c r="L65" s="79"/>
+      <c r="M65" s="79"/>
+      <c r="N65" s="79"/>
+      <c r="O65" s="79"/>
+      <c r="P65" s="79"/>
+      <c r="Q65" s="79"/>
+      <c r="R65" s="79"/>
+      <c r="S65" s="79"/>
+      <c r="T65" s="79"/>
+      <c r="U65" s="79"/>
+      <c r="V65" s="79"/>
+      <c r="W65" s="79"/>
+      <c r="X65" s="79"/>
+      <c r="Y65" s="79"/>
+      <c r="Z65" s="79"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="45" t="s">
@@ -4735,7 +4727,7 @@
       <c r="B66" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="81" t="s">
+      <c r="C66" s="80" t="s">
         <v>179</v>
       </c>
       <c r="D66" s="45" t="s">
@@ -4748,25 +4740,25 @@
       <c r="G66" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="H66" s="80"/>
-      <c r="I66" s="80"/>
-      <c r="J66" s="80"/>
-      <c r="K66" s="80"/>
-      <c r="L66" s="80"/>
-      <c r="M66" s="80"/>
-      <c r="N66" s="80"/>
-      <c r="O66" s="80"/>
-      <c r="P66" s="80"/>
-      <c r="Q66" s="80"/>
-      <c r="R66" s="80"/>
-      <c r="S66" s="80"/>
-      <c r="T66" s="80"/>
-      <c r="U66" s="80"/>
-      <c r="V66" s="80"/>
-      <c r="W66" s="80"/>
-      <c r="X66" s="80"/>
-      <c r="Y66" s="80"/>
-      <c r="Z66" s="80"/>
+      <c r="H66" s="79"/>
+      <c r="I66" s="79"/>
+      <c r="J66" s="79"/>
+      <c r="K66" s="79"/>
+      <c r="L66" s="79"/>
+      <c r="M66" s="79"/>
+      <c r="N66" s="79"/>
+      <c r="O66" s="79"/>
+      <c r="P66" s="79"/>
+      <c r="Q66" s="79"/>
+      <c r="R66" s="79"/>
+      <c r="S66" s="79"/>
+      <c r="T66" s="79"/>
+      <c r="U66" s="79"/>
+      <c r="V66" s="79"/>
+      <c r="W66" s="79"/>
+      <c r="X66" s="79"/>
+      <c r="Y66" s="79"/>
+      <c r="Z66" s="79"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="45" t="s">
@@ -4781,30 +4773,30 @@
       <c r="D67" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E67" s="83"/>
+      <c r="E67" s="82"/>
       <c r="F67" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="G67" s="79"/>
-      <c r="H67" s="80"/>
-      <c r="I67" s="80"/>
-      <c r="J67" s="80"/>
-      <c r="K67" s="80"/>
-      <c r="L67" s="80"/>
-      <c r="M67" s="80"/>
-      <c r="N67" s="80"/>
-      <c r="O67" s="80"/>
-      <c r="P67" s="80"/>
-      <c r="Q67" s="80"/>
-      <c r="R67" s="80"/>
-      <c r="S67" s="80"/>
-      <c r="T67" s="80"/>
-      <c r="U67" s="80"/>
-      <c r="V67" s="80"/>
-      <c r="W67" s="80"/>
-      <c r="X67" s="80"/>
-      <c r="Y67" s="80"/>
-      <c r="Z67" s="80"/>
+      <c r="G67" s="78"/>
+      <c r="H67" s="79"/>
+      <c r="I67" s="79"/>
+      <c r="J67" s="79"/>
+      <c r="K67" s="79"/>
+      <c r="L67" s="79"/>
+      <c r="M67" s="79"/>
+      <c r="N67" s="79"/>
+      <c r="O67" s="79"/>
+      <c r="P67" s="79"/>
+      <c r="Q67" s="79"/>
+      <c r="R67" s="79"/>
+      <c r="S67" s="79"/>
+      <c r="T67" s="79"/>
+      <c r="U67" s="79"/>
+      <c r="V67" s="79"/>
+      <c r="W67" s="79"/>
+      <c r="X67" s="79"/>
+      <c r="Y67" s="79"/>
+      <c r="Z67" s="79"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="45" t="s">
@@ -4819,30 +4811,30 @@
       <c r="D68" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="E68" s="83"/>
+      <c r="E68" s="82"/>
       <c r="F68" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="G68" s="79"/>
-      <c r="H68" s="80"/>
-      <c r="I68" s="80"/>
-      <c r="J68" s="80"/>
-      <c r="K68" s="80"/>
-      <c r="L68" s="80"/>
-      <c r="M68" s="80"/>
-      <c r="N68" s="80"/>
-      <c r="O68" s="80"/>
-      <c r="P68" s="80"/>
-      <c r="Q68" s="80"/>
-      <c r="R68" s="80"/>
-      <c r="S68" s="80"/>
-      <c r="T68" s="80"/>
-      <c r="U68" s="80"/>
-      <c r="V68" s="80"/>
-      <c r="W68" s="80"/>
-      <c r="X68" s="80"/>
-      <c r="Y68" s="80"/>
-      <c r="Z68" s="80"/>
+      <c r="G68" s="78"/>
+      <c r="H68" s="79"/>
+      <c r="I68" s="79"/>
+      <c r="J68" s="79"/>
+      <c r="K68" s="79"/>
+      <c r="L68" s="79"/>
+      <c r="M68" s="79"/>
+      <c r="N68" s="79"/>
+      <c r="O68" s="79"/>
+      <c r="P68" s="79"/>
+      <c r="Q68" s="79"/>
+      <c r="R68" s="79"/>
+      <c r="S68" s="79"/>
+      <c r="T68" s="79"/>
+      <c r="U68" s="79"/>
+      <c r="V68" s="79"/>
+      <c r="W68" s="79"/>
+      <c r="X68" s="79"/>
+      <c r="Y68" s="79"/>
+      <c r="Z68" s="79"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="45" t="s">
@@ -4851,7 +4843,7 @@
       <c r="B69" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="C69" s="81" t="s">
+      <c r="C69" s="80" t="s">
         <v>190</v>
       </c>
       <c r="D69" s="45" t="s">
@@ -4861,26 +4853,26 @@
       <c r="F69" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="G69" s="79"/>
-      <c r="H69" s="80"/>
-      <c r="I69" s="80"/>
-      <c r="J69" s="80"/>
-      <c r="K69" s="80"/>
-      <c r="L69" s="80"/>
-      <c r="M69" s="80"/>
-      <c r="N69" s="80"/>
-      <c r="O69" s="80"/>
-      <c r="P69" s="80"/>
-      <c r="Q69" s="80"/>
-      <c r="R69" s="80"/>
-      <c r="S69" s="80"/>
-      <c r="T69" s="80"/>
-      <c r="U69" s="80"/>
-      <c r="V69" s="80"/>
-      <c r="W69" s="80"/>
-      <c r="X69" s="80"/>
-      <c r="Y69" s="80"/>
-      <c r="Z69" s="80"/>
+      <c r="G69" s="78"/>
+      <c r="H69" s="79"/>
+      <c r="I69" s="79"/>
+      <c r="J69" s="79"/>
+      <c r="K69" s="79"/>
+      <c r="L69" s="79"/>
+      <c r="M69" s="79"/>
+      <c r="N69" s="79"/>
+      <c r="O69" s="79"/>
+      <c r="P69" s="79"/>
+      <c r="Q69" s="79"/>
+      <c r="R69" s="79"/>
+      <c r="S69" s="79"/>
+      <c r="T69" s="79"/>
+      <c r="U69" s="79"/>
+      <c r="V69" s="79"/>
+      <c r="W69" s="79"/>
+      <c r="X69" s="79"/>
+      <c r="Y69" s="79"/>
+      <c r="Z69" s="79"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="45" t="s">
@@ -4895,30 +4887,30 @@
       <c r="D70" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E70" s="83"/>
+      <c r="E70" s="82"/>
       <c r="F70" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="G70" s="79"/>
-      <c r="H70" s="80"/>
-      <c r="I70" s="80"/>
-      <c r="J70" s="80"/>
-      <c r="K70" s="80"/>
-      <c r="L70" s="80"/>
-      <c r="M70" s="80"/>
-      <c r="N70" s="80"/>
-      <c r="O70" s="80"/>
-      <c r="P70" s="80"/>
-      <c r="Q70" s="80"/>
-      <c r="R70" s="80"/>
-      <c r="S70" s="80"/>
-      <c r="T70" s="80"/>
-      <c r="U70" s="80"/>
-      <c r="V70" s="80"/>
-      <c r="W70" s="80"/>
-      <c r="X70" s="80"/>
-      <c r="Y70" s="80"/>
-      <c r="Z70" s="80"/>
+      <c r="G70" s="78"/>
+      <c r="H70" s="79"/>
+      <c r="I70" s="79"/>
+      <c r="J70" s="79"/>
+      <c r="K70" s="79"/>
+      <c r="L70" s="79"/>
+      <c r="M70" s="79"/>
+      <c r="N70" s="79"/>
+      <c r="O70" s="79"/>
+      <c r="P70" s="79"/>
+      <c r="Q70" s="79"/>
+      <c r="R70" s="79"/>
+      <c r="S70" s="79"/>
+      <c r="T70" s="79"/>
+      <c r="U70" s="79"/>
+      <c r="V70" s="79"/>
+      <c r="W70" s="79"/>
+      <c r="X70" s="79"/>
+      <c r="Y70" s="79"/>
+      <c r="Z70" s="79"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="45" t="s">
@@ -4927,7 +4919,7 @@
       <c r="B71" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="C71" s="81" t="s">
+      <c r="C71" s="80" t="s">
         <v>196</v>
       </c>
       <c r="D71" s="45" t="s">
@@ -4937,26 +4929,26 @@
       <c r="F71" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="G71" s="79"/>
-      <c r="H71" s="80"/>
-      <c r="I71" s="80"/>
-      <c r="J71" s="80"/>
-      <c r="K71" s="80"/>
-      <c r="L71" s="80"/>
-      <c r="M71" s="80"/>
-      <c r="N71" s="80"/>
-      <c r="O71" s="80"/>
-      <c r="P71" s="80"/>
-      <c r="Q71" s="80"/>
-      <c r="R71" s="80"/>
-      <c r="S71" s="80"/>
-      <c r="T71" s="80"/>
-      <c r="U71" s="80"/>
-      <c r="V71" s="80"/>
-      <c r="W71" s="80"/>
-      <c r="X71" s="80"/>
-      <c r="Y71" s="80"/>
-      <c r="Z71" s="80"/>
+      <c r="G71" s="78"/>
+      <c r="H71" s="79"/>
+      <c r="I71" s="79"/>
+      <c r="J71" s="79"/>
+      <c r="K71" s="79"/>
+      <c r="L71" s="79"/>
+      <c r="M71" s="79"/>
+      <c r="N71" s="79"/>
+      <c r="O71" s="79"/>
+      <c r="P71" s="79"/>
+      <c r="Q71" s="79"/>
+      <c r="R71" s="79"/>
+      <c r="S71" s="79"/>
+      <c r="T71" s="79"/>
+      <c r="U71" s="79"/>
+      <c r="V71" s="79"/>
+      <c r="W71" s="79"/>
+      <c r="X71" s="79"/>
+      <c r="Y71" s="79"/>
+      <c r="Z71" s="79"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="45" t="s">
@@ -4975,26 +4967,26 @@
       <c r="F72" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="G72" s="79"/>
-      <c r="H72" s="80"/>
-      <c r="I72" s="80"/>
-      <c r="J72" s="80"/>
-      <c r="K72" s="80"/>
-      <c r="L72" s="80"/>
-      <c r="M72" s="80"/>
-      <c r="N72" s="80"/>
-      <c r="O72" s="80"/>
-      <c r="P72" s="80"/>
-      <c r="Q72" s="80"/>
-      <c r="R72" s="80"/>
-      <c r="S72" s="80"/>
-      <c r="T72" s="80"/>
-      <c r="U72" s="80"/>
-      <c r="V72" s="80"/>
-      <c r="W72" s="80"/>
-      <c r="X72" s="80"/>
-      <c r="Y72" s="80"/>
-      <c r="Z72" s="80"/>
+      <c r="G72" s="78"/>
+      <c r="H72" s="79"/>
+      <c r="I72" s="79"/>
+      <c r="J72" s="79"/>
+      <c r="K72" s="79"/>
+      <c r="L72" s="79"/>
+      <c r="M72" s="79"/>
+      <c r="N72" s="79"/>
+      <c r="O72" s="79"/>
+      <c r="P72" s="79"/>
+      <c r="Q72" s="79"/>
+      <c r="R72" s="79"/>
+      <c r="S72" s="79"/>
+      <c r="T72" s="79"/>
+      <c r="U72" s="79"/>
+      <c r="V72" s="79"/>
+      <c r="W72" s="79"/>
+      <c r="X72" s="79"/>
+      <c r="Y72" s="79"/>
+      <c r="Z72" s="79"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="45" t="s">
@@ -5013,26 +5005,26 @@
       <c r="F73" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="G73" s="79"/>
-      <c r="H73" s="80"/>
-      <c r="I73" s="80"/>
-      <c r="J73" s="80"/>
-      <c r="K73" s="80"/>
-      <c r="L73" s="80"/>
-      <c r="M73" s="80"/>
-      <c r="N73" s="80"/>
-      <c r="O73" s="80"/>
-      <c r="P73" s="80"/>
-      <c r="Q73" s="80"/>
-      <c r="R73" s="80"/>
-      <c r="S73" s="80"/>
-      <c r="T73" s="80"/>
-      <c r="U73" s="80"/>
-      <c r="V73" s="80"/>
-      <c r="W73" s="80"/>
-      <c r="X73" s="80"/>
-      <c r="Y73" s="80"/>
-      <c r="Z73" s="80"/>
+      <c r="G73" s="78"/>
+      <c r="H73" s="79"/>
+      <c r="I73" s="79"/>
+      <c r="J73" s="79"/>
+      <c r="K73" s="79"/>
+      <c r="L73" s="79"/>
+      <c r="M73" s="79"/>
+      <c r="N73" s="79"/>
+      <c r="O73" s="79"/>
+      <c r="P73" s="79"/>
+      <c r="Q73" s="79"/>
+      <c r="R73" s="79"/>
+      <c r="S73" s="79"/>
+      <c r="T73" s="79"/>
+      <c r="U73" s="79"/>
+      <c r="V73" s="79"/>
+      <c r="W73" s="79"/>
+      <c r="X73" s="79"/>
+      <c r="Y73" s="79"/>
+      <c r="Z73" s="79"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="45" t="s">
@@ -5047,30 +5039,30 @@
       <c r="D74" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="E74" s="83"/>
+      <c r="E74" s="82"/>
       <c r="F74" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="G74" s="79"/>
-      <c r="H74" s="80"/>
-      <c r="I74" s="80"/>
-      <c r="J74" s="80"/>
-      <c r="K74" s="80"/>
-      <c r="L74" s="80"/>
-      <c r="M74" s="80"/>
-      <c r="N74" s="80"/>
-      <c r="O74" s="80"/>
-      <c r="P74" s="80"/>
-      <c r="Q74" s="80"/>
-      <c r="R74" s="80"/>
-      <c r="S74" s="80"/>
-      <c r="T74" s="80"/>
-      <c r="U74" s="80"/>
-      <c r="V74" s="80"/>
-      <c r="W74" s="80"/>
-      <c r="X74" s="80"/>
-      <c r="Y74" s="80"/>
-      <c r="Z74" s="80"/>
+      <c r="G74" s="78"/>
+      <c r="H74" s="79"/>
+      <c r="I74" s="79"/>
+      <c r="J74" s="79"/>
+      <c r="K74" s="79"/>
+      <c r="L74" s="79"/>
+      <c r="M74" s="79"/>
+      <c r="N74" s="79"/>
+      <c r="O74" s="79"/>
+      <c r="P74" s="79"/>
+      <c r="Q74" s="79"/>
+      <c r="R74" s="79"/>
+      <c r="S74" s="79"/>
+      <c r="T74" s="79"/>
+      <c r="U74" s="79"/>
+      <c r="V74" s="79"/>
+      <c r="W74" s="79"/>
+      <c r="X74" s="79"/>
+      <c r="Y74" s="79"/>
+      <c r="Z74" s="79"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="45" t="s">
@@ -5085,37 +5077,37 @@
       <c r="D75" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="E75" s="83"/>
+      <c r="E75" s="82"/>
       <c r="F75" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="G75" s="79"/>
-      <c r="H75" s="80"/>
-      <c r="I75" s="80"/>
-      <c r="J75" s="80"/>
-      <c r="K75" s="80"/>
-      <c r="L75" s="80"/>
-      <c r="M75" s="80"/>
-      <c r="N75" s="80"/>
-      <c r="O75" s="80"/>
-      <c r="P75" s="80"/>
-      <c r="Q75" s="80"/>
-      <c r="R75" s="80"/>
-      <c r="S75" s="80"/>
-      <c r="T75" s="80"/>
-      <c r="U75" s="80"/>
-      <c r="V75" s="80"/>
-      <c r="W75" s="80"/>
-      <c r="X75" s="80"/>
-      <c r="Y75" s="80"/>
-      <c r="Z75" s="80"/>
+      <c r="G75" s="78"/>
+      <c r="H75" s="79"/>
+      <c r="I75" s="79"/>
+      <c r="J75" s="79"/>
+      <c r="K75" s="79"/>
+      <c r="L75" s="79"/>
+      <c r="M75" s="79"/>
+      <c r="N75" s="79"/>
+      <c r="O75" s="79"/>
+      <c r="P75" s="79"/>
+      <c r="Q75" s="79"/>
+      <c r="R75" s="79"/>
+      <c r="S75" s="79"/>
+      <c r="T75" s="79"/>
+      <c r="U75" s="79"/>
+      <c r="V75" s="79"/>
+      <c r="W75" s="79"/>
+      <c r="X75" s="79"/>
+      <c r="Y75" s="79"/>
+      <c r="Z75" s="79"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="4"/>
       <c r="G76" s="5"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="84"/>
+      <c r="A77" s="83"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
State 6 Implementation v1.0.2 - model - DbId
State 6 Implementation v1.0.2 - model - DbId
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="M52kuVW8mRZN8chrqIoPPkCVHra5SFvKktRC6XPmuMg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="mSOLnJlHQS9tEmlAYMTMBf0i4q6yQ6CnumUiyuKYyXs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="204">
   <si>
     <t>Waterfall Methodology</t>
   </si>
@@ -1395,6 +1395,12 @@
       </rPr>
       <t xml:space="preserve"> that will acts as a database access  is implemented in JAVA to simulate database access in JAVA</t>
     </r>
+  </si>
+  <si>
+    <t>Implement inheritance for Db id and debug functionalies in Domain Model</t>
+  </si>
+  <si>
+    <t>Classes in model domain inherits the DbId class that implements db id and debug functionalities</t>
   </si>
   <si>
     <t>Development</t>
@@ -3911,97 +3917,99 @@
       <c r="Z36" s="42"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="65" t="s">
+      <c r="A37" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="65" t="s">
+      <c r="C37" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C37" s="65" t="s">
+      <c r="D37" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="43">
+        <v>45872.0</v>
+      </c>
+      <c r="F37" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="64"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="42"/>
+      <c r="Q37" s="42"/>
+      <c r="R37" s="42"/>
+      <c r="S37" s="42"/>
+      <c r="T37" s="42"/>
+      <c r="U37" s="42"/>
+      <c r="V37" s="42"/>
+      <c r="W37" s="42"/>
+      <c r="X37" s="42"/>
+      <c r="Y37" s="42"/>
+      <c r="Z37" s="42"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="65" t="s">
+      <c r="B38" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="67" t="s">
+      <c r="E38" s="66"/>
+      <c r="F38" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="G37" s="68"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="69"/>
-      <c r="N37" s="69"/>
-      <c r="O37" s="69"/>
-      <c r="P37" s="69"/>
-      <c r="Q37" s="69"/>
-      <c r="R37" s="69"/>
-      <c r="S37" s="69"/>
-      <c r="T37" s="69"/>
-      <c r="U37" s="69"/>
-      <c r="V37" s="69"/>
-      <c r="W37" s="69"/>
-      <c r="X37" s="69"/>
-      <c r="Y37" s="69"/>
-      <c r="Z37" s="69"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="70"/>
-      <c r="F38" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G38" s="71"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="72"/>
-      <c r="N38" s="72"/>
-      <c r="O38" s="72"/>
-      <c r="P38" s="72"/>
-      <c r="Q38" s="72"/>
-      <c r="R38" s="72"/>
-      <c r="S38" s="72"/>
-      <c r="T38" s="72"/>
-      <c r="U38" s="72"/>
-      <c r="V38" s="72"/>
-      <c r="W38" s="72"/>
-      <c r="X38" s="72"/>
-      <c r="Y38" s="72"/>
-      <c r="Z38" s="72"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
+      <c r="Q38" s="69"/>
+      <c r="R38" s="69"/>
+      <c r="S38" s="69"/>
+      <c r="T38" s="69"/>
+      <c r="U38" s="69"/>
+      <c r="V38" s="69"/>
+      <c r="W38" s="69"/>
+      <c r="X38" s="69"/>
+      <c r="Y38" s="69"/>
+      <c r="Z38" s="69"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="C39" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="26" t="s">
-        <v>128</v>
-      </c>
       <c r="D39" s="25" t="s">
-        <v>129</v>
+        <v>30</v>
       </c>
       <c r="E39" s="70"/>
       <c r="F39" s="28" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="G39" s="71"/>
       <c r="H39" s="72"/>
@@ -4026,20 +4034,20 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" s="25" t="s">
         <v>131</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>86</v>
       </c>
       <c r="E40" s="70"/>
       <c r="F40" s="28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G40" s="71"/>
       <c r="H40" s="72"/>
@@ -4063,51 +4071,80 @@
       <c r="Z40" s="72"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="D41" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="70"/>
+      <c r="F41" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="G41" s="71"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
+      <c r="K41" s="72"/>
+      <c r="L41" s="72"/>
+      <c r="M41" s="72"/>
+      <c r="N41" s="72"/>
+      <c r="O41" s="72"/>
+      <c r="P41" s="72"/>
+      <c r="Q41" s="72"/>
+      <c r="R41" s="72"/>
+      <c r="S41" s="72"/>
+      <c r="T41" s="72"/>
+      <c r="U41" s="72"/>
+      <c r="V41" s="72"/>
+      <c r="W41" s="72"/>
+      <c r="X41" s="72"/>
+      <c r="Y41" s="72"/>
+      <c r="Z41" s="72"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="B42" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="9"/>
-      <c r="F41" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="G41" s="73"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="74"/>
-      <c r="L41" s="74"/>
-      <c r="M41" s="74"/>
-      <c r="N41" s="74"/>
-      <c r="O41" s="74"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="74"/>
-      <c r="R41" s="74"/>
-      <c r="S41" s="74"/>
-      <c r="T41" s="74"/>
-      <c r="U41" s="74"/>
-      <c r="V41" s="74"/>
-      <c r="W41" s="74"/>
-      <c r="X41" s="74"/>
-      <c r="Y41" s="74"/>
-      <c r="Z41" s="74"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="75"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="5"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G42" s="73"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="74"/>
+      <c r="M42" s="74"/>
+      <c r="N42" s="74"/>
+      <c r="O42" s="74"/>
+      <c r="P42" s="74"/>
+      <c r="Q42" s="74"/>
+      <c r="R42" s="74"/>
+      <c r="S42" s="74"/>
+      <c r="T42" s="74"/>
+      <c r="U42" s="74"/>
+      <c r="V42" s="74"/>
+      <c r="W42" s="74"/>
+      <c r="X42" s="74"/>
+      <c r="Y42" s="74"/>
+      <c r="Z42" s="74"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="75"/>
@@ -4119,94 +4156,65 @@
       <c r="G43" s="5"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="4"/>
+      <c r="A44" s="75"/>
+      <c r="B44" s="75"/>
+      <c r="C44" s="75"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="77"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="A45" s="4"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="4"/>
+      <c r="A46" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="G46" s="5"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="4"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B48" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F47" s="7" t="s">
+      <c r="D48" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="5"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="C48" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="D48" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E48" s="45"/>
-      <c r="F48" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="78"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="79"/>
-      <c r="J48" s="79"/>
-      <c r="K48" s="79"/>
-      <c r="L48" s="79"/>
-      <c r="M48" s="79"/>
-      <c r="N48" s="79"/>
-      <c r="O48" s="79"/>
-      <c r="P48" s="79"/>
-      <c r="Q48" s="79"/>
-      <c r="R48" s="79"/>
-      <c r="S48" s="79"/>
-      <c r="T48" s="79"/>
-      <c r="U48" s="79"/>
-      <c r="V48" s="79"/>
-      <c r="W48" s="79"/>
-      <c r="X48" s="79"/>
-      <c r="Y48" s="79"/>
-      <c r="Z48" s="79"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="45" t="s">
+      <c r="C49" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="C49" s="80" t="s">
-        <v>146</v>
-      </c>
       <c r="D49" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E49" s="45"/>
       <c r="F49" s="44" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="G49" s="78"/>
       <c r="H49" s="79"/>
@@ -4231,20 +4239,20 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="80" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="45" t="s">
-        <v>150</v>
-      </c>
       <c r="D50" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E50" s="45"/>
       <c r="F50" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G50" s="78"/>
       <c r="H50" s="79"/>
@@ -4269,20 +4277,20 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="B51" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="C51" s="80" t="s">
-        <v>154</v>
-      </c>
       <c r="D51" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E51" s="45"/>
       <c r="F51" s="44" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G51" s="78"/>
       <c r="H51" s="79"/>
@@ -4307,20 +4315,20 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="45" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B52" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="80" t="s">
         <v>156</v>
       </c>
       <c r="D52" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E52" s="45"/>
       <c r="F52" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G52" s="78"/>
       <c r="H52" s="79"/>
@@ -4345,20 +4353,20 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="45" t="s">
+      <c r="C53" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="80" t="s">
-        <v>159</v>
-      </c>
       <c r="D53" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E53" s="45"/>
       <c r="F53" s="44" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G53" s="78"/>
       <c r="H53" s="79"/>
@@ -4383,20 +4391,20 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="45" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B54" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="C54" s="45" t="s">
+      <c r="C54" s="80" t="s">
         <v>161</v>
       </c>
       <c r="D54" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E54" s="45"/>
       <c r="F54" s="44" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="G54" s="78"/>
       <c r="H54" s="79"/>
@@ -4421,20 +4429,20 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="B55" s="45" t="s">
+      <c r="C55" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="C55" s="81" t="s">
-        <v>164</v>
-      </c>
       <c r="D55" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E55" s="45"/>
       <c r="F55" s="44" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="G55" s="78"/>
       <c r="H55" s="79"/>
@@ -4459,20 +4467,20 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="45" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="B56" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="C56" s="45" t="s">
-        <v>161</v>
+      <c r="C56" s="81" t="s">
+        <v>166</v>
       </c>
       <c r="D56" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E56" s="45"/>
       <c r="F56" s="44" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="G56" s="78"/>
       <c r="H56" s="79"/>
@@ -4497,20 +4505,20 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="45" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B57" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="C57" s="81" t="s">
-        <v>168</v>
+      <c r="C57" s="45" t="s">
+        <v>163</v>
       </c>
       <c r="D57" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E57" s="45"/>
       <c r="F57" s="44" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="G57" s="78"/>
       <c r="H57" s="79"/>
@@ -4535,20 +4543,20 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="45" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="B58" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="C58" s="45" t="s">
-        <v>133</v>
+        <v>169</v>
+      </c>
+      <c r="C58" s="81" t="s">
+        <v>170</v>
       </c>
       <c r="D58" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E58" s="45"/>
       <c r="F58" s="44" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="G58" s="78"/>
       <c r="H58" s="79"/>
@@ -4573,20 +4581,20 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="45" t="s">
         <v>135</v>
-      </c>
-      <c r="B59" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="C59" s="45" t="s">
-        <v>137</v>
       </c>
       <c r="D59" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E59" s="45"/>
       <c r="F59" s="44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G59" s="78"/>
       <c r="H59" s="79"/>
@@ -4610,96 +4618,94 @@
       <c r="Z59" s="79"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="4"/>
-      <c r="G60" s="5"/>
+      <c r="A60" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E60" s="45"/>
+      <c r="F60" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="G60" s="78"/>
+      <c r="H60" s="79"/>
+      <c r="I60" s="79"/>
+      <c r="J60" s="79"/>
+      <c r="K60" s="79"/>
+      <c r="L60" s="79"/>
+      <c r="M60" s="79"/>
+      <c r="N60" s="79"/>
+      <c r="O60" s="79"/>
+      <c r="P60" s="79"/>
+      <c r="Q60" s="79"/>
+      <c r="R60" s="79"/>
+      <c r="S60" s="79"/>
+      <c r="T60" s="79"/>
+      <c r="U60" s="79"/>
+      <c r="V60" s="79"/>
+      <c r="W60" s="79"/>
+      <c r="X60" s="79"/>
+      <c r="Y60" s="79"/>
+      <c r="Z60" s="79"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="A61" s="4"/>
       <c r="G61" s="5"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="4"/>
+      <c r="A62" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="G62" s="5"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="4"/>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B64" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D63" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E63" s="6"/>
-      <c r="F63" s="7" t="s">
+      <c r="D64" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E64" s="6"/>
+      <c r="F64" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G63" s="5"/>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="B64" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C64" s="80" t="s">
-        <v>173</v>
-      </c>
-      <c r="D64" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E64" s="45"/>
-      <c r="F64" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" s="78"/>
-      <c r="H64" s="79"/>
-      <c r="I64" s="79"/>
-      <c r="J64" s="79"/>
-      <c r="K64" s="79"/>
-      <c r="L64" s="79"/>
-      <c r="M64" s="79"/>
-      <c r="N64" s="79"/>
-      <c r="O64" s="79"/>
-      <c r="P64" s="79"/>
-      <c r="Q64" s="79"/>
-      <c r="R64" s="79"/>
-      <c r="S64" s="79"/>
-      <c r="T64" s="79"/>
-      <c r="U64" s="79"/>
-      <c r="V64" s="79"/>
-      <c r="W64" s="79"/>
-      <c r="X64" s="79"/>
-      <c r="Y64" s="79"/>
-      <c r="Z64" s="79"/>
+      <c r="G64" s="5"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="B65" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="B65" s="45" t="s">
+      <c r="C65" s="80" t="s">
         <v>175</v>
       </c>
-      <c r="C65" s="80" t="s">
-        <v>176</v>
-      </c>
       <c r="D65" s="45" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E65" s="45"/>
       <c r="F65" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G65" s="45" t="s">
-        <v>177</v>
-      </c>
+      <c r="G65" s="78"/>
       <c r="H65" s="79"/>
       <c r="I65" s="79"/>
       <c r="J65" s="79"/>
@@ -4722,23 +4728,23 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="B66" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="B66" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C66" s="80" t="s">
-        <v>179</v>
-      </c>
       <c r="D66" s="45" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="E66" s="45"/>
       <c r="F66" s="44" t="s">
-        <v>181</v>
+        <v>13</v>
       </c>
       <c r="G66" s="45" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H66" s="79"/>
       <c r="I66" s="79"/>
@@ -4762,22 +4768,24 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="E67" s="45"/>
+      <c r="F67" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="B67" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="C67" s="45" t="s">
+      <c r="G67" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="D67" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E67" s="82"/>
-      <c r="F67" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G67" s="78"/>
       <c r="H67" s="79"/>
       <c r="I67" s="79"/>
       <c r="J67" s="79"/>
@@ -4803,17 +4811,17 @@
         <v>185</v>
       </c>
       <c r="B68" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="C68" s="45" t="s">
-        <v>187</v>
-      </c>
       <c r="D68" s="45" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E68" s="82"/>
       <c r="F68" s="44" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="G68" s="78"/>
       <c r="H68" s="79"/>
@@ -4838,20 +4846,20 @@
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="B69" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="B69" s="45" t="s">
+      <c r="C69" s="45" t="s">
         <v>189</v>
-      </c>
-      <c r="C69" s="80" t="s">
-        <v>190</v>
       </c>
       <c r="D69" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="E69" s="45"/>
+      <c r="E69" s="82"/>
       <c r="F69" s="44" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="G69" s="78"/>
       <c r="H69" s="79"/>
@@ -4876,18 +4884,18 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="B70" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="B70" s="45" t="s">
+      <c r="C70" s="80" t="s">
         <v>192</v>
       </c>
-      <c r="C70" s="45" t="s">
-        <v>193</v>
-      </c>
       <c r="D70" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E70" s="82"/>
+        <v>11</v>
+      </c>
+      <c r="E70" s="45"/>
       <c r="F70" s="44" t="s">
         <v>54</v>
       </c>
@@ -4914,20 +4922,20 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B71" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="B71" s="45" t="s">
+      <c r="C71" s="45" t="s">
         <v>195</v>
-      </c>
-      <c r="C71" s="80" t="s">
-        <v>196</v>
       </c>
       <c r="D71" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E71" s="45"/>
+      <c r="E71" s="82"/>
       <c r="F71" s="44" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="G71" s="78"/>
       <c r="H71" s="79"/>
@@ -4952,16 +4960,16 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="B72" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="B72" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C72" s="45" t="s">
+      <c r="C72" s="80" t="s">
         <v>198</v>
       </c>
       <c r="D72" s="45" t="s">
-        <v>199</v>
+        <v>30</v>
       </c>
       <c r="E72" s="45"/>
       <c r="F72" s="44" t="s">
@@ -4990,20 +4998,20 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="45" t="s">
-        <v>126</v>
+        <v>199</v>
       </c>
       <c r="B73" s="45" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C73" s="45" t="s">
         <v>200</v>
       </c>
       <c r="D73" s="45" t="s">
-        <v>30</v>
+        <v>201</v>
       </c>
       <c r="E73" s="45"/>
       <c r="F73" s="44" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="G73" s="78"/>
       <c r="H73" s="79"/>
@@ -5028,20 +5036,20 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B74" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="D74" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" s="45"/>
+      <c r="F74" s="44" t="s">
         <v>132</v>
-      </c>
-      <c r="C74" s="45" t="s">
-        <v>201</v>
-      </c>
-      <c r="D74" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E74" s="82"/>
-      <c r="F74" s="44" t="s">
-        <v>134</v>
       </c>
       <c r="G74" s="78"/>
       <c r="H74" s="79"/>
@@ -5066,20 +5074,20 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B75" s="45" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>137</v>
+        <v>203</v>
       </c>
       <c r="D75" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E75" s="82"/>
       <c r="F75" s="44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G75" s="78"/>
       <c r="H75" s="79"/>
@@ -5103,14 +5111,49 @@
       <c r="Z75" s="79"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="4"/>
-      <c r="G76" s="5"/>
+      <c r="A76" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B76" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D76" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E76" s="82"/>
+      <c r="F76" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="G76" s="78"/>
+      <c r="H76" s="79"/>
+      <c r="I76" s="79"/>
+      <c r="J76" s="79"/>
+      <c r="K76" s="79"/>
+      <c r="L76" s="79"/>
+      <c r="M76" s="79"/>
+      <c r="N76" s="79"/>
+      <c r="O76" s="79"/>
+      <c r="P76" s="79"/>
+      <c r="Q76" s="79"/>
+      <c r="R76" s="79"/>
+      <c r="S76" s="79"/>
+      <c r="T76" s="79"/>
+      <c r="U76" s="79"/>
+      <c r="V76" s="79"/>
+      <c r="W76" s="79"/>
+      <c r="X76" s="79"/>
+      <c r="Y76" s="79"/>
+      <c r="Z76" s="79"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="83"/>
+      <c r="A77" s="4"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
+      <c r="A78" s="83"/>
       <c r="G78" s="5"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
State 6 Implementation v1.0.3 - model - Test Mode
State 6 Implementation v1.0.3 - model - Test Mode
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="mSOLnJlHQS9tEmlAYMTMBf0i4q6yQ6CnumUiyuKYyXs="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="cjTK7CeZuVzKWMAuZRk7pYViYT1P7addmWiQOAXdj9k="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="206">
   <si>
     <t>Waterfall Methodology</t>
   </si>
@@ -1401,6 +1401,12 @@
   </si>
   <si>
     <t>Classes in model domain inherits the DbId class that implements db id and debug functionalities</t>
+  </si>
+  <si>
+    <t>Implement a Test Mode</t>
+  </si>
+  <si>
+    <t>java app may be started in normal or unit test mode</t>
   </si>
   <si>
     <t>Development</t>
@@ -3957,97 +3963,99 @@
       <c r="Z37" s="42"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="65" t="s">
+      <c r="A38" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="65" t="s">
+      <c r="C38" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C38" s="65" t="s">
+      <c r="D38" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="43">
+        <v>45872.0</v>
+      </c>
+      <c r="F38" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="64"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="42"/>
+      <c r="Q38" s="42"/>
+      <c r="R38" s="42"/>
+      <c r="S38" s="42"/>
+      <c r="T38" s="42"/>
+      <c r="U38" s="42"/>
+      <c r="V38" s="42"/>
+      <c r="W38" s="42"/>
+      <c r="X38" s="42"/>
+      <c r="Y38" s="42"/>
+      <c r="Z38" s="42"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="D38" s="65" t="s">
+      <c r="B39" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="66"/>
-      <c r="F38" s="67" t="s">
+      <c r="E39" s="66"/>
+      <c r="F39" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="G38" s="68"/>
-      <c r="H38" s="69"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="69"/>
-      <c r="K38" s="69"/>
-      <c r="L38" s="69"/>
-      <c r="M38" s="69"/>
-      <c r="N38" s="69"/>
-      <c r="O38" s="69"/>
-      <c r="P38" s="69"/>
-      <c r="Q38" s="69"/>
-      <c r="R38" s="69"/>
-      <c r="S38" s="69"/>
-      <c r="T38" s="69"/>
-      <c r="U38" s="69"/>
-      <c r="V38" s="69"/>
-      <c r="W38" s="69"/>
-      <c r="X38" s="69"/>
-      <c r="Y38" s="69"/>
-      <c r="Z38" s="69"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="70"/>
-      <c r="F39" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G39" s="71"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="72"/>
-      <c r="N39" s="72"/>
-      <c r="O39" s="72"/>
-      <c r="P39" s="72"/>
-      <c r="Q39" s="72"/>
-      <c r="R39" s="72"/>
-      <c r="S39" s="72"/>
-      <c r="T39" s="72"/>
-      <c r="U39" s="72"/>
-      <c r="V39" s="72"/>
-      <c r="W39" s="72"/>
-      <c r="X39" s="72"/>
-      <c r="Y39" s="72"/>
-      <c r="Z39" s="72"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="69"/>
+      <c r="K39" s="69"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="69"/>
+      <c r="P39" s="69"/>
+      <c r="Q39" s="69"/>
+      <c r="R39" s="69"/>
+      <c r="S39" s="69"/>
+      <c r="T39" s="69"/>
+      <c r="U39" s="69"/>
+      <c r="V39" s="69"/>
+      <c r="W39" s="69"/>
+      <c r="X39" s="69"/>
+      <c r="Y39" s="69"/>
+      <c r="Z39" s="69"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="C40" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C40" s="26" t="s">
-        <v>130</v>
-      </c>
       <c r="D40" s="25" t="s">
-        <v>131</v>
+        <v>30</v>
       </c>
       <c r="E40" s="70"/>
       <c r="F40" s="28" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="G40" s="71"/>
       <c r="H40" s="72"/>
@@ -4072,20 +4080,20 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="25" t="s">
         <v>133</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>86</v>
       </c>
       <c r="E41" s="70"/>
       <c r="F41" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G41" s="71"/>
       <c r="H41" s="72"/>
@@ -4109,51 +4117,80 @@
       <c r="Z41" s="72"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="D42" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="70"/>
+      <c r="F42" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="G42" s="71"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+      <c r="N42" s="72"/>
+      <c r="O42" s="72"/>
+      <c r="P42" s="72"/>
+      <c r="Q42" s="72"/>
+      <c r="R42" s="72"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
+      <c r="W42" s="72"/>
+      <c r="X42" s="72"/>
+      <c r="Y42" s="72"/>
+      <c r="Z42" s="72"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="B43" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="G42" s="73"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="74"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="74"/>
-      <c r="M42" s="74"/>
-      <c r="N42" s="74"/>
-      <c r="O42" s="74"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
-      <c r="T42" s="74"/>
-      <c r="U42" s="74"/>
-      <c r="V42" s="74"/>
-      <c r="W42" s="74"/>
-      <c r="X42" s="74"/>
-      <c r="Y42" s="74"/>
-      <c r="Z42" s="74"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="75"/>
-      <c r="B43" s="75"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="77"/>
-      <c r="G43" s="5"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43" s="73"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="74"/>
+      <c r="L43" s="74"/>
+      <c r="M43" s="74"/>
+      <c r="N43" s="74"/>
+      <c r="O43" s="74"/>
+      <c r="P43" s="74"/>
+      <c r="Q43" s="74"/>
+      <c r="R43" s="74"/>
+      <c r="S43" s="74"/>
+      <c r="T43" s="74"/>
+      <c r="U43" s="74"/>
+      <c r="V43" s="74"/>
+      <c r="W43" s="74"/>
+      <c r="X43" s="74"/>
+      <c r="Y43" s="74"/>
+      <c r="Z43" s="74"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="75"/>
@@ -4165,94 +4202,65 @@
       <c r="G44" s="5"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="4"/>
+      <c r="A45" s="75"/>
+      <c r="B45" s="75"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="77"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>140</v>
-      </c>
+      <c r="A46" s="4"/>
       <c r="G46" s="5"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="4"/>
+      <c r="A47" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="G47" s="5"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="4"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B49" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F48" s="7" t="s">
+      <c r="D49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="5"/>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="B49" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="C49" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E49" s="45"/>
-      <c r="F49" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" s="78"/>
-      <c r="H49" s="79"/>
-      <c r="I49" s="79"/>
-      <c r="J49" s="79"/>
-      <c r="K49" s="79"/>
-      <c r="L49" s="79"/>
-      <c r="M49" s="79"/>
-      <c r="N49" s="79"/>
-      <c r="O49" s="79"/>
-      <c r="P49" s="79"/>
-      <c r="Q49" s="79"/>
-      <c r="R49" s="79"/>
-      <c r="S49" s="79"/>
-      <c r="T49" s="79"/>
-      <c r="U49" s="79"/>
-      <c r="V49" s="79"/>
-      <c r="W49" s="79"/>
-      <c r="X49" s="79"/>
-      <c r="Y49" s="79"/>
-      <c r="Z49" s="79"/>
+      <c r="G49" s="5"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="B50" s="45" t="s">
+      <c r="C50" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="80" t="s">
-        <v>148</v>
-      </c>
       <c r="D50" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E50" s="45"/>
       <c r="F50" s="44" t="s">
-        <v>149</v>
+        <v>13</v>
       </c>
       <c r="G50" s="78"/>
       <c r="H50" s="79"/>
@@ -4277,20 +4285,20 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="B51" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="45" t="s">
-        <v>152</v>
-      </c>
       <c r="D51" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E51" s="45"/>
       <c r="F51" s="44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G51" s="78"/>
       <c r="H51" s="79"/>
@@ -4315,20 +4323,20 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="B52" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="C52" s="80" t="s">
-        <v>156</v>
-      </c>
       <c r="D52" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E52" s="45"/>
       <c r="F52" s="44" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="G52" s="78"/>
       <c r="H52" s="79"/>
@@ -4353,20 +4361,20 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="45" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B53" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="C53" s="45" t="s">
+      <c r="C53" s="80" t="s">
         <v>158</v>
       </c>
       <c r="D53" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E53" s="45"/>
       <c r="F53" s="44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G53" s="78"/>
       <c r="H53" s="79"/>
@@ -4391,20 +4399,20 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="B54" s="45" t="s">
+      <c r="C54" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="C54" s="80" t="s">
-        <v>161</v>
-      </c>
       <c r="D54" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E54" s="45"/>
       <c r="F54" s="44" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="G54" s="78"/>
       <c r="H54" s="79"/>
@@ -4429,20 +4437,20 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="45" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B55" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="80" t="s">
         <v>163</v>
       </c>
       <c r="D55" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E55" s="45"/>
       <c r="F55" s="44" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="G55" s="78"/>
       <c r="H55" s="79"/>
@@ -4467,20 +4475,20 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="B56" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="B56" s="45" t="s">
+      <c r="C56" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="C56" s="81" t="s">
-        <v>166</v>
-      </c>
       <c r="D56" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E56" s="45"/>
       <c r="F56" s="44" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="G56" s="78"/>
       <c r="H56" s="79"/>
@@ -4505,20 +4513,20 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="45" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="B57" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="C57" s="45" t="s">
-        <v>163</v>
+      <c r="C57" s="81" t="s">
+        <v>168</v>
       </c>
       <c r="D57" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E57" s="45"/>
       <c r="F57" s="44" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="G57" s="78"/>
       <c r="H57" s="79"/>
@@ -4543,20 +4551,20 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="45" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="B58" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="C58" s="81" t="s">
-        <v>170</v>
+      <c r="C58" s="45" t="s">
+        <v>165</v>
       </c>
       <c r="D58" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E58" s="45"/>
       <c r="F58" s="44" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="G58" s="78"/>
       <c r="H58" s="79"/>
@@ -4581,20 +4589,20 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="45" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="B59" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="C59" s="45" t="s">
-        <v>135</v>
+        <v>171</v>
+      </c>
+      <c r="C59" s="81" t="s">
+        <v>172</v>
       </c>
       <c r="D59" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E59" s="45"/>
       <c r="F59" s="44" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="G59" s="78"/>
       <c r="H59" s="79"/>
@@ -4619,20 +4627,20 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="45" t="s">
         <v>137</v>
-      </c>
-      <c r="B60" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="C60" s="45" t="s">
-        <v>139</v>
       </c>
       <c r="D60" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E60" s="45"/>
       <c r="F60" s="44" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G60" s="78"/>
       <c r="H60" s="79"/>
@@ -4656,96 +4664,96 @@
       <c r="Z60" s="79"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="4"/>
-      <c r="G61" s="5"/>
+      <c r="A61" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="45"/>
+      <c r="F61" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="G61" s="78"/>
+      <c r="H61" s="79"/>
+      <c r="I61" s="79"/>
+      <c r="J61" s="79"/>
+      <c r="K61" s="79"/>
+      <c r="L61" s="79"/>
+      <c r="M61" s="79"/>
+      <c r="N61" s="79"/>
+      <c r="O61" s="79"/>
+      <c r="P61" s="79"/>
+      <c r="Q61" s="79"/>
+      <c r="R61" s="79"/>
+      <c r="S61" s="79"/>
+      <c r="T61" s="79"/>
+      <c r="U61" s="79"/>
+      <c r="V61" s="79"/>
+      <c r="W61" s="79"/>
+      <c r="X61" s="79"/>
+      <c r="Y61" s="79"/>
+      <c r="Z61" s="79"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="A62" s="4"/>
       <c r="G62" s="5"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="4"/>
+      <c r="A63" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="G63" s="5"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="4"/>
+      <c r="G64" s="5"/>
+    </row>
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="A65" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B65" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D64" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E64" s="6"/>
-      <c r="F64" s="7" t="s">
+      <c r="D65" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="5"/>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="B65" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="C65" s="80" t="s">
-        <v>175</v>
-      </c>
-      <c r="D65" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" s="45"/>
-      <c r="F65" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G65" s="78"/>
-      <c r="H65" s="79"/>
-      <c r="I65" s="79"/>
-      <c r="J65" s="79"/>
-      <c r="K65" s="79"/>
-      <c r="L65" s="79"/>
-      <c r="M65" s="79"/>
-      <c r="N65" s="79"/>
-      <c r="O65" s="79"/>
-      <c r="P65" s="79"/>
-      <c r="Q65" s="79"/>
-      <c r="R65" s="79"/>
-      <c r="S65" s="79"/>
-      <c r="T65" s="79"/>
-      <c r="U65" s="79"/>
-      <c r="V65" s="79"/>
-      <c r="W65" s="79"/>
-      <c r="X65" s="79"/>
-      <c r="Y65" s="79"/>
-      <c r="Z65" s="79"/>
+      <c r="G65" s="5"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="B66" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="B66" s="45" t="s">
+      <c r="C66" s="80" t="s">
         <v>177</v>
       </c>
-      <c r="C66" s="80" t="s">
-        <v>178</v>
-      </c>
       <c r="D66" s="45" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E66" s="45"/>
       <c r="F66" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="G66" s="45" t="s">
-        <v>179</v>
-      </c>
+      <c r="G66" s="78"/>
       <c r="H66" s="79"/>
       <c r="I66" s="79"/>
       <c r="J66" s="79"/>
@@ -4768,23 +4776,23 @@
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B67" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="C67" s="80" t="s">
         <v>180</v>
       </c>
-      <c r="B67" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C67" s="80" t="s">
-        <v>181</v>
-      </c>
       <c r="D67" s="45" t="s">
-        <v>182</v>
+        <v>11</v>
       </c>
       <c r="E67" s="45"/>
       <c r="F67" s="44" t="s">
-        <v>183</v>
+        <v>13</v>
       </c>
       <c r="G67" s="45" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H67" s="79"/>
       <c r="I67" s="79"/>
@@ -4808,22 +4816,24 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="B68" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C68" s="80" t="s">
+        <v>183</v>
+      </c>
+      <c r="D68" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="E68" s="45"/>
+      <c r="F68" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="B68" s="45" t="s">
-        <v>147</v>
-      </c>
-      <c r="C68" s="45" t="s">
+      <c r="G68" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="D68" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E68" s="82"/>
-      <c r="F68" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G68" s="78"/>
       <c r="H68" s="79"/>
       <c r="I68" s="79"/>
       <c r="J68" s="79"/>
@@ -4849,17 +4859,17 @@
         <v>187</v>
       </c>
       <c r="B69" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="C69" s="45" t="s">
-        <v>189</v>
-      </c>
       <c r="D69" s="45" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E69" s="82"/>
       <c r="F69" s="44" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="G69" s="78"/>
       <c r="H69" s="79"/>
@@ -4884,20 +4894,20 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B70" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="B70" s="45" t="s">
+      <c r="C70" s="45" t="s">
         <v>191</v>
-      </c>
-      <c r="C70" s="80" t="s">
-        <v>192</v>
       </c>
       <c r="D70" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="45"/>
+      <c r="E70" s="82"/>
       <c r="F70" s="44" t="s">
-        <v>54</v>
+        <v>134</v>
       </c>
       <c r="G70" s="78"/>
       <c r="H70" s="79"/>
@@ -4922,18 +4932,18 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="B71" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="B71" s="45" t="s">
+      <c r="C71" s="80" t="s">
         <v>194</v>
       </c>
-      <c r="C71" s="45" t="s">
-        <v>195</v>
-      </c>
       <c r="D71" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E71" s="82"/>
+        <v>11</v>
+      </c>
+      <c r="E71" s="45"/>
       <c r="F71" s="44" t="s">
         <v>54</v>
       </c>
@@ -4960,20 +4970,20 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B72" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="B72" s="45" t="s">
+      <c r="C72" s="45" t="s">
         <v>197</v>
-      </c>
-      <c r="C72" s="80" t="s">
-        <v>198</v>
       </c>
       <c r="D72" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E72" s="45"/>
+      <c r="E72" s="82"/>
       <c r="F72" s="44" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="G72" s="78"/>
       <c r="H72" s="79"/>
@@ -4998,16 +5008,16 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="B73" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="B73" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C73" s="45" t="s">
+      <c r="C73" s="80" t="s">
         <v>200</v>
       </c>
       <c r="D73" s="45" t="s">
-        <v>201</v>
+        <v>30</v>
       </c>
       <c r="E73" s="45"/>
       <c r="F73" s="44" t="s">
@@ -5036,20 +5046,20 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="45" t="s">
-        <v>128</v>
+        <v>201</v>
       </c>
       <c r="B74" s="45" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C74" s="45" t="s">
         <v>202</v>
       </c>
       <c r="D74" s="45" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="E74" s="45"/>
       <c r="F74" s="44" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="G74" s="78"/>
       <c r="H74" s="79"/>
@@ -5074,20 +5084,20 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="45" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B75" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="D75" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E75" s="45"/>
+      <c r="F75" s="44" t="s">
         <v>134</v>
-      </c>
-      <c r="C75" s="45" t="s">
-        <v>203</v>
-      </c>
-      <c r="D75" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E75" s="82"/>
-      <c r="F75" s="44" t="s">
-        <v>136</v>
       </c>
       <c r="G75" s="78"/>
       <c r="H75" s="79"/>
@@ -5112,20 +5122,20 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B76" s="45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C76" s="45" t="s">
-        <v>139</v>
+        <v>205</v>
       </c>
       <c r="D76" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E76" s="82"/>
       <c r="F76" s="44" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G76" s="78"/>
       <c r="H76" s="79"/>
@@ -5149,14 +5159,49 @@
       <c r="Z76" s="79"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="4"/>
-      <c r="G77" s="5"/>
+      <c r="A77" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C77" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D77" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E77" s="82"/>
+      <c r="F77" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="G77" s="78"/>
+      <c r="H77" s="79"/>
+      <c r="I77" s="79"/>
+      <c r="J77" s="79"/>
+      <c r="K77" s="79"/>
+      <c r="L77" s="79"/>
+      <c r="M77" s="79"/>
+      <c r="N77" s="79"/>
+      <c r="O77" s="79"/>
+      <c r="P77" s="79"/>
+      <c r="Q77" s="79"/>
+      <c r="R77" s="79"/>
+      <c r="S77" s="79"/>
+      <c r="T77" s="79"/>
+      <c r="U77" s="79"/>
+      <c r="V77" s="79"/>
+      <c r="W77" s="79"/>
+      <c r="X77" s="79"/>
+      <c r="Y77" s="79"/>
+      <c r="Z77" s="79"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="83"/>
+      <c r="A78" s="4"/>
       <c r="G78" s="5"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
+      <c r="A79" s="83"/>
       <c r="G79" s="5"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
State 6 Implementation v3.0.0 - navigation - Application Status
State 6 Implementation v3.0.0 - navigation - Application Status
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="6AsrQOzvsaAWM3w7gUsjvQconsHAEQV1XvBR0/kvfiQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="9RE5WWv/1Z/enEj8mWwpWuwrwng687r8dWKhSScwD+w="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="239">
   <si>
     <t>Waterfall Methodology</t>
   </si>
@@ -1424,7 +1424,281 @@
     <t>HomeView can be visualized</t>
   </si>
   <si>
+    <t>Design, test plan</t>
+  </si>
+  <si>
+    <t>For design complexity. we deleted the option of deleting user for now and we only show the top 5 players. Accepted by phone call by my uncles</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <color rgb="FF980000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>updated</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <b/>
+        <color rgb="FF980000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> requirements list</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <color rgb="FF980000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <b/>
+        <color rgb="FF980000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">use cases </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <color rgb="FF980000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <b/>
+        <color rgb="FF980000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>test plan</t>
+    </r>
+  </si>
+  <si>
+    <t>Implement PlayerSelection (without navigation)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <color rgb="FF156082"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>PlayerSelectionView can be visualized. Found a third party class to properly show jcombo with objects. We changed</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FF156082"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> Sketch, View and Navigation Model </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF156082"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>to better UX</t>
+    </r>
+  </si>
+  <si>
+    <t>Call phone to my uncle CTO to validate the change in the view of PlayerSelection</t>
+  </si>
+  <si>
+    <t>Implement GameView (without game logic and without navigation)</t>
+  </si>
+  <si>
+    <t>GameView can be visualized.</t>
+  </si>
+  <si>
+    <t>Implement ResultView (without game logic and without navigation)</t>
+  </si>
+  <si>
+    <t>ResultView Can be visualized for null match anf won match</t>
+  </si>
+  <si>
+    <t>03/13/2025</t>
+  </si>
+  <si>
     <t>Development</t>
+  </si>
+  <si>
+    <t>Implement PlayerCreateView and PlayerEditView (without game logic and without navigation)</t>
+  </si>
+  <si>
+    <t>PlayerCreate and PlayerEditView can be visualized</t>
+  </si>
+  <si>
+    <t>03/14/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we actualized MockUpDB to add create and edit players and match result submit </t>
+  </si>
+  <si>
+    <t>Actualize code comments</t>
+  </si>
+  <si>
+    <t>Code comment revised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review View Implementation with my uncle and some users (players) of my family: Demo, and feedback </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <b/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>feedback</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <b/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>model</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> refinment, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <b/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>requirement list</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> actualization</t>
+    </r>
+  </si>
+  <si>
+    <t>03/15/2025</t>
+  </si>
+  <si>
+    <t>Revise Doc</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Documentation according to client review and features implemented </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <b/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>to now: UML Domain Model, UML class Model</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <b/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Sketch-View </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <b/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> Navigation Model</t>
+    </r>
+  </si>
+  <si>
+    <t>03/18/2025</t>
+  </si>
+  <si>
+    <t>Criterion C: Development  Criterion B: Solution Overview</t>
+  </si>
+  <si>
+    <t>Note: we change 2 requirements (number of top players shown, and delete player is not anymore in MVP). Validated by client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a Status for our App that will manage the players and game ' s selection </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <color rgb="FF156082"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Added a AppStatus class with unit test for main flow views (homeview, selectplayerview, gameview,resultview). Other views (PlayerEditView and PlayerCreateView) dont requires it since they dont requires a selection change. See</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FF156082"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>•	Navigation and AppStatus</t>
+    </r>
+  </si>
+  <si>
+    <t>6 hours</t>
   </si>
   <si>
     <t>Implement the database</t>
@@ -1946,10 +2220,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="18">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -2023,12 +2298,34 @@
       <name val="Aptos Narrow"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF980000"/>
+      <name val="Quattrocento Sans"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF980000"/>
+      <name val="Quattrocento Sans"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF156082"/>
+      <name val="Quattrocento Sans"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <color theme="4"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FFFF0000"/>
       <name val="Quattrocento Sans"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2051,6 +2348,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFAE2D5"/>
         <bgColor rgb="FFFAE2D5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8AF"/>
+        <bgColor rgb="FFE6B8AF"/>
       </patternFill>
     </fill>
   </fills>
@@ -2128,7 +2431,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="93">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2306,6 +2609,29 @@
     <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -2346,7 +2672,7 @@
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -4101,20 +4427,16 @@
       <c r="A41" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="B41" s="65" t="s">
+      <c r="B41" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="C41" s="65" t="s">
+      <c r="C41" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="D41" s="65" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="66"/>
-      <c r="F41" s="67" t="s">
-        <v>107</v>
-      </c>
-      <c r="G41" s="68"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="69"/>
       <c r="H41" s="69"/>
       <c r="I41" s="69"/>
       <c r="J41" s="69"/>
@@ -4136,1194 +4458,1529 @@
       <c r="Z41" s="69"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="70" t="s">
         <v>132</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="C42" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="D42" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="43">
+        <v>45964.0</v>
+      </c>
+      <c r="F42" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="42"/>
+      <c r="T42" s="42"/>
+      <c r="U42" s="42"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="42"/>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="42"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="43">
+        <v>45994.0</v>
+      </c>
+      <c r="F43" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="64"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="42"/>
+      <c r="Q43" s="42"/>
+      <c r="R43" s="42"/>
+      <c r="S43" s="42"/>
+      <c r="T43" s="42"/>
+      <c r="U43" s="42"/>
+      <c r="V43" s="42"/>
+      <c r="W43" s="42"/>
+      <c r="X43" s="42"/>
+      <c r="Y43" s="42"/>
+      <c r="Z43" s="42"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="F44" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="64"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="42"/>
+      <c r="L44" s="42"/>
+      <c r="M44" s="42"/>
+      <c r="N44" s="42"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="42"/>
+      <c r="Q44" s="42"/>
+      <c r="R44" s="42"/>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="42"/>
+      <c r="V44" s="42"/>
+      <c r="W44" s="42"/>
+      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="42"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="F45" s="41"/>
+      <c r="G45" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="42"/>
+      <c r="L45" s="42"/>
+      <c r="M45" s="42"/>
+      <c r="N45" s="42"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="42"/>
+      <c r="Q45" s="42"/>
+      <c r="R45" s="42"/>
+      <c r="S45" s="42"/>
+      <c r="T45" s="42"/>
+      <c r="U45" s="42"/>
+      <c r="V45" s="42"/>
+      <c r="W45" s="42"/>
+      <c r="X45" s="42"/>
+      <c r="Y45" s="42"/>
+      <c r="Z45" s="42"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="F46" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="64"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="42"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="42"/>
+      <c r="N46" s="42"/>
+      <c r="O46" s="42"/>
+      <c r="P46" s="42"/>
+      <c r="Q46" s="42"/>
+      <c r="R46" s="42"/>
+      <c r="S46" s="42"/>
+      <c r="T46" s="42"/>
+      <c r="U46" s="42"/>
+      <c r="V46" s="42"/>
+      <c r="W46" s="42"/>
+      <c r="X46" s="42"/>
+      <c r="Y46" s="42"/>
+      <c r="Z46" s="42"/>
+    </row>
+    <row r="47" ht="52.5" customHeight="1">
+      <c r="A47" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="F47" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" s="64"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="42"/>
+      <c r="L47" s="42"/>
+      <c r="M47" s="42"/>
+      <c r="N47" s="42"/>
+      <c r="O47" s="42"/>
+      <c r="P47" s="42"/>
+      <c r="Q47" s="42"/>
+      <c r="R47" s="42"/>
+      <c r="S47" s="42"/>
+      <c r="T47" s="42"/>
+      <c r="U47" s="42"/>
+      <c r="V47" s="42"/>
+      <c r="W47" s="42"/>
+      <c r="X47" s="42"/>
+      <c r="Y47" s="42"/>
+      <c r="Z47" s="42"/>
+    </row>
+    <row r="48" ht="51.75" customHeight="1">
+      <c r="A48" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G48" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="18"/>
+      <c r="U48" s="18"/>
+      <c r="V48" s="18"/>
+      <c r="W48" s="18"/>
+      <c r="X48" s="18"/>
+      <c r="Y48" s="18"/>
+      <c r="Z48" s="18"/>
+    </row>
+    <row r="49" ht="85.5" customHeight="1">
+      <c r="A49" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G49" s="72"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="18"/>
+      <c r="U49" s="18"/>
+      <c r="V49" s="18"/>
+      <c r="W49" s="18"/>
+      <c r="X49" s="18"/>
+      <c r="Y49" s="18"/>
+      <c r="Z49" s="18"/>
+    </row>
+    <row r="50" ht="45.75" customHeight="1">
+      <c r="A50" s="74" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="75"/>
+      <c r="F50" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="G50" s="77"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
+      <c r="L50" s="78"/>
+      <c r="M50" s="78"/>
+      <c r="N50" s="78"/>
+      <c r="O50" s="78"/>
+      <c r="P50" s="78"/>
+      <c r="Q50" s="78"/>
+      <c r="R50" s="78"/>
+      <c r="S50" s="78"/>
+      <c r="T50" s="78"/>
+      <c r="U50" s="78"/>
+      <c r="V50" s="78"/>
+      <c r="W50" s="78"/>
+      <c r="X50" s="78"/>
+      <c r="Y50" s="78"/>
+      <c r="Z50" s="78"/>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D51" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="70"/>
-      <c r="F42" s="28" t="s">
+      <c r="E51" s="79"/>
+      <c r="F51" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="G42" s="71"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
-      <c r="M42" s="72"/>
-      <c r="N42" s="72"/>
-      <c r="O42" s="72"/>
-      <c r="P42" s="72"/>
-      <c r="Q42" s="72"/>
-      <c r="R42" s="72"/>
-      <c r="S42" s="72"/>
-      <c r="T42" s="72"/>
-      <c r="U42" s="72"/>
-      <c r="V42" s="72"/>
-      <c r="W42" s="72"/>
-      <c r="X42" s="72"/>
-      <c r="Y42" s="72"/>
-      <c r="Z42" s="72"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="E43" s="70"/>
-      <c r="F43" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="G43" s="71"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="72"/>
-      <c r="L43" s="72"/>
-      <c r="M43" s="72"/>
-      <c r="N43" s="72"/>
-      <c r="O43" s="72"/>
-      <c r="P43" s="72"/>
-      <c r="Q43" s="72"/>
-      <c r="R43" s="72"/>
-      <c r="S43" s="72"/>
-      <c r="T43" s="72"/>
-      <c r="U43" s="72"/>
-      <c r="V43" s="72"/>
-      <c r="W43" s="72"/>
-      <c r="X43" s="72"/>
-      <c r="Y43" s="72"/>
-      <c r="Z43" s="72"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="D44" s="25" t="s">
+      <c r="G51" s="80"/>
+      <c r="H51" s="81"/>
+      <c r="I51" s="81"/>
+      <c r="J51" s="81"/>
+      <c r="K51" s="81"/>
+      <c r="L51" s="81"/>
+      <c r="M51" s="81"/>
+      <c r="N51" s="81"/>
+      <c r="O51" s="81"/>
+      <c r="P51" s="81"/>
+      <c r="Q51" s="81"/>
+      <c r="R51" s="81"/>
+      <c r="S51" s="81"/>
+      <c r="T51" s="81"/>
+      <c r="U51" s="81"/>
+      <c r="V51" s="81"/>
+      <c r="W51" s="81"/>
+      <c r="X51" s="81"/>
+      <c r="Y51" s="81"/>
+      <c r="Z51" s="81"/>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="79"/>
+      <c r="F52" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G52" s="80"/>
+      <c r="H52" s="81"/>
+      <c r="I52" s="81"/>
+      <c r="J52" s="81"/>
+      <c r="K52" s="81"/>
+      <c r="L52" s="81"/>
+      <c r="M52" s="81"/>
+      <c r="N52" s="81"/>
+      <c r="O52" s="81"/>
+      <c r="P52" s="81"/>
+      <c r="Q52" s="81"/>
+      <c r="R52" s="81"/>
+      <c r="S52" s="81"/>
+      <c r="T52" s="81"/>
+      <c r="U52" s="81"/>
+      <c r="V52" s="81"/>
+      <c r="W52" s="81"/>
+      <c r="X52" s="81"/>
+      <c r="Y52" s="81"/>
+      <c r="Z52" s="81"/>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D53" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="70"/>
-      <c r="F44" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="G44" s="71"/>
-      <c r="H44" s="72"/>
-      <c r="I44" s="72"/>
-      <c r="J44" s="72"/>
-      <c r="K44" s="72"/>
-      <c r="L44" s="72"/>
-      <c r="M44" s="72"/>
-      <c r="N44" s="72"/>
-      <c r="O44" s="72"/>
-      <c r="P44" s="72"/>
-      <c r="Q44" s="72"/>
-      <c r="R44" s="72"/>
-      <c r="S44" s="72"/>
-      <c r="T44" s="72"/>
-      <c r="U44" s="72"/>
-      <c r="V44" s="72"/>
-      <c r="W44" s="72"/>
-      <c r="X44" s="72"/>
-      <c r="Y44" s="72"/>
-      <c r="Z44" s="72"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" s="8" t="s">
+      <c r="E53" s="79"/>
+      <c r="F53" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G53" s="80"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="81"/>
+      <c r="J53" s="81"/>
+      <c r="K53" s="81"/>
+      <c r="L53" s="81"/>
+      <c r="M53" s="81"/>
+      <c r="N53" s="81"/>
+      <c r="O53" s="81"/>
+      <c r="P53" s="81"/>
+      <c r="Q53" s="81"/>
+      <c r="R53" s="81"/>
+      <c r="S53" s="81"/>
+      <c r="T53" s="81"/>
+      <c r="U53" s="81"/>
+      <c r="V53" s="81"/>
+      <c r="W53" s="81"/>
+      <c r="X53" s="81"/>
+      <c r="Y53" s="81"/>
+      <c r="Z53" s="81"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E45" s="9"/>
-      <c r="F45" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="G45" s="73"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
-      <c r="M45" s="74"/>
-      <c r="N45" s="74"/>
-      <c r="O45" s="74"/>
-      <c r="P45" s="74"/>
-      <c r="Q45" s="74"/>
-      <c r="R45" s="74"/>
-      <c r="S45" s="74"/>
-      <c r="T45" s="74"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="74"/>
-      <c r="W45" s="74"/>
-      <c r="X45" s="74"/>
-      <c r="Y45" s="74"/>
-      <c r="Z45" s="74"/>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="75"/>
-      <c r="B46" s="75"/>
-      <c r="C46" s="75"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="77"/>
-      <c r="G46" s="5"/>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="75"/>
-      <c r="B47" s="75"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="76"/>
-      <c r="F47" s="77"/>
-      <c r="G47" s="5"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="4"/>
-      <c r="G48" s="5"/>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G49" s="5"/>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="4"/>
-      <c r="G50" s="5"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="6" t="s">
+      <c r="E54" s="9"/>
+      <c r="F54" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="G54" s="82"/>
+      <c r="H54" s="83"/>
+      <c r="I54" s="83"/>
+      <c r="J54" s="83"/>
+      <c r="K54" s="83"/>
+      <c r="L54" s="83"/>
+      <c r="M54" s="83"/>
+      <c r="N54" s="83"/>
+      <c r="O54" s="83"/>
+      <c r="P54" s="83"/>
+      <c r="Q54" s="83"/>
+      <c r="R54" s="83"/>
+      <c r="S54" s="83"/>
+      <c r="T54" s="83"/>
+      <c r="U54" s="83"/>
+      <c r="V54" s="83"/>
+      <c r="W54" s="83"/>
+      <c r="X54" s="83"/>
+      <c r="Y54" s="83"/>
+      <c r="Z54" s="83"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="84"/>
+      <c r="B55" s="84"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="85"/>
+      <c r="F55" s="86"/>
+      <c r="G55" s="5"/>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="84"/>
+      <c r="B56" s="84"/>
+      <c r="C56" s="84"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="86"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="4"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="4"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="D60" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G51" s="5"/>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="B52" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="C52" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="D52" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E52" s="45"/>
-      <c r="F52" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="78"/>
-      <c r="H52" s="79"/>
-      <c r="I52" s="79"/>
-      <c r="J52" s="79"/>
-      <c r="K52" s="79"/>
-      <c r="L52" s="79"/>
-      <c r="M52" s="79"/>
-      <c r="N52" s="79"/>
-      <c r="O52" s="79"/>
-      <c r="P52" s="79"/>
-      <c r="Q52" s="79"/>
-      <c r="R52" s="79"/>
-      <c r="S52" s="79"/>
-      <c r="T52" s="79"/>
-      <c r="U52" s="79"/>
-      <c r="V52" s="79"/>
-      <c r="W52" s="79"/>
-      <c r="X52" s="79"/>
-      <c r="Y52" s="79"/>
-      <c r="Z52" s="79"/>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="B53" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="C53" s="80" t="s">
-        <v>155</v>
-      </c>
-      <c r="D53" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="45"/>
-      <c r="F53" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="G53" s="78"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="79"/>
-      <c r="M53" s="79"/>
-      <c r="N53" s="79"/>
-      <c r="O53" s="79"/>
-      <c r="P53" s="79"/>
-      <c r="Q53" s="79"/>
-      <c r="R53" s="79"/>
-      <c r="S53" s="79"/>
-      <c r="T53" s="79"/>
-      <c r="U53" s="79"/>
-      <c r="V53" s="79"/>
-      <c r="W53" s="79"/>
-      <c r="X53" s="79"/>
-      <c r="Y53" s="79"/>
-      <c r="Z53" s="79"/>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B54" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="C54" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="D54" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="45"/>
-      <c r="F54" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="G54" s="78"/>
-      <c r="H54" s="79"/>
-      <c r="I54" s="79"/>
-      <c r="J54" s="79"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="79"/>
-      <c r="M54" s="79"/>
-      <c r="N54" s="79"/>
-      <c r="O54" s="79"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
-      <c r="R54" s="79"/>
-      <c r="S54" s="79"/>
-      <c r="T54" s="79"/>
-      <c r="U54" s="79"/>
-      <c r="V54" s="79"/>
-      <c r="W54" s="79"/>
-      <c r="X54" s="79"/>
-      <c r="Y54" s="79"/>
-      <c r="Z54" s="79"/>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="B55" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="80" t="s">
-        <v>163</v>
-      </c>
-      <c r="D55" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="45"/>
-      <c r="F55" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="G55" s="78"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
-      <c r="M55" s="79"/>
-      <c r="N55" s="79"/>
-      <c r="O55" s="79"/>
-      <c r="P55" s="79"/>
-      <c r="Q55" s="79"/>
-      <c r="R55" s="79"/>
-      <c r="S55" s="79"/>
-      <c r="T55" s="79"/>
-      <c r="U55" s="79"/>
-      <c r="V55" s="79"/>
-      <c r="W55" s="79"/>
-      <c r="X55" s="79"/>
-      <c r="Y55" s="79"/>
-      <c r="Z55" s="79"/>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B56" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="C56" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="D56" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="45"/>
-      <c r="F56" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="G56" s="78"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="79"/>
-      <c r="J56" s="79"/>
-      <c r="K56" s="79"/>
-      <c r="L56" s="79"/>
-      <c r="M56" s="79"/>
-      <c r="N56" s="79"/>
-      <c r="O56" s="79"/>
-      <c r="P56" s="79"/>
-      <c r="Q56" s="79"/>
-      <c r="R56" s="79"/>
-      <c r="S56" s="79"/>
-      <c r="T56" s="79"/>
-      <c r="U56" s="79"/>
-      <c r="V56" s="79"/>
-      <c r="W56" s="79"/>
-      <c r="X56" s="79"/>
-      <c r="Y56" s="79"/>
-      <c r="Z56" s="79"/>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="B57" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="C57" s="80" t="s">
-        <v>168</v>
-      </c>
-      <c r="D57" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E57" s="45"/>
-      <c r="F57" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="G57" s="78"/>
-      <c r="H57" s="79"/>
-      <c r="I57" s="79"/>
-      <c r="J57" s="79"/>
-      <c r="K57" s="79"/>
-      <c r="L57" s="79"/>
-      <c r="M57" s="79"/>
-      <c r="N57" s="79"/>
-      <c r="O57" s="79"/>
-      <c r="P57" s="79"/>
-      <c r="Q57" s="79"/>
-      <c r="R57" s="79"/>
-      <c r="S57" s="79"/>
-      <c r="T57" s="79"/>
-      <c r="U57" s="79"/>
-      <c r="V57" s="79"/>
-      <c r="W57" s="79"/>
-      <c r="X57" s="79"/>
-      <c r="Y57" s="79"/>
-      <c r="Z57" s="79"/>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B58" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="C58" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="D58" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E58" s="45"/>
-      <c r="F58" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G58" s="78"/>
-      <c r="H58" s="79"/>
-      <c r="I58" s="79"/>
-      <c r="J58" s="79"/>
-      <c r="K58" s="79"/>
-      <c r="L58" s="79"/>
-      <c r="M58" s="79"/>
-      <c r="N58" s="79"/>
-      <c r="O58" s="79"/>
-      <c r="P58" s="79"/>
-      <c r="Q58" s="79"/>
-      <c r="R58" s="79"/>
-      <c r="S58" s="79"/>
-      <c r="T58" s="79"/>
-      <c r="U58" s="79"/>
-      <c r="V58" s="79"/>
-      <c r="W58" s="79"/>
-      <c r="X58" s="79"/>
-      <c r="Y58" s="79"/>
-      <c r="Z58" s="79"/>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="B59" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C59" s="81" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E59" s="45"/>
-      <c r="F59" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="G59" s="78"/>
-      <c r="H59" s="79"/>
-      <c r="I59" s="79"/>
-      <c r="J59" s="79"/>
-      <c r="K59" s="79"/>
-      <c r="L59" s="79"/>
-      <c r="M59" s="79"/>
-      <c r="N59" s="79"/>
-      <c r="O59" s="79"/>
-      <c r="P59" s="79"/>
-      <c r="Q59" s="79"/>
-      <c r="R59" s="79"/>
-      <c r="S59" s="79"/>
-      <c r="T59" s="79"/>
-      <c r="U59" s="79"/>
-      <c r="V59" s="79"/>
-      <c r="W59" s="79"/>
-      <c r="X59" s="79"/>
-      <c r="Y59" s="79"/>
-      <c r="Z59" s="79"/>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B60" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="C60" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E60" s="45"/>
-      <c r="F60" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G60" s="78"/>
-      <c r="H60" s="79"/>
-      <c r="I60" s="79"/>
-      <c r="J60" s="79"/>
-      <c r="K60" s="79"/>
-      <c r="L60" s="79"/>
-      <c r="M60" s="79"/>
-      <c r="N60" s="79"/>
-      <c r="O60" s="79"/>
-      <c r="P60" s="79"/>
-      <c r="Q60" s="79"/>
-      <c r="R60" s="79"/>
-      <c r="S60" s="79"/>
-      <c r="T60" s="79"/>
-      <c r="U60" s="79"/>
-      <c r="V60" s="79"/>
-      <c r="W60" s="79"/>
-      <c r="X60" s="79"/>
-      <c r="Y60" s="79"/>
-      <c r="Z60" s="79"/>
+      <c r="G60" s="5"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="45" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B61" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="C61" s="81" t="s">
-        <v>177</v>
+        <v>179</v>
+      </c>
+      <c r="C61" s="45" t="s">
+        <v>180</v>
       </c>
       <c r="D61" s="45" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E61" s="45"/>
       <c r="F61" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="G61" s="78"/>
-      <c r="H61" s="79"/>
-      <c r="I61" s="79"/>
-      <c r="J61" s="79"/>
-      <c r="K61" s="79"/>
-      <c r="L61" s="79"/>
-      <c r="M61" s="79"/>
-      <c r="N61" s="79"/>
-      <c r="O61" s="79"/>
-      <c r="P61" s="79"/>
-      <c r="Q61" s="79"/>
-      <c r="R61" s="79"/>
-      <c r="S61" s="79"/>
-      <c r="T61" s="79"/>
-      <c r="U61" s="79"/>
-      <c r="V61" s="79"/>
-      <c r="W61" s="79"/>
-      <c r="X61" s="79"/>
-      <c r="Y61" s="79"/>
-      <c r="Z61" s="79"/>
+        <v>13</v>
+      </c>
+      <c r="G61" s="87"/>
+      <c r="H61" s="88"/>
+      <c r="I61" s="88"/>
+      <c r="J61" s="88"/>
+      <c r="K61" s="88"/>
+      <c r="L61" s="88"/>
+      <c r="M61" s="88"/>
+      <c r="N61" s="88"/>
+      <c r="O61" s="88"/>
+      <c r="P61" s="88"/>
+      <c r="Q61" s="88"/>
+      <c r="R61" s="88"/>
+      <c r="S61" s="88"/>
+      <c r="T61" s="88"/>
+      <c r="U61" s="88"/>
+      <c r="V61" s="88"/>
+      <c r="W61" s="88"/>
+      <c r="X61" s="88"/>
+      <c r="Y61" s="88"/>
+      <c r="Z61" s="88"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="45" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="B62" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="C62" s="45" t="s">
-        <v>142</v>
+        <v>182</v>
+      </c>
+      <c r="C62" s="89" t="s">
+        <v>183</v>
       </c>
       <c r="D62" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E62" s="45"/>
       <c r="F62" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="G62" s="78"/>
-      <c r="H62" s="79"/>
-      <c r="I62" s="79"/>
-      <c r="J62" s="79"/>
-      <c r="K62" s="79"/>
-      <c r="L62" s="79"/>
-      <c r="M62" s="79"/>
-      <c r="N62" s="79"/>
-      <c r="O62" s="79"/>
-      <c r="P62" s="79"/>
-      <c r="Q62" s="79"/>
-      <c r="R62" s="79"/>
-      <c r="S62" s="79"/>
-      <c r="T62" s="79"/>
-      <c r="U62" s="79"/>
-      <c r="V62" s="79"/>
-      <c r="W62" s="79"/>
-      <c r="X62" s="79"/>
-      <c r="Y62" s="79"/>
-      <c r="Z62" s="79"/>
+        <v>184</v>
+      </c>
+      <c r="G62" s="87"/>
+      <c r="H62" s="88"/>
+      <c r="I62" s="88"/>
+      <c r="J62" s="88"/>
+      <c r="K62" s="88"/>
+      <c r="L62" s="88"/>
+      <c r="M62" s="88"/>
+      <c r="N62" s="88"/>
+      <c r="O62" s="88"/>
+      <c r="P62" s="88"/>
+      <c r="Q62" s="88"/>
+      <c r="R62" s="88"/>
+      <c r="S62" s="88"/>
+      <c r="T62" s="88"/>
+      <c r="U62" s="88"/>
+      <c r="V62" s="88"/>
+      <c r="W62" s="88"/>
+      <c r="X62" s="88"/>
+      <c r="Y62" s="88"/>
+      <c r="Z62" s="88"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="45" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="B63" s="45" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E63" s="45"/>
       <c r="F63" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="G63" s="78"/>
-      <c r="H63" s="79"/>
-      <c r="I63" s="79"/>
-      <c r="J63" s="79"/>
-      <c r="K63" s="79"/>
-      <c r="L63" s="79"/>
-      <c r="M63" s="79"/>
-      <c r="N63" s="79"/>
-      <c r="O63" s="79"/>
-      <c r="P63" s="79"/>
-      <c r="Q63" s="79"/>
-      <c r="R63" s="79"/>
-      <c r="S63" s="79"/>
-      <c r="T63" s="79"/>
-      <c r="U63" s="79"/>
-      <c r="V63" s="79"/>
-      <c r="W63" s="79"/>
-      <c r="X63" s="79"/>
-      <c r="Y63" s="79"/>
-      <c r="Z63" s="79"/>
+        <v>188</v>
+      </c>
+      <c r="G63" s="87"/>
+      <c r="H63" s="88"/>
+      <c r="I63" s="88"/>
+      <c r="J63" s="88"/>
+      <c r="K63" s="88"/>
+      <c r="L63" s="88"/>
+      <c r="M63" s="88"/>
+      <c r="N63" s="88"/>
+      <c r="O63" s="88"/>
+      <c r="P63" s="88"/>
+      <c r="Q63" s="88"/>
+      <c r="R63" s="88"/>
+      <c r="S63" s="88"/>
+      <c r="T63" s="88"/>
+      <c r="U63" s="88"/>
+      <c r="V63" s="88"/>
+      <c r="W63" s="88"/>
+      <c r="X63" s="88"/>
+      <c r="Y63" s="88"/>
+      <c r="Z63" s="88"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="4"/>
-      <c r="G64" s="5"/>
+      <c r="A64" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B64" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" s="89" t="s">
+        <v>191</v>
+      </c>
+      <c r="D64" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" s="45"/>
+      <c r="F64" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G64" s="87"/>
+      <c r="H64" s="88"/>
+      <c r="I64" s="88"/>
+      <c r="J64" s="88"/>
+      <c r="K64" s="88"/>
+      <c r="L64" s="88"/>
+      <c r="M64" s="88"/>
+      <c r="N64" s="88"/>
+      <c r="O64" s="88"/>
+      <c r="P64" s="88"/>
+      <c r="Q64" s="88"/>
+      <c r="R64" s="88"/>
+      <c r="S64" s="88"/>
+      <c r="T64" s="88"/>
+      <c r="U64" s="88"/>
+      <c r="V64" s="88"/>
+      <c r="W64" s="88"/>
+      <c r="X64" s="88"/>
+      <c r="Y64" s="88"/>
+      <c r="Z64" s="88"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G65" s="5"/>
+      <c r="A65" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="C65" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" s="45"/>
+      <c r="F65" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="G65" s="87"/>
+      <c r="H65" s="88"/>
+      <c r="I65" s="88"/>
+      <c r="J65" s="88"/>
+      <c r="K65" s="88"/>
+      <c r="L65" s="88"/>
+      <c r="M65" s="88"/>
+      <c r="N65" s="88"/>
+      <c r="O65" s="88"/>
+      <c r="P65" s="88"/>
+      <c r="Q65" s="88"/>
+      <c r="R65" s="88"/>
+      <c r="S65" s="88"/>
+      <c r="T65" s="88"/>
+      <c r="U65" s="88"/>
+      <c r="V65" s="88"/>
+      <c r="W65" s="88"/>
+      <c r="X65" s="88"/>
+      <c r="Y65" s="88"/>
+      <c r="Z65" s="88"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="4"/>
-      <c r="G66" s="5"/>
+      <c r="A66" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="C66" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="D66" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" s="45"/>
+      <c r="F66" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G66" s="87"/>
+      <c r="H66" s="88"/>
+      <c r="I66" s="88"/>
+      <c r="J66" s="88"/>
+      <c r="K66" s="88"/>
+      <c r="L66" s="88"/>
+      <c r="M66" s="88"/>
+      <c r="N66" s="88"/>
+      <c r="O66" s="88"/>
+      <c r="P66" s="88"/>
+      <c r="Q66" s="88"/>
+      <c r="R66" s="88"/>
+      <c r="S66" s="88"/>
+      <c r="T66" s="88"/>
+      <c r="U66" s="88"/>
+      <c r="V66" s="88"/>
+      <c r="W66" s="88"/>
+      <c r="X66" s="88"/>
+      <c r="Y66" s="88"/>
+      <c r="Z66" s="88"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G67" s="5"/>
+      <c r="A67" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="B67" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" s="45"/>
+      <c r="F67" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="G67" s="87"/>
+      <c r="H67" s="88"/>
+      <c r="I67" s="88"/>
+      <c r="J67" s="88"/>
+      <c r="K67" s="88"/>
+      <c r="L67" s="88"/>
+      <c r="M67" s="88"/>
+      <c r="N67" s="88"/>
+      <c r="O67" s="88"/>
+      <c r="P67" s="88"/>
+      <c r="Q67" s="88"/>
+      <c r="R67" s="88"/>
+      <c r="S67" s="88"/>
+      <c r="T67" s="88"/>
+      <c r="U67" s="88"/>
+      <c r="V67" s="88"/>
+      <c r="W67" s="88"/>
+      <c r="X67" s="88"/>
+      <c r="Y67" s="88"/>
+      <c r="Z67" s="88"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="45" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="B68" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="C68" s="80" t="s">
-        <v>182</v>
+        <v>200</v>
+      </c>
+      <c r="C68" s="90" t="s">
+        <v>201</v>
       </c>
       <c r="D68" s="45" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E68" s="45"/>
       <c r="F68" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="78"/>
-      <c r="H68" s="79"/>
-      <c r="I68" s="79"/>
-      <c r="J68" s="79"/>
-      <c r="K68" s="79"/>
-      <c r="L68" s="79"/>
-      <c r="M68" s="79"/>
-      <c r="N68" s="79"/>
-      <c r="O68" s="79"/>
-      <c r="P68" s="79"/>
-      <c r="Q68" s="79"/>
-      <c r="R68" s="79"/>
-      <c r="S68" s="79"/>
-      <c r="T68" s="79"/>
-      <c r="U68" s="79"/>
-      <c r="V68" s="79"/>
-      <c r="W68" s="79"/>
-      <c r="X68" s="79"/>
-      <c r="Y68" s="79"/>
-      <c r="Z68" s="79"/>
+        <v>184</v>
+      </c>
+      <c r="G68" s="87"/>
+      <c r="H68" s="88"/>
+      <c r="I68" s="88"/>
+      <c r="J68" s="88"/>
+      <c r="K68" s="88"/>
+      <c r="L68" s="88"/>
+      <c r="M68" s="88"/>
+      <c r="N68" s="88"/>
+      <c r="O68" s="88"/>
+      <c r="P68" s="88"/>
+      <c r="Q68" s="88"/>
+      <c r="R68" s="88"/>
+      <c r="S68" s="88"/>
+      <c r="T68" s="88"/>
+      <c r="U68" s="88"/>
+      <c r="V68" s="88"/>
+      <c r="W68" s="88"/>
+      <c r="X68" s="88"/>
+      <c r="Y68" s="88"/>
+      <c r="Z68" s="88"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="45" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B69" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="C69" s="80" t="s">
-        <v>185</v>
+        <v>202</v>
+      </c>
+      <c r="C69" s="45" t="s">
+        <v>198</v>
       </c>
       <c r="D69" s="45" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="E69" s="45"/>
       <c r="F69" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G69" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="H69" s="79"/>
-      <c r="I69" s="79"/>
-      <c r="J69" s="79"/>
-      <c r="K69" s="79"/>
-      <c r="L69" s="79"/>
-      <c r="M69" s="79"/>
-      <c r="N69" s="79"/>
-      <c r="O69" s="79"/>
-      <c r="P69" s="79"/>
-      <c r="Q69" s="79"/>
-      <c r="R69" s="79"/>
-      <c r="S69" s="79"/>
-      <c r="T69" s="79"/>
-      <c r="U69" s="79"/>
-      <c r="V69" s="79"/>
-      <c r="W69" s="79"/>
-      <c r="X69" s="79"/>
-      <c r="Y69" s="79"/>
-      <c r="Z69" s="79"/>
+        <v>167</v>
+      </c>
+      <c r="G69" s="87"/>
+      <c r="H69" s="88"/>
+      <c r="I69" s="88"/>
+      <c r="J69" s="88"/>
+      <c r="K69" s="88"/>
+      <c r="L69" s="88"/>
+      <c r="M69" s="88"/>
+      <c r="N69" s="88"/>
+      <c r="O69" s="88"/>
+      <c r="P69" s="88"/>
+      <c r="Q69" s="88"/>
+      <c r="R69" s="88"/>
+      <c r="S69" s="88"/>
+      <c r="T69" s="88"/>
+      <c r="U69" s="88"/>
+      <c r="V69" s="88"/>
+      <c r="W69" s="88"/>
+      <c r="X69" s="88"/>
+      <c r="Y69" s="88"/>
+      <c r="Z69" s="88"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="45" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="B70" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C70" s="80" t="s">
-        <v>188</v>
+        <v>204</v>
+      </c>
+      <c r="C70" s="90" t="s">
+        <v>205</v>
       </c>
       <c r="D70" s="45" t="s">
-        <v>189</v>
+        <v>30</v>
       </c>
       <c r="E70" s="45"/>
       <c r="F70" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="G70" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="H70" s="79"/>
-      <c r="I70" s="79"/>
-      <c r="J70" s="79"/>
-      <c r="K70" s="79"/>
-      <c r="L70" s="79"/>
-      <c r="M70" s="79"/>
-      <c r="N70" s="79"/>
-      <c r="O70" s="79"/>
-      <c r="P70" s="79"/>
-      <c r="Q70" s="79"/>
-      <c r="R70" s="79"/>
-      <c r="S70" s="79"/>
-      <c r="T70" s="79"/>
-      <c r="U70" s="79"/>
-      <c r="V70" s="79"/>
-      <c r="W70" s="79"/>
-      <c r="X70" s="79"/>
-      <c r="Y70" s="79"/>
-      <c r="Z70" s="79"/>
+        <v>206</v>
+      </c>
+      <c r="G70" s="87"/>
+      <c r="H70" s="88"/>
+      <c r="I70" s="88"/>
+      <c r="J70" s="88"/>
+      <c r="K70" s="88"/>
+      <c r="L70" s="88"/>
+      <c r="M70" s="88"/>
+      <c r="N70" s="88"/>
+      <c r="O70" s="88"/>
+      <c r="P70" s="88"/>
+      <c r="Q70" s="88"/>
+      <c r="R70" s="88"/>
+      <c r="S70" s="88"/>
+      <c r="T70" s="88"/>
+      <c r="U70" s="88"/>
+      <c r="V70" s="88"/>
+      <c r="W70" s="88"/>
+      <c r="X70" s="88"/>
+      <c r="Y70" s="88"/>
+      <c r="Z70" s="88"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="45" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="C71" s="45" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="D71" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E71" s="82"/>
+        <v>86</v>
+      </c>
+      <c r="E71" s="45"/>
       <c r="F71" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G71" s="78"/>
-      <c r="H71" s="79"/>
-      <c r="I71" s="79"/>
-      <c r="J71" s="79"/>
-      <c r="K71" s="79"/>
-      <c r="L71" s="79"/>
-      <c r="M71" s="79"/>
-      <c r="N71" s="79"/>
-      <c r="O71" s="79"/>
-      <c r="P71" s="79"/>
-      <c r="Q71" s="79"/>
-      <c r="R71" s="79"/>
-      <c r="S71" s="79"/>
-      <c r="T71" s="79"/>
-      <c r="U71" s="79"/>
-      <c r="V71" s="79"/>
-      <c r="W71" s="79"/>
-      <c r="X71" s="79"/>
-      <c r="Y71" s="79"/>
-      <c r="Z71" s="79"/>
+        <v>171</v>
+      </c>
+      <c r="G71" s="87"/>
+      <c r="H71" s="88"/>
+      <c r="I71" s="88"/>
+      <c r="J71" s="88"/>
+      <c r="K71" s="88"/>
+      <c r="L71" s="88"/>
+      <c r="M71" s="88"/>
+      <c r="N71" s="88"/>
+      <c r="O71" s="88"/>
+      <c r="P71" s="88"/>
+      <c r="Q71" s="88"/>
+      <c r="R71" s="88"/>
+      <c r="S71" s="88"/>
+      <c r="T71" s="88"/>
+      <c r="U71" s="88"/>
+      <c r="V71" s="88"/>
+      <c r="W71" s="88"/>
+      <c r="X71" s="88"/>
+      <c r="Y71" s="88"/>
+      <c r="Z71" s="88"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="45" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="B72" s="45" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="C72" s="45" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D72" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="82"/>
+        <v>86</v>
+      </c>
+      <c r="E72" s="45"/>
       <c r="F72" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G72" s="78"/>
-      <c r="H72" s="79"/>
-      <c r="I72" s="79"/>
-      <c r="J72" s="79"/>
-      <c r="K72" s="79"/>
-      <c r="L72" s="79"/>
-      <c r="M72" s="79"/>
-      <c r="N72" s="79"/>
-      <c r="O72" s="79"/>
-      <c r="P72" s="79"/>
-      <c r="Q72" s="79"/>
-      <c r="R72" s="79"/>
-      <c r="S72" s="79"/>
-      <c r="T72" s="79"/>
-      <c r="U72" s="79"/>
-      <c r="V72" s="79"/>
-      <c r="W72" s="79"/>
-      <c r="X72" s="79"/>
-      <c r="Y72" s="79"/>
-      <c r="Z72" s="79"/>
+        <v>171</v>
+      </c>
+      <c r="G72" s="87"/>
+      <c r="H72" s="88"/>
+      <c r="I72" s="88"/>
+      <c r="J72" s="88"/>
+      <c r="K72" s="88"/>
+      <c r="L72" s="88"/>
+      <c r="M72" s="88"/>
+      <c r="N72" s="88"/>
+      <c r="O72" s="88"/>
+      <c r="P72" s="88"/>
+      <c r="Q72" s="88"/>
+      <c r="R72" s="88"/>
+      <c r="S72" s="88"/>
+      <c r="T72" s="88"/>
+      <c r="U72" s="88"/>
+      <c r="V72" s="88"/>
+      <c r="W72" s="88"/>
+      <c r="X72" s="88"/>
+      <c r="Y72" s="88"/>
+      <c r="Z72" s="88"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="45" t="s">
-        <v>197</v>
-      </c>
-      <c r="B73" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="C73" s="80" t="s">
-        <v>199</v>
-      </c>
-      <c r="D73" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="45"/>
-      <c r="F73" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G73" s="78"/>
-      <c r="H73" s="79"/>
-      <c r="I73" s="79"/>
-      <c r="J73" s="79"/>
-      <c r="K73" s="79"/>
-      <c r="L73" s="79"/>
-      <c r="M73" s="79"/>
-      <c r="N73" s="79"/>
-      <c r="O73" s="79"/>
-      <c r="P73" s="79"/>
-      <c r="Q73" s="79"/>
-      <c r="R73" s="79"/>
-      <c r="S73" s="79"/>
-      <c r="T73" s="79"/>
-      <c r="U73" s="79"/>
-      <c r="V73" s="79"/>
-      <c r="W73" s="79"/>
-      <c r="X73" s="79"/>
-      <c r="Y73" s="79"/>
-      <c r="Z73" s="79"/>
+      <c r="A73" s="4"/>
+      <c r="G73" s="5"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="45" t="s">
-        <v>200</v>
-      </c>
-      <c r="B74" s="45" t="s">
-        <v>201</v>
-      </c>
-      <c r="C74" s="45" t="s">
-        <v>202</v>
-      </c>
-      <c r="D74" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E74" s="82"/>
-      <c r="F74" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G74" s="78"/>
-      <c r="H74" s="79"/>
-      <c r="I74" s="79"/>
-      <c r="J74" s="79"/>
-      <c r="K74" s="79"/>
-      <c r="L74" s="79"/>
-      <c r="M74" s="79"/>
-      <c r="N74" s="79"/>
-      <c r="O74" s="79"/>
-      <c r="P74" s="79"/>
-      <c r="Q74" s="79"/>
-      <c r="R74" s="79"/>
-      <c r="S74" s="79"/>
-      <c r="T74" s="79"/>
-      <c r="U74" s="79"/>
-      <c r="V74" s="79"/>
-      <c r="W74" s="79"/>
-      <c r="X74" s="79"/>
-      <c r="Y74" s="79"/>
-      <c r="Z74" s="79"/>
+      <c r="A74" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G74" s="5"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="45" t="s">
-        <v>203</v>
-      </c>
-      <c r="B75" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="C75" s="80" t="s">
-        <v>205</v>
-      </c>
-      <c r="D75" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E75" s="45"/>
-      <c r="F75" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G75" s="78"/>
-      <c r="H75" s="79"/>
-      <c r="I75" s="79"/>
-      <c r="J75" s="79"/>
-      <c r="K75" s="79"/>
-      <c r="L75" s="79"/>
-      <c r="M75" s="79"/>
-      <c r="N75" s="79"/>
-      <c r="O75" s="79"/>
-      <c r="P75" s="79"/>
-      <c r="Q75" s="79"/>
-      <c r="R75" s="79"/>
-      <c r="S75" s="79"/>
-      <c r="T75" s="79"/>
-      <c r="U75" s="79"/>
-      <c r="V75" s="79"/>
-      <c r="W75" s="79"/>
-      <c r="X75" s="79"/>
-      <c r="Y75" s="79"/>
-      <c r="Z75" s="79"/>
+      <c r="A75" s="4"/>
+      <c r="G75" s="5"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="45" t="s">
-        <v>206</v>
-      </c>
-      <c r="B76" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C76" s="45" t="s">
-        <v>207</v>
-      </c>
-      <c r="D76" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="E76" s="45"/>
-      <c r="F76" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G76" s="78"/>
-      <c r="H76" s="79"/>
-      <c r="I76" s="79"/>
-      <c r="J76" s="79"/>
-      <c r="K76" s="79"/>
-      <c r="L76" s="79"/>
-      <c r="M76" s="79"/>
-      <c r="N76" s="79"/>
-      <c r="O76" s="79"/>
-      <c r="P76" s="79"/>
-      <c r="Q76" s="79"/>
-      <c r="R76" s="79"/>
-      <c r="S76" s="79"/>
-      <c r="T76" s="79"/>
-      <c r="U76" s="79"/>
-      <c r="V76" s="79"/>
-      <c r="W76" s="79"/>
-      <c r="X76" s="79"/>
-      <c r="Y76" s="79"/>
-      <c r="Z76" s="79"/>
+      <c r="A76" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G76" s="5"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="45" t="s">
-        <v>135</v>
+        <v>208</v>
       </c>
       <c r="B77" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="C77" s="45" t="s">
         <v>209</v>
       </c>
+      <c r="C77" s="89" t="s">
+        <v>210</v>
+      </c>
       <c r="D77" s="45" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E77" s="45"/>
       <c r="F77" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G77" s="78"/>
-      <c r="H77" s="79"/>
-      <c r="I77" s="79"/>
-      <c r="J77" s="79"/>
-      <c r="K77" s="79"/>
-      <c r="L77" s="79"/>
-      <c r="M77" s="79"/>
-      <c r="N77" s="79"/>
-      <c r="O77" s="79"/>
-      <c r="P77" s="79"/>
-      <c r="Q77" s="79"/>
-      <c r="R77" s="79"/>
-      <c r="S77" s="79"/>
-      <c r="T77" s="79"/>
-      <c r="U77" s="79"/>
-      <c r="V77" s="79"/>
-      <c r="W77" s="79"/>
-      <c r="X77" s="79"/>
-      <c r="Y77" s="79"/>
-      <c r="Z77" s="79"/>
+        <v>13</v>
+      </c>
+      <c r="G77" s="87"/>
+      <c r="H77" s="88"/>
+      <c r="I77" s="88"/>
+      <c r="J77" s="88"/>
+      <c r="K77" s="88"/>
+      <c r="L77" s="88"/>
+      <c r="M77" s="88"/>
+      <c r="N77" s="88"/>
+      <c r="O77" s="88"/>
+      <c r="P77" s="88"/>
+      <c r="Q77" s="88"/>
+      <c r="R77" s="88"/>
+      <c r="S77" s="88"/>
+      <c r="T77" s="88"/>
+      <c r="U77" s="88"/>
+      <c r="V77" s="88"/>
+      <c r="W77" s="88"/>
+      <c r="X77" s="88"/>
+      <c r="Y77" s="88"/>
+      <c r="Z77" s="88"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="45" t="s">
-        <v>140</v>
+        <v>211</v>
       </c>
       <c r="B78" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="C78" s="45" t="s">
-        <v>210</v>
+        <v>212</v>
+      </c>
+      <c r="C78" s="89" t="s">
+        <v>213</v>
       </c>
       <c r="D78" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E78" s="82"/>
+        <v>11</v>
+      </c>
+      <c r="E78" s="45"/>
       <c r="F78" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="G78" s="78"/>
-      <c r="H78" s="79"/>
-      <c r="I78" s="79"/>
-      <c r="J78" s="79"/>
-      <c r="K78" s="79"/>
-      <c r="L78" s="79"/>
-      <c r="M78" s="79"/>
-      <c r="N78" s="79"/>
-      <c r="O78" s="79"/>
-      <c r="P78" s="79"/>
-      <c r="Q78" s="79"/>
-      <c r="R78" s="79"/>
-      <c r="S78" s="79"/>
-      <c r="T78" s="79"/>
-      <c r="U78" s="79"/>
-      <c r="V78" s="79"/>
-      <c r="W78" s="79"/>
-      <c r="X78" s="79"/>
-      <c r="Y78" s="79"/>
-      <c r="Z78" s="79"/>
+        <v>13</v>
+      </c>
+      <c r="G78" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="H78" s="88"/>
+      <c r="I78" s="88"/>
+      <c r="J78" s="88"/>
+      <c r="K78" s="88"/>
+      <c r="L78" s="88"/>
+      <c r="M78" s="88"/>
+      <c r="N78" s="88"/>
+      <c r="O78" s="88"/>
+      <c r="P78" s="88"/>
+      <c r="Q78" s="88"/>
+      <c r="R78" s="88"/>
+      <c r="S78" s="88"/>
+      <c r="T78" s="88"/>
+      <c r="U78" s="88"/>
+      <c r="V78" s="88"/>
+      <c r="W78" s="88"/>
+      <c r="X78" s="88"/>
+      <c r="Y78" s="88"/>
+      <c r="Z78" s="88"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="45" t="s">
-        <v>144</v>
+        <v>215</v>
       </c>
       <c r="B79" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="C79" s="45" t="s">
-        <v>146</v>
+        <v>28</v>
+      </c>
+      <c r="C79" s="89" t="s">
+        <v>216</v>
       </c>
       <c r="D79" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="E79" s="45"/>
+      <c r="F79" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="G79" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="H79" s="88"/>
+      <c r="I79" s="88"/>
+      <c r="J79" s="88"/>
+      <c r="K79" s="88"/>
+      <c r="L79" s="88"/>
+      <c r="M79" s="88"/>
+      <c r="N79" s="88"/>
+      <c r="O79" s="88"/>
+      <c r="P79" s="88"/>
+      <c r="Q79" s="88"/>
+      <c r="R79" s="88"/>
+      <c r="S79" s="88"/>
+      <c r="T79" s="88"/>
+      <c r="U79" s="88"/>
+      <c r="V79" s="88"/>
+      <c r="W79" s="88"/>
+      <c r="X79" s="88"/>
+      <c r="Y79" s="88"/>
+      <c r="Z79" s="88"/>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="45" t="s">
+        <v>220</v>
+      </c>
+      <c r="B80" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="D80" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" s="91"/>
+      <c r="F80" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="G80" s="87"/>
+      <c r="H80" s="88"/>
+      <c r="I80" s="88"/>
+      <c r="J80" s="88"/>
+      <c r="K80" s="88"/>
+      <c r="L80" s="88"/>
+      <c r="M80" s="88"/>
+      <c r="N80" s="88"/>
+      <c r="O80" s="88"/>
+      <c r="P80" s="88"/>
+      <c r="Q80" s="88"/>
+      <c r="R80" s="88"/>
+      <c r="S80" s="88"/>
+      <c r="T80" s="88"/>
+      <c r="U80" s="88"/>
+      <c r="V80" s="88"/>
+      <c r="W80" s="88"/>
+      <c r="X80" s="88"/>
+      <c r="Y80" s="88"/>
+      <c r="Z80" s="88"/>
+    </row>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="A81" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="B81" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="C81" s="45" t="s">
+        <v>224</v>
+      </c>
+      <c r="D81" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="91"/>
+      <c r="F81" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="G81" s="87"/>
+      <c r="H81" s="88"/>
+      <c r="I81" s="88"/>
+      <c r="J81" s="88"/>
+      <c r="K81" s="88"/>
+      <c r="L81" s="88"/>
+      <c r="M81" s="88"/>
+      <c r="N81" s="88"/>
+      <c r="O81" s="88"/>
+      <c r="P81" s="88"/>
+      <c r="Q81" s="88"/>
+      <c r="R81" s="88"/>
+      <c r="S81" s="88"/>
+      <c r="T81" s="88"/>
+      <c r="U81" s="88"/>
+      <c r="V81" s="88"/>
+      <c r="W81" s="88"/>
+      <c r="X81" s="88"/>
+      <c r="Y81" s="88"/>
+      <c r="Z81" s="88"/>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="B82" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="C82" s="89" t="s">
+        <v>227</v>
+      </c>
+      <c r="D82" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="45"/>
+      <c r="F82" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G82" s="87"/>
+      <c r="H82" s="88"/>
+      <c r="I82" s="88"/>
+      <c r="J82" s="88"/>
+      <c r="K82" s="88"/>
+      <c r="L82" s="88"/>
+      <c r="M82" s="88"/>
+      <c r="N82" s="88"/>
+      <c r="O82" s="88"/>
+      <c r="P82" s="88"/>
+      <c r="Q82" s="88"/>
+      <c r="R82" s="88"/>
+      <c r="S82" s="88"/>
+      <c r="T82" s="88"/>
+      <c r="U82" s="88"/>
+      <c r="V82" s="88"/>
+      <c r="W82" s="88"/>
+      <c r="X82" s="88"/>
+      <c r="Y82" s="88"/>
+      <c r="Z82" s="88"/>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="B83" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="C83" s="45" t="s">
+        <v>230</v>
+      </c>
+      <c r="D83" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E83" s="91"/>
+      <c r="F83" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G83" s="87"/>
+      <c r="H83" s="88"/>
+      <c r="I83" s="88"/>
+      <c r="J83" s="88"/>
+      <c r="K83" s="88"/>
+      <c r="L83" s="88"/>
+      <c r="M83" s="88"/>
+      <c r="N83" s="88"/>
+      <c r="O83" s="88"/>
+      <c r="P83" s="88"/>
+      <c r="Q83" s="88"/>
+      <c r="R83" s="88"/>
+      <c r="S83" s="88"/>
+      <c r="T83" s="88"/>
+      <c r="U83" s="88"/>
+      <c r="V83" s="88"/>
+      <c r="W83" s="88"/>
+      <c r="X83" s="88"/>
+      <c r="Y83" s="88"/>
+      <c r="Z83" s="88"/>
+    </row>
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="A84" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="B84" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="C84" s="89" t="s">
+        <v>233</v>
+      </c>
+      <c r="D84" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E84" s="45"/>
+      <c r="F84" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="G84" s="87"/>
+      <c r="H84" s="88"/>
+      <c r="I84" s="88"/>
+      <c r="J84" s="88"/>
+      <c r="K84" s="88"/>
+      <c r="L84" s="88"/>
+      <c r="M84" s="88"/>
+      <c r="N84" s="88"/>
+      <c r="O84" s="88"/>
+      <c r="P84" s="88"/>
+      <c r="Q84" s="88"/>
+      <c r="R84" s="88"/>
+      <c r="S84" s="88"/>
+      <c r="T84" s="88"/>
+      <c r="U84" s="88"/>
+      <c r="V84" s="88"/>
+      <c r="W84" s="88"/>
+      <c r="X84" s="88"/>
+      <c r="Y84" s="88"/>
+      <c r="Z84" s="88"/>
+    </row>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="B85" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C85" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="D85" s="45" t="s">
+        <v>236</v>
+      </c>
+      <c r="E85" s="45"/>
+      <c r="F85" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="G85" s="87"/>
+      <c r="H85" s="88"/>
+      <c r="I85" s="88"/>
+      <c r="J85" s="88"/>
+      <c r="K85" s="88"/>
+      <c r="L85" s="88"/>
+      <c r="M85" s="88"/>
+      <c r="N85" s="88"/>
+      <c r="O85" s="88"/>
+      <c r="P85" s="88"/>
+      <c r="Q85" s="88"/>
+      <c r="R85" s="88"/>
+      <c r="S85" s="88"/>
+      <c r="T85" s="88"/>
+      <c r="U85" s="88"/>
+      <c r="V85" s="88"/>
+      <c r="W85" s="88"/>
+      <c r="X85" s="88"/>
+      <c r="Y85" s="88"/>
+      <c r="Z85" s="88"/>
+    </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C86" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="D86" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E86" s="45"/>
+      <c r="F86" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="G86" s="87"/>
+      <c r="H86" s="88"/>
+      <c r="I86" s="88"/>
+      <c r="J86" s="88"/>
+      <c r="K86" s="88"/>
+      <c r="L86" s="88"/>
+      <c r="M86" s="88"/>
+      <c r="N86" s="88"/>
+      <c r="O86" s="88"/>
+      <c r="P86" s="88"/>
+      <c r="Q86" s="88"/>
+      <c r="R86" s="88"/>
+      <c r="S86" s="88"/>
+      <c r="T86" s="88"/>
+      <c r="U86" s="88"/>
+      <c r="V86" s="88"/>
+      <c r="W86" s="88"/>
+      <c r="X86" s="88"/>
+      <c r="Y86" s="88"/>
+      <c r="Z86" s="88"/>
+    </row>
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="A87" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="C87" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="D87" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="E79" s="82"/>
-      <c r="F79" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="G79" s="78"/>
-      <c r="H79" s="79"/>
-      <c r="I79" s="79"/>
-      <c r="J79" s="79"/>
-      <c r="K79" s="79"/>
-      <c r="L79" s="79"/>
-      <c r="M79" s="79"/>
-      <c r="N79" s="79"/>
-      <c r="O79" s="79"/>
-      <c r="P79" s="79"/>
-      <c r="Q79" s="79"/>
-      <c r="R79" s="79"/>
-      <c r="S79" s="79"/>
-      <c r="T79" s="79"/>
-      <c r="U79" s="79"/>
-      <c r="V79" s="79"/>
-      <c r="W79" s="79"/>
-      <c r="X79" s="79"/>
-      <c r="Y79" s="79"/>
-      <c r="Z79" s="79"/>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="4"/>
-      <c r="G80" s="5"/>
-    </row>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="83"/>
-      <c r="G81" s="5"/>
-    </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="G82" s="5"/>
-    </row>
-    <row r="83" ht="15.75" customHeight="1">
-      <c r="G83" s="5"/>
-    </row>
-    <row r="84" ht="15.75" customHeight="1">
-      <c r="G84" s="5"/>
-    </row>
-    <row r="85" ht="15.75" customHeight="1">
-      <c r="G85" s="5"/>
-    </row>
-    <row r="86" ht="15.75" customHeight="1">
-      <c r="G86" s="5"/>
-    </row>
-    <row r="87" ht="15.75" customHeight="1">
-      <c r="G87" s="5"/>
+      <c r="E87" s="91"/>
+      <c r="F87" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G87" s="87"/>
+      <c r="H87" s="88"/>
+      <c r="I87" s="88"/>
+      <c r="J87" s="88"/>
+      <c r="K87" s="88"/>
+      <c r="L87" s="88"/>
+      <c r="M87" s="88"/>
+      <c r="N87" s="88"/>
+      <c r="O87" s="88"/>
+      <c r="P87" s="88"/>
+      <c r="Q87" s="88"/>
+      <c r="R87" s="88"/>
+      <c r="S87" s="88"/>
+      <c r="T87" s="88"/>
+      <c r="U87" s="88"/>
+      <c r="V87" s="88"/>
+      <c r="W87" s="88"/>
+      <c r="X87" s="88"/>
+      <c r="Y87" s="88"/>
+      <c r="Z87" s="88"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="G88" s="5"/>
+      <c r="A88" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C88" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="D88" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" s="91"/>
+      <c r="F88" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G88" s="87"/>
+      <c r="H88" s="88"/>
+      <c r="I88" s="88"/>
+      <c r="J88" s="88"/>
+      <c r="K88" s="88"/>
+      <c r="L88" s="88"/>
+      <c r="M88" s="88"/>
+      <c r="N88" s="88"/>
+      <c r="O88" s="88"/>
+      <c r="P88" s="88"/>
+      <c r="Q88" s="88"/>
+      <c r="R88" s="88"/>
+      <c r="S88" s="88"/>
+      <c r="T88" s="88"/>
+      <c r="U88" s="88"/>
+      <c r="V88" s="88"/>
+      <c r="W88" s="88"/>
+      <c r="X88" s="88"/>
+      <c r="Y88" s="88"/>
+      <c r="Z88" s="88"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
+      <c r="A89" s="4"/>
       <c r="G89" s="5"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
+      <c r="A90" s="92"/>
       <c r="G90" s="5"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
@@ -8046,15 +8703,6 @@
     </row>
     <row r="997" ht="15.75" customHeight="1">
       <c r="G997" s="5"/>
-    </row>
-    <row r="998" ht="15.75" customHeight="1">
-      <c r="G998" s="5"/>
-    </row>
-    <row r="999" ht="15.75" customHeight="1">
-      <c r="G999" s="5"/>
-    </row>
-    <row r="1000" ht="15.75" customHeight="1">
-      <c r="G1000" s="5"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>

<commit_message>
State 6 Implementation v3.0.1 - navigation - Navigation
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="9RE5WWv/1Z/enEj8mWwpWuwrwng687r8dWKhSScwD+w="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="pgWysHQ5Yo9Prt6sSqAqWa/b/LCqrBERFY36Uj/DZCU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="247">
   <si>
     <t>Waterfall Methodology</t>
   </si>
@@ -1694,11 +1694,35 @@
         <color rgb="FF156082"/>
         <sz val="11.0"/>
       </rPr>
-      <t>•	Navigation and AppStatus</t>
+      <t xml:space="preserve"> •        Navigation and AppStatus</t>
     </r>
   </si>
   <si>
     <t>6 hours</t>
+  </si>
+  <si>
+    <t>Create a NavigationController to handle the View Flow</t>
+  </si>
+  <si>
+    <t>NavigationController can be tested via Unit Test</t>
+  </si>
+  <si>
+    <t>03/20/2025</t>
+  </si>
+  <si>
+    <t>Integrate NavigationController in views</t>
+  </si>
+  <si>
+    <t>The views are know working the navigation flow</t>
+  </si>
+  <si>
+    <t>12 hours</t>
+  </si>
+  <si>
+    <t>03/25/2025</t>
+  </si>
+  <si>
+    <t>we had to adapt and change a lot the previous navigation controller</t>
   </si>
   <si>
     <t>Implement the database</t>
@@ -2221,10 +2245,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -2312,6 +2336,11 @@
       <sz val="11.0"/>
       <color rgb="FF156082"/>
       <name val="Quattrocento Sans"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF156082"/>
+      <name val="Aptos Narrow"/>
     </font>
     <font>
       <i/>
@@ -2431,7 +2460,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="96">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2610,23 +2639,33 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="5" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="2" fillId="0" fontId="15" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2652,6 +2691,9 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="15" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -2672,7 +2714,7 @@
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -4436,68 +4478,68 @@
       <c r="D41" s="67"/>
       <c r="E41" s="68"/>
       <c r="F41" s="67"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="69"/>
-      <c r="J41" s="69"/>
-      <c r="K41" s="69"/>
-      <c r="L41" s="69"/>
-      <c r="M41" s="69"/>
-      <c r="N41" s="69"/>
-      <c r="O41" s="69"/>
-      <c r="P41" s="69"/>
-      <c r="Q41" s="69"/>
-      <c r="R41" s="69"/>
-      <c r="S41" s="69"/>
-      <c r="T41" s="69"/>
-      <c r="U41" s="69"/>
-      <c r="V41" s="69"/>
-      <c r="W41" s="69"/>
-      <c r="X41" s="69"/>
-      <c r="Y41" s="69"/>
-      <c r="Z41" s="69"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="67"/>
+      <c r="J41" s="67"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="67"/>
+      <c r="M41" s="67"/>
+      <c r="N41" s="67"/>
+      <c r="O41" s="67"/>
+      <c r="P41" s="67"/>
+      <c r="Q41" s="67"/>
+      <c r="R41" s="67"/>
+      <c r="S41" s="67"/>
+      <c r="T41" s="67"/>
+      <c r="U41" s="67"/>
+      <c r="V41" s="67"/>
+      <c r="W41" s="67"/>
+      <c r="X41" s="67"/>
+      <c r="Y41" s="67"/>
+      <c r="Z41" s="67"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="C42" s="71" t="s">
+      <c r="C42" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="43">
+      <c r="E42" s="70">
         <v>45964.0</v>
       </c>
-      <c r="F42" s="41" t="s">
+      <c r="F42" s="71" t="s">
         <v>107</v>
       </c>
-      <c r="G42" s="64" t="s">
+      <c r="G42" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="42"/>
-      <c r="Q42" s="42"/>
-      <c r="R42" s="42"/>
-      <c r="S42" s="42"/>
-      <c r="T42" s="42"/>
-      <c r="U42" s="42"/>
-      <c r="V42" s="42"/>
-      <c r="W42" s="42"/>
-      <c r="X42" s="42"/>
-      <c r="Y42" s="42"/>
-      <c r="Z42" s="42"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="73"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="73"/>
+      <c r="M42" s="73"/>
+      <c r="N42" s="73"/>
+      <c r="O42" s="73"/>
+      <c r="P42" s="73"/>
+      <c r="Q42" s="73"/>
+      <c r="R42" s="73"/>
+      <c r="S42" s="73"/>
+      <c r="T42" s="73"/>
+      <c r="U42" s="73"/>
+      <c r="V42" s="73"/>
+      <c r="W42" s="73"/>
+      <c r="X42" s="73"/>
+      <c r="Y42" s="73"/>
+      <c r="Z42" s="73"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="13" t="s">
@@ -4718,7 +4760,7 @@
       <c r="F48" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="G48" s="72" t="s">
+      <c r="G48" s="74" t="s">
         <v>154</v>
       </c>
       <c r="H48" s="18"/>
@@ -4748,7 +4790,7 @@
       <c r="B49" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="C49" s="73" t="s">
+      <c r="C49" s="75" t="s">
         <v>156</v>
       </c>
       <c r="D49" s="14" t="s">
@@ -4760,7 +4802,7 @@
       <c r="F49" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="G49" s="72"/>
+      <c r="G49" s="74"/>
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
@@ -4781,119 +4823,125 @@
       <c r="Y49" s="18"/>
       <c r="Z49" s="18"/>
     </row>
-    <row r="50" ht="45.75" customHeight="1">
-      <c r="A50" s="74" t="s">
+    <row r="50" ht="51.75" customHeight="1">
+      <c r="A50" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B50" s="74" t="s">
+      <c r="B50" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C50" s="74" t="s">
+      <c r="C50" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D50" s="74" t="s">
+      <c r="D50" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F50" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G50" s="74"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="18"/>
+      <c r="U50" s="18"/>
+      <c r="V50" s="18"/>
+      <c r="W50" s="18"/>
+      <c r="X50" s="18"/>
+      <c r="Y50" s="18"/>
+      <c r="Z50" s="18"/>
+    </row>
+    <row r="51" ht="51.75" customHeight="1">
+      <c r="A51" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F51" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G51" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
+      <c r="S51" s="18"/>
+      <c r="T51" s="18"/>
+      <c r="U51" s="18"/>
+      <c r="V51" s="18"/>
+      <c r="W51" s="18"/>
+      <c r="X51" s="18"/>
+      <c r="Y51" s="18"/>
+      <c r="Z51" s="18"/>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="75"/>
-      <c r="F50" s="76" t="s">
+      <c r="E52" s="77"/>
+      <c r="F52" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="G50" s="77"/>
-      <c r="H50" s="78"/>
-      <c r="I50" s="78"/>
-      <c r="J50" s="78"/>
-      <c r="K50" s="78"/>
-      <c r="L50" s="78"/>
-      <c r="M50" s="78"/>
-      <c r="N50" s="78"/>
-      <c r="O50" s="78"/>
-      <c r="P50" s="78"/>
-      <c r="Q50" s="78"/>
-      <c r="R50" s="78"/>
-      <c r="S50" s="78"/>
-      <c r="T50" s="78"/>
-      <c r="U50" s="78"/>
-      <c r="V50" s="78"/>
-      <c r="W50" s="78"/>
-      <c r="X50" s="78"/>
-      <c r="Y50" s="78"/>
-      <c r="Z50" s="78"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="C51" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E51" s="79"/>
-      <c r="F51" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G51" s="80"/>
-      <c r="H51" s="81"/>
-      <c r="I51" s="81"/>
-      <c r="J51" s="81"/>
-      <c r="K51" s="81"/>
-      <c r="L51" s="81"/>
-      <c r="M51" s="81"/>
-      <c r="N51" s="81"/>
-      <c r="O51" s="81"/>
-      <c r="P51" s="81"/>
-      <c r="Q51" s="81"/>
-      <c r="R51" s="81"/>
-      <c r="S51" s="81"/>
-      <c r="T51" s="81"/>
-      <c r="U51" s="81"/>
-      <c r="V51" s="81"/>
-      <c r="W51" s="81"/>
-      <c r="X51" s="81"/>
-      <c r="Y51" s="81"/>
-      <c r="Z51" s="81"/>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="E52" s="79"/>
-      <c r="F52" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="G52" s="80"/>
-      <c r="H52" s="81"/>
-      <c r="I52" s="81"/>
-      <c r="J52" s="81"/>
-      <c r="K52" s="81"/>
-      <c r="L52" s="81"/>
-      <c r="M52" s="81"/>
-      <c r="N52" s="81"/>
-      <c r="O52" s="81"/>
-      <c r="P52" s="81"/>
-      <c r="Q52" s="81"/>
-      <c r="R52" s="81"/>
-      <c r="S52" s="81"/>
-      <c r="T52" s="81"/>
-      <c r="U52" s="81"/>
-      <c r="V52" s="81"/>
-      <c r="W52" s="81"/>
-      <c r="X52" s="81"/>
-      <c r="Y52" s="81"/>
-      <c r="Z52" s="81"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="80"/>
+      <c r="I52" s="80"/>
+      <c r="J52" s="80"/>
+      <c r="K52" s="80"/>
+      <c r="L52" s="80"/>
+      <c r="M52" s="80"/>
+      <c r="N52" s="80"/>
+      <c r="O52" s="80"/>
+      <c r="P52" s="80"/>
+      <c r="Q52" s="80"/>
+      <c r="R52" s="80"/>
+      <c r="S52" s="80"/>
+      <c r="T52" s="80"/>
+      <c r="U52" s="80"/>
+      <c r="V52" s="80"/>
+      <c r="W52" s="80"/>
+      <c r="X52" s="80"/>
+      <c r="Y52" s="80"/>
+      <c r="Z52" s="80"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="25" t="s">
@@ -4906,49 +4954,49 @@
         <v>170</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" s="79"/>
+        <v>30</v>
+      </c>
+      <c r="E53" s="81"/>
       <c r="F53" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G53" s="82"/>
+      <c r="H53" s="83"/>
+      <c r="I53" s="83"/>
+      <c r="J53" s="83"/>
+      <c r="K53" s="83"/>
+      <c r="L53" s="83"/>
+      <c r="M53" s="83"/>
+      <c r="N53" s="83"/>
+      <c r="O53" s="83"/>
+      <c r="P53" s="83"/>
+      <c r="Q53" s="83"/>
+      <c r="R53" s="83"/>
+      <c r="S53" s="83"/>
+      <c r="T53" s="83"/>
+      <c r="U53" s="83"/>
+      <c r="V53" s="83"/>
+      <c r="W53" s="83"/>
+      <c r="X53" s="83"/>
+      <c r="Y53" s="83"/>
+      <c r="Z53" s="83"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="G53" s="80"/>
-      <c r="H53" s="81"/>
-      <c r="I53" s="81"/>
-      <c r="J53" s="81"/>
-      <c r="K53" s="81"/>
-      <c r="L53" s="81"/>
-      <c r="M53" s="81"/>
-      <c r="N53" s="81"/>
-      <c r="O53" s="81"/>
-      <c r="P53" s="81"/>
-      <c r="Q53" s="81"/>
-      <c r="R53" s="81"/>
-      <c r="S53" s="81"/>
-      <c r="T53" s="81"/>
-      <c r="U53" s="81"/>
-      <c r="V53" s="81"/>
-      <c r="W53" s="81"/>
-      <c r="X53" s="81"/>
-      <c r="Y53" s="81"/>
-      <c r="Z53" s="81"/>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="8" t="s">
+      <c r="B54" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="C54" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="D54" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="D54" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="9"/>
-      <c r="F54" s="10" t="s">
-        <v>171</v>
+      <c r="E54" s="81"/>
+      <c r="F54" s="28" t="s">
+        <v>175</v>
       </c>
       <c r="G54" s="82"/>
       <c r="H54" s="83"/>
@@ -4972,31 +5020,97 @@
       <c r="Z54" s="83"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="84"/>
-      <c r="B55" s="84"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="85"/>
-      <c r="F55" s="86"/>
-      <c r="G55" s="5"/>
+      <c r="A55" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" s="81"/>
+      <c r="F55" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="G55" s="82"/>
+      <c r="H55" s="83"/>
+      <c r="I55" s="83"/>
+      <c r="J55" s="83"/>
+      <c r="K55" s="83"/>
+      <c r="L55" s="83"/>
+      <c r="M55" s="83"/>
+      <c r="N55" s="83"/>
+      <c r="O55" s="83"/>
+      <c r="P55" s="83"/>
+      <c r="Q55" s="83"/>
+      <c r="R55" s="83"/>
+      <c r="S55" s="83"/>
+      <c r="T55" s="83"/>
+      <c r="U55" s="83"/>
+      <c r="V55" s="83"/>
+      <c r="W55" s="83"/>
+      <c r="X55" s="83"/>
+      <c r="Y55" s="83"/>
+      <c r="Z55" s="83"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="84"/>
-      <c r="B56" s="84"/>
-      <c r="C56" s="84"/>
-      <c r="D56" s="84"/>
-      <c r="E56" s="85"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="5"/>
+      <c r="A56" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="84"/>
+      <c r="F56" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G56" s="85"/>
+      <c r="H56" s="86"/>
+      <c r="I56" s="86"/>
+      <c r="J56" s="86"/>
+      <c r="K56" s="86"/>
+      <c r="L56" s="86"/>
+      <c r="M56" s="86"/>
+      <c r="N56" s="86"/>
+      <c r="O56" s="86"/>
+      <c r="P56" s="86"/>
+      <c r="Q56" s="86"/>
+      <c r="R56" s="86"/>
+      <c r="S56" s="86"/>
+      <c r="T56" s="86"/>
+      <c r="U56" s="86"/>
+      <c r="V56" s="86"/>
+      <c r="W56" s="86"/>
+      <c r="X56" s="86"/>
+      <c r="Y56" s="86"/>
+      <c r="Z56" s="86"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="4"/>
+      <c r="A57" s="87"/>
+      <c r="B57" s="87"/>
+      <c r="C57" s="87"/>
+      <c r="D57" s="87"/>
+      <c r="E57" s="88"/>
+      <c r="F57" s="89"/>
       <c r="G57" s="5"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="A58" s="87"/>
+      <c r="B58" s="87"/>
+      <c r="C58" s="87"/>
+      <c r="D58" s="87"/>
+      <c r="E58" s="88"/>
+      <c r="F58" s="89"/>
       <c r="G58" s="5"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -5004,139 +5118,73 @@
       <c r="G59" s="5"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="4"/>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B62" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="F60" s="7" t="s">
+      <c r="D62" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G60" s="5"/>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="B61" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="C61" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="D61" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E61" s="45"/>
-      <c r="F61" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="87"/>
-      <c r="H61" s="88"/>
-      <c r="I61" s="88"/>
-      <c r="J61" s="88"/>
-      <c r="K61" s="88"/>
-      <c r="L61" s="88"/>
-      <c r="M61" s="88"/>
-      <c r="N61" s="88"/>
-      <c r="O61" s="88"/>
-      <c r="P61" s="88"/>
-      <c r="Q61" s="88"/>
-      <c r="R61" s="88"/>
-      <c r="S61" s="88"/>
-      <c r="T61" s="88"/>
-      <c r="U61" s="88"/>
-      <c r="V61" s="88"/>
-      <c r="W61" s="88"/>
-      <c r="X61" s="88"/>
-      <c r="Y61" s="88"/>
-      <c r="Z61" s="88"/>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="B62" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="C62" s="89" t="s">
-        <v>183</v>
-      </c>
-      <c r="D62" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E62" s="45"/>
-      <c r="F62" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="G62" s="87"/>
-      <c r="H62" s="88"/>
-      <c r="I62" s="88"/>
-      <c r="J62" s="88"/>
-      <c r="K62" s="88"/>
-      <c r="L62" s="88"/>
-      <c r="M62" s="88"/>
-      <c r="N62" s="88"/>
-      <c r="O62" s="88"/>
-      <c r="P62" s="88"/>
-      <c r="Q62" s="88"/>
-      <c r="R62" s="88"/>
-      <c r="S62" s="88"/>
-      <c r="T62" s="88"/>
-      <c r="U62" s="88"/>
-      <c r="V62" s="88"/>
-      <c r="W62" s="88"/>
-      <c r="X62" s="88"/>
-      <c r="Y62" s="88"/>
-      <c r="Z62" s="88"/>
+      <c r="G62" s="5"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="45" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B63" s="45" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E63" s="45"/>
       <c r="F63" s="44" t="s">
-        <v>188</v>
-      </c>
-      <c r="G63" s="87"/>
-      <c r="H63" s="88"/>
-      <c r="I63" s="88"/>
-      <c r="J63" s="88"/>
-      <c r="K63" s="88"/>
-      <c r="L63" s="88"/>
-      <c r="M63" s="88"/>
-      <c r="N63" s="88"/>
-      <c r="O63" s="88"/>
-      <c r="P63" s="88"/>
-      <c r="Q63" s="88"/>
-      <c r="R63" s="88"/>
-      <c r="S63" s="88"/>
-      <c r="T63" s="88"/>
-      <c r="U63" s="88"/>
-      <c r="V63" s="88"/>
-      <c r="W63" s="88"/>
-      <c r="X63" s="88"/>
-      <c r="Y63" s="88"/>
-      <c r="Z63" s="88"/>
+        <v>13</v>
+      </c>
+      <c r="G63" s="90"/>
+      <c r="H63" s="91"/>
+      <c r="I63" s="91"/>
+      <c r="J63" s="91"/>
+      <c r="K63" s="91"/>
+      <c r="L63" s="91"/>
+      <c r="M63" s="91"/>
+      <c r="N63" s="91"/>
+      <c r="O63" s="91"/>
+      <c r="P63" s="91"/>
+      <c r="Q63" s="91"/>
+      <c r="R63" s="91"/>
+      <c r="S63" s="91"/>
+      <c r="T63" s="91"/>
+      <c r="U63" s="91"/>
+      <c r="V63" s="91"/>
+      <c r="W63" s="91"/>
+      <c r="X63" s="91"/>
+      <c r="Y63" s="91"/>
+      <c r="Z63" s="91"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="45" t="s">
@@ -5145,7 +5193,7 @@
       <c r="B64" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="C64" s="89" t="s">
+      <c r="C64" s="92" t="s">
         <v>191</v>
       </c>
       <c r="D64" s="45" t="s">
@@ -5153,840 +5201,910 @@
       </c>
       <c r="E64" s="45"/>
       <c r="F64" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="G64" s="87"/>
-      <c r="H64" s="88"/>
-      <c r="I64" s="88"/>
-      <c r="J64" s="88"/>
-      <c r="K64" s="88"/>
-      <c r="L64" s="88"/>
-      <c r="M64" s="88"/>
-      <c r="N64" s="88"/>
-      <c r="O64" s="88"/>
-      <c r="P64" s="88"/>
-      <c r="Q64" s="88"/>
-      <c r="R64" s="88"/>
-      <c r="S64" s="88"/>
-      <c r="T64" s="88"/>
-      <c r="U64" s="88"/>
-      <c r="V64" s="88"/>
-      <c r="W64" s="88"/>
-      <c r="X64" s="88"/>
-      <c r="Y64" s="88"/>
-      <c r="Z64" s="88"/>
+        <v>192</v>
+      </c>
+      <c r="G64" s="90"/>
+      <c r="H64" s="91"/>
+      <c r="I64" s="91"/>
+      <c r="J64" s="91"/>
+      <c r="K64" s="91"/>
+      <c r="L64" s="91"/>
+      <c r="M64" s="91"/>
+      <c r="N64" s="91"/>
+      <c r="O64" s="91"/>
+      <c r="P64" s="91"/>
+      <c r="Q64" s="91"/>
+      <c r="R64" s="91"/>
+      <c r="S64" s="91"/>
+      <c r="T64" s="91"/>
+      <c r="U64" s="91"/>
+      <c r="V64" s="91"/>
+      <c r="W64" s="91"/>
+      <c r="X64" s="91"/>
+      <c r="Y64" s="91"/>
+      <c r="Z64" s="91"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="45" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B65" s="45" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D65" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E65" s="45"/>
       <c r="F65" s="44" t="s">
-        <v>188</v>
-      </c>
-      <c r="G65" s="87"/>
-      <c r="H65" s="88"/>
-      <c r="I65" s="88"/>
-      <c r="J65" s="88"/>
-      <c r="K65" s="88"/>
-      <c r="L65" s="88"/>
-      <c r="M65" s="88"/>
-      <c r="N65" s="88"/>
-      <c r="O65" s="88"/>
-      <c r="P65" s="88"/>
-      <c r="Q65" s="88"/>
-      <c r="R65" s="88"/>
-      <c r="S65" s="88"/>
-      <c r="T65" s="88"/>
-      <c r="U65" s="88"/>
-      <c r="V65" s="88"/>
-      <c r="W65" s="88"/>
-      <c r="X65" s="88"/>
-      <c r="Y65" s="88"/>
-      <c r="Z65" s="88"/>
+        <v>196</v>
+      </c>
+      <c r="G65" s="90"/>
+      <c r="H65" s="91"/>
+      <c r="I65" s="91"/>
+      <c r="J65" s="91"/>
+      <c r="K65" s="91"/>
+      <c r="L65" s="91"/>
+      <c r="M65" s="91"/>
+      <c r="N65" s="91"/>
+      <c r="O65" s="91"/>
+      <c r="P65" s="91"/>
+      <c r="Q65" s="91"/>
+      <c r="R65" s="91"/>
+      <c r="S65" s="91"/>
+      <c r="T65" s="91"/>
+      <c r="U65" s="91"/>
+      <c r="V65" s="91"/>
+      <c r="W65" s="91"/>
+      <c r="X65" s="91"/>
+      <c r="Y65" s="91"/>
+      <c r="Z65" s="91"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="45" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B66" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="C66" s="89" t="s">
-        <v>196</v>
+        <v>198</v>
+      </c>
+      <c r="C66" s="92" t="s">
+        <v>199</v>
       </c>
       <c r="D66" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E66" s="45"/>
       <c r="F66" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="G66" s="87"/>
-      <c r="H66" s="88"/>
-      <c r="I66" s="88"/>
-      <c r="J66" s="88"/>
-      <c r="K66" s="88"/>
-      <c r="L66" s="88"/>
-      <c r="M66" s="88"/>
-      <c r="N66" s="88"/>
-      <c r="O66" s="88"/>
-      <c r="P66" s="88"/>
-      <c r="Q66" s="88"/>
-      <c r="R66" s="88"/>
-      <c r="S66" s="88"/>
-      <c r="T66" s="88"/>
-      <c r="U66" s="88"/>
-      <c r="V66" s="88"/>
-      <c r="W66" s="88"/>
-      <c r="X66" s="88"/>
-      <c r="Y66" s="88"/>
-      <c r="Z66" s="88"/>
+        <v>192</v>
+      </c>
+      <c r="G66" s="90"/>
+      <c r="H66" s="91"/>
+      <c r="I66" s="91"/>
+      <c r="J66" s="91"/>
+      <c r="K66" s="91"/>
+      <c r="L66" s="91"/>
+      <c r="M66" s="91"/>
+      <c r="N66" s="91"/>
+      <c r="O66" s="91"/>
+      <c r="P66" s="91"/>
+      <c r="Q66" s="91"/>
+      <c r="R66" s="91"/>
+      <c r="S66" s="91"/>
+      <c r="T66" s="91"/>
+      <c r="U66" s="91"/>
+      <c r="V66" s="91"/>
+      <c r="W66" s="91"/>
+      <c r="X66" s="91"/>
+      <c r="Y66" s="91"/>
+      <c r="Z66" s="91"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="45" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B67" s="45" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D67" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E67" s="45"/>
       <c r="F67" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="G67" s="87"/>
-      <c r="H67" s="88"/>
-      <c r="I67" s="88"/>
-      <c r="J67" s="88"/>
-      <c r="K67" s="88"/>
-      <c r="L67" s="88"/>
-      <c r="M67" s="88"/>
-      <c r="N67" s="88"/>
-      <c r="O67" s="88"/>
-      <c r="P67" s="88"/>
-      <c r="Q67" s="88"/>
-      <c r="R67" s="88"/>
-      <c r="S67" s="88"/>
-      <c r="T67" s="88"/>
-      <c r="U67" s="88"/>
-      <c r="V67" s="88"/>
-      <c r="W67" s="88"/>
-      <c r="X67" s="88"/>
-      <c r="Y67" s="88"/>
-      <c r="Z67" s="88"/>
+        <v>196</v>
+      </c>
+      <c r="G67" s="90"/>
+      <c r="H67" s="91"/>
+      <c r="I67" s="91"/>
+      <c r="J67" s="91"/>
+      <c r="K67" s="91"/>
+      <c r="L67" s="91"/>
+      <c r="M67" s="91"/>
+      <c r="N67" s="91"/>
+      <c r="O67" s="91"/>
+      <c r="P67" s="91"/>
+      <c r="Q67" s="91"/>
+      <c r="R67" s="91"/>
+      <c r="S67" s="91"/>
+      <c r="T67" s="91"/>
+      <c r="U67" s="91"/>
+      <c r="V67" s="91"/>
+      <c r="W67" s="91"/>
+      <c r="X67" s="91"/>
+      <c r="Y67" s="91"/>
+      <c r="Z67" s="91"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="45" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B68" s="45" t="s">
-        <v>200</v>
-      </c>
-      <c r="C68" s="90" t="s">
-        <v>201</v>
+        <v>203</v>
+      </c>
+      <c r="C68" s="92" t="s">
+        <v>204</v>
       </c>
       <c r="D68" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E68" s="45"/>
       <c r="F68" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="G68" s="87"/>
-      <c r="H68" s="88"/>
-      <c r="I68" s="88"/>
-      <c r="J68" s="88"/>
-      <c r="K68" s="88"/>
-      <c r="L68" s="88"/>
-      <c r="M68" s="88"/>
-      <c r="N68" s="88"/>
-      <c r="O68" s="88"/>
-      <c r="P68" s="88"/>
-      <c r="Q68" s="88"/>
-      <c r="R68" s="88"/>
-      <c r="S68" s="88"/>
-      <c r="T68" s="88"/>
-      <c r="U68" s="88"/>
-      <c r="V68" s="88"/>
-      <c r="W68" s="88"/>
-      <c r="X68" s="88"/>
-      <c r="Y68" s="88"/>
-      <c r="Z68" s="88"/>
+        <v>192</v>
+      </c>
+      <c r="G68" s="90"/>
+      <c r="H68" s="91"/>
+      <c r="I68" s="91"/>
+      <c r="J68" s="91"/>
+      <c r="K68" s="91"/>
+      <c r="L68" s="91"/>
+      <c r="M68" s="91"/>
+      <c r="N68" s="91"/>
+      <c r="O68" s="91"/>
+      <c r="P68" s="91"/>
+      <c r="Q68" s="91"/>
+      <c r="R68" s="91"/>
+      <c r="S68" s="91"/>
+      <c r="T68" s="91"/>
+      <c r="U68" s="91"/>
+      <c r="V68" s="91"/>
+      <c r="W68" s="91"/>
+      <c r="X68" s="91"/>
+      <c r="Y68" s="91"/>
+      <c r="Z68" s="91"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="45" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B69" s="45" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="D69" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E69" s="45"/>
       <c r="F69" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="G69" s="87"/>
-      <c r="H69" s="88"/>
-      <c r="I69" s="88"/>
-      <c r="J69" s="88"/>
-      <c r="K69" s="88"/>
-      <c r="L69" s="88"/>
-      <c r="M69" s="88"/>
-      <c r="N69" s="88"/>
-      <c r="O69" s="88"/>
-      <c r="P69" s="88"/>
-      <c r="Q69" s="88"/>
-      <c r="R69" s="88"/>
-      <c r="S69" s="88"/>
-      <c r="T69" s="88"/>
-      <c r="U69" s="88"/>
-      <c r="V69" s="88"/>
-      <c r="W69" s="88"/>
-      <c r="X69" s="88"/>
-      <c r="Y69" s="88"/>
-      <c r="Z69" s="88"/>
+        <v>175</v>
+      </c>
+      <c r="G69" s="90"/>
+      <c r="H69" s="91"/>
+      <c r="I69" s="91"/>
+      <c r="J69" s="91"/>
+      <c r="K69" s="91"/>
+      <c r="L69" s="91"/>
+      <c r="M69" s="91"/>
+      <c r="N69" s="91"/>
+      <c r="O69" s="91"/>
+      <c r="P69" s="91"/>
+      <c r="Q69" s="91"/>
+      <c r="R69" s="91"/>
+      <c r="S69" s="91"/>
+      <c r="T69" s="91"/>
+      <c r="U69" s="91"/>
+      <c r="V69" s="91"/>
+      <c r="W69" s="91"/>
+      <c r="X69" s="91"/>
+      <c r="Y69" s="91"/>
+      <c r="Z69" s="91"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="45" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B70" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="C70" s="90" t="s">
-        <v>205</v>
+        <v>208</v>
+      </c>
+      <c r="C70" s="93" t="s">
+        <v>209</v>
       </c>
       <c r="D70" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E70" s="45"/>
       <c r="F70" s="44" t="s">
-        <v>206</v>
-      </c>
-      <c r="G70" s="87"/>
-      <c r="H70" s="88"/>
-      <c r="I70" s="88"/>
-      <c r="J70" s="88"/>
-      <c r="K70" s="88"/>
-      <c r="L70" s="88"/>
-      <c r="M70" s="88"/>
-      <c r="N70" s="88"/>
-      <c r="O70" s="88"/>
-      <c r="P70" s="88"/>
-      <c r="Q70" s="88"/>
-      <c r="R70" s="88"/>
-      <c r="S70" s="88"/>
-      <c r="T70" s="88"/>
-      <c r="U70" s="88"/>
-      <c r="V70" s="88"/>
-      <c r="W70" s="88"/>
-      <c r="X70" s="88"/>
-      <c r="Y70" s="88"/>
-      <c r="Z70" s="88"/>
+        <v>192</v>
+      </c>
+      <c r="G70" s="90"/>
+      <c r="H70" s="91"/>
+      <c r="I70" s="91"/>
+      <c r="J70" s="91"/>
+      <c r="K70" s="91"/>
+      <c r="L70" s="91"/>
+      <c r="M70" s="91"/>
+      <c r="N70" s="91"/>
+      <c r="O70" s="91"/>
+      <c r="P70" s="91"/>
+      <c r="Q70" s="91"/>
+      <c r="R70" s="91"/>
+      <c r="S70" s="91"/>
+      <c r="T70" s="91"/>
+      <c r="U70" s="91"/>
+      <c r="V70" s="91"/>
+      <c r="W70" s="91"/>
+      <c r="X70" s="91"/>
+      <c r="Y70" s="91"/>
+      <c r="Z70" s="91"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="45" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="C71" s="45" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="D71" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E71" s="45"/>
       <c r="F71" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="G71" s="87"/>
-      <c r="H71" s="88"/>
-      <c r="I71" s="88"/>
-      <c r="J71" s="88"/>
-      <c r="K71" s="88"/>
-      <c r="L71" s="88"/>
-      <c r="M71" s="88"/>
-      <c r="N71" s="88"/>
-      <c r="O71" s="88"/>
-      <c r="P71" s="88"/>
-      <c r="Q71" s="88"/>
-      <c r="R71" s="88"/>
-      <c r="S71" s="88"/>
-      <c r="T71" s="88"/>
-      <c r="U71" s="88"/>
-      <c r="V71" s="88"/>
-      <c r="W71" s="88"/>
-      <c r="X71" s="88"/>
-      <c r="Y71" s="88"/>
-      <c r="Z71" s="88"/>
+        <v>175</v>
+      </c>
+      <c r="G71" s="90"/>
+      <c r="H71" s="91"/>
+      <c r="I71" s="91"/>
+      <c r="J71" s="91"/>
+      <c r="K71" s="91"/>
+      <c r="L71" s="91"/>
+      <c r="M71" s="91"/>
+      <c r="N71" s="91"/>
+      <c r="O71" s="91"/>
+      <c r="P71" s="91"/>
+      <c r="Q71" s="91"/>
+      <c r="R71" s="91"/>
+      <c r="S71" s="91"/>
+      <c r="T71" s="91"/>
+      <c r="U71" s="91"/>
+      <c r="V71" s="91"/>
+      <c r="W71" s="91"/>
+      <c r="X71" s="91"/>
+      <c r="Y71" s="91"/>
+      <c r="Z71" s="91"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="45" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="B72" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="C72" s="45" t="s">
-        <v>174</v>
+        <v>212</v>
+      </c>
+      <c r="C72" s="93" t="s">
+        <v>213</v>
       </c>
       <c r="D72" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E72" s="45"/>
       <c r="F72" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="G72" s="87"/>
-      <c r="H72" s="88"/>
-      <c r="I72" s="88"/>
-      <c r="J72" s="88"/>
-      <c r="K72" s="88"/>
-      <c r="L72" s="88"/>
-      <c r="M72" s="88"/>
-      <c r="N72" s="88"/>
-      <c r="O72" s="88"/>
-      <c r="P72" s="88"/>
-      <c r="Q72" s="88"/>
-      <c r="R72" s="88"/>
-      <c r="S72" s="88"/>
-      <c r="T72" s="88"/>
-      <c r="U72" s="88"/>
-      <c r="V72" s="88"/>
-      <c r="W72" s="88"/>
-      <c r="X72" s="88"/>
-      <c r="Y72" s="88"/>
-      <c r="Z72" s="88"/>
+        <v>214</v>
+      </c>
+      <c r="G72" s="90"/>
+      <c r="H72" s="91"/>
+      <c r="I72" s="91"/>
+      <c r="J72" s="91"/>
+      <c r="K72" s="91"/>
+      <c r="L72" s="91"/>
+      <c r="M72" s="91"/>
+      <c r="N72" s="91"/>
+      <c r="O72" s="91"/>
+      <c r="P72" s="91"/>
+      <c r="Q72" s="91"/>
+      <c r="R72" s="91"/>
+      <c r="S72" s="91"/>
+      <c r="T72" s="91"/>
+      <c r="U72" s="91"/>
+      <c r="V72" s="91"/>
+      <c r="W72" s="91"/>
+      <c r="X72" s="91"/>
+      <c r="Y72" s="91"/>
+      <c r="Z72" s="91"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="4"/>
-      <c r="G73" s="5"/>
+      <c r="A73" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="B73" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="D73" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E73" s="45"/>
+      <c r="F73" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="G73" s="90"/>
+      <c r="H73" s="91"/>
+      <c r="I73" s="91"/>
+      <c r="J73" s="91"/>
+      <c r="K73" s="91"/>
+      <c r="L73" s="91"/>
+      <c r="M73" s="91"/>
+      <c r="N73" s="91"/>
+      <c r="O73" s="91"/>
+      <c r="P73" s="91"/>
+      <c r="Q73" s="91"/>
+      <c r="R73" s="91"/>
+      <c r="S73" s="91"/>
+      <c r="T73" s="91"/>
+      <c r="U73" s="91"/>
+      <c r="V73" s="91"/>
+      <c r="W73" s="91"/>
+      <c r="X73" s="91"/>
+      <c r="Y73" s="91"/>
+      <c r="Z73" s="91"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G74" s="5"/>
+      <c r="A74" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="D74" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E74" s="45"/>
+      <c r="F74" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="G74" s="90"/>
+      <c r="H74" s="91"/>
+      <c r="I74" s="91"/>
+      <c r="J74" s="91"/>
+      <c r="K74" s="91"/>
+      <c r="L74" s="91"/>
+      <c r="M74" s="91"/>
+      <c r="N74" s="91"/>
+      <c r="O74" s="91"/>
+      <c r="P74" s="91"/>
+      <c r="Q74" s="91"/>
+      <c r="R74" s="91"/>
+      <c r="S74" s="91"/>
+      <c r="T74" s="91"/>
+      <c r="U74" s="91"/>
+      <c r="V74" s="91"/>
+      <c r="W74" s="91"/>
+      <c r="X74" s="91"/>
+      <c r="Y74" s="91"/>
+      <c r="Z74" s="91"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="4"/>
       <c r="G75" s="5"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G76" s="5"/>
+    </row>
+    <row r="77" ht="15.75" customHeight="1">
+      <c r="A77" s="4"/>
+      <c r="G77" s="5"/>
+    </row>
+    <row r="78" ht="15.75" customHeight="1">
+      <c r="A78" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B78" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="F76" s="7" t="s">
+      <c r="D78" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F78" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G76" s="5"/>
-    </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="B77" s="45" t="s">
-        <v>209</v>
-      </c>
-      <c r="C77" s="89" t="s">
-        <v>210</v>
-      </c>
-      <c r="D77" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E77" s="45"/>
-      <c r="F77" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G77" s="87"/>
-      <c r="H77" s="88"/>
-      <c r="I77" s="88"/>
-      <c r="J77" s="88"/>
-      <c r="K77" s="88"/>
-      <c r="L77" s="88"/>
-      <c r="M77" s="88"/>
-      <c r="N77" s="88"/>
-      <c r="O77" s="88"/>
-      <c r="P77" s="88"/>
-      <c r="Q77" s="88"/>
-      <c r="R77" s="88"/>
-      <c r="S77" s="88"/>
-      <c r="T77" s="88"/>
-      <c r="U77" s="88"/>
-      <c r="V77" s="88"/>
-      <c r="W77" s="88"/>
-      <c r="X77" s="88"/>
-      <c r="Y77" s="88"/>
-      <c r="Z77" s="88"/>
-    </row>
-    <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="B78" s="45" t="s">
-        <v>212</v>
-      </c>
-      <c r="C78" s="89" t="s">
-        <v>213</v>
-      </c>
-      <c r="D78" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="45"/>
-      <c r="F78" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G78" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="H78" s="88"/>
-      <c r="I78" s="88"/>
-      <c r="J78" s="88"/>
-      <c r="K78" s="88"/>
-      <c r="L78" s="88"/>
-      <c r="M78" s="88"/>
-      <c r="N78" s="88"/>
-      <c r="O78" s="88"/>
-      <c r="P78" s="88"/>
-      <c r="Q78" s="88"/>
-      <c r="R78" s="88"/>
-      <c r="S78" s="88"/>
-      <c r="T78" s="88"/>
-      <c r="U78" s="88"/>
-      <c r="V78" s="88"/>
-      <c r="W78" s="88"/>
-      <c r="X78" s="88"/>
-      <c r="Y78" s="88"/>
-      <c r="Z78" s="88"/>
+      <c r="G78" s="5"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="45" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B79" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C79" s="89" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="C79" s="92" t="s">
+        <v>218</v>
       </c>
       <c r="D79" s="45" t="s">
-        <v>217</v>
+        <v>16</v>
       </c>
       <c r="E79" s="45"/>
       <c r="F79" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="G79" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="H79" s="88"/>
-      <c r="I79" s="88"/>
-      <c r="J79" s="88"/>
-      <c r="K79" s="88"/>
-      <c r="L79" s="88"/>
-      <c r="M79" s="88"/>
-      <c r="N79" s="88"/>
-      <c r="O79" s="88"/>
-      <c r="P79" s="88"/>
-      <c r="Q79" s="88"/>
-      <c r="R79" s="88"/>
-      <c r="S79" s="88"/>
-      <c r="T79" s="88"/>
-      <c r="U79" s="88"/>
-      <c r="V79" s="88"/>
-      <c r="W79" s="88"/>
-      <c r="X79" s="88"/>
-      <c r="Y79" s="88"/>
-      <c r="Z79" s="88"/>
+        <v>13</v>
+      </c>
+      <c r="G79" s="90"/>
+      <c r="H79" s="91"/>
+      <c r="I79" s="91"/>
+      <c r="J79" s="91"/>
+      <c r="K79" s="91"/>
+      <c r="L79" s="91"/>
+      <c r="M79" s="91"/>
+      <c r="N79" s="91"/>
+      <c r="O79" s="91"/>
+      <c r="P79" s="91"/>
+      <c r="Q79" s="91"/>
+      <c r="R79" s="91"/>
+      <c r="S79" s="91"/>
+      <c r="T79" s="91"/>
+      <c r="U79" s="91"/>
+      <c r="V79" s="91"/>
+      <c r="W79" s="91"/>
+      <c r="X79" s="91"/>
+      <c r="Y79" s="91"/>
+      <c r="Z79" s="91"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="B80" s="45" t="s">
         <v>220</v>
       </c>
-      <c r="B80" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="C80" s="45" t="s">
+      <c r="C80" s="92" t="s">
         <v>221</v>
       </c>
       <c r="D80" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E80" s="91"/>
+        <v>11</v>
+      </c>
+      <c r="E80" s="45"/>
       <c r="F80" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G80" s="87"/>
-      <c r="H80" s="88"/>
-      <c r="I80" s="88"/>
-      <c r="J80" s="88"/>
-      <c r="K80" s="88"/>
-      <c r="L80" s="88"/>
-      <c r="M80" s="88"/>
-      <c r="N80" s="88"/>
-      <c r="O80" s="88"/>
-      <c r="P80" s="88"/>
-      <c r="Q80" s="88"/>
-      <c r="R80" s="88"/>
-      <c r="S80" s="88"/>
-      <c r="T80" s="88"/>
-      <c r="U80" s="88"/>
-      <c r="V80" s="88"/>
-      <c r="W80" s="88"/>
-      <c r="X80" s="88"/>
-      <c r="Y80" s="88"/>
-      <c r="Z80" s="88"/>
+        <v>13</v>
+      </c>
+      <c r="G80" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="H80" s="91"/>
+      <c r="I80" s="91"/>
+      <c r="J80" s="91"/>
+      <c r="K80" s="91"/>
+      <c r="L80" s="91"/>
+      <c r="M80" s="91"/>
+      <c r="N80" s="91"/>
+      <c r="O80" s="91"/>
+      <c r="P80" s="91"/>
+      <c r="Q80" s="91"/>
+      <c r="R80" s="91"/>
+      <c r="S80" s="91"/>
+      <c r="T80" s="91"/>
+      <c r="U80" s="91"/>
+      <c r="V80" s="91"/>
+      <c r="W80" s="91"/>
+      <c r="X80" s="91"/>
+      <c r="Y80" s="91"/>
+      <c r="Z80" s="91"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="45" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B81" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="C81" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C81" s="92" t="s">
         <v>224</v>
       </c>
       <c r="D81" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="91"/>
+        <v>225</v>
+      </c>
+      <c r="E81" s="45"/>
       <c r="F81" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="G81" s="87"/>
-      <c r="H81" s="88"/>
-      <c r="I81" s="88"/>
-      <c r="J81" s="88"/>
-      <c r="K81" s="88"/>
-      <c r="L81" s="88"/>
-      <c r="M81" s="88"/>
-      <c r="N81" s="88"/>
-      <c r="O81" s="88"/>
-      <c r="P81" s="88"/>
-      <c r="Q81" s="88"/>
-      <c r="R81" s="88"/>
-      <c r="S81" s="88"/>
-      <c r="T81" s="88"/>
-      <c r="U81" s="88"/>
-      <c r="V81" s="88"/>
-      <c r="W81" s="88"/>
-      <c r="X81" s="88"/>
-      <c r="Y81" s="88"/>
-      <c r="Z81" s="88"/>
+        <v>226</v>
+      </c>
+      <c r="G81" s="45" t="s">
+        <v>227</v>
+      </c>
+      <c r="H81" s="91"/>
+      <c r="I81" s="91"/>
+      <c r="J81" s="91"/>
+      <c r="K81" s="91"/>
+      <c r="L81" s="91"/>
+      <c r="M81" s="91"/>
+      <c r="N81" s="91"/>
+      <c r="O81" s="91"/>
+      <c r="P81" s="91"/>
+      <c r="Q81" s="91"/>
+      <c r="R81" s="91"/>
+      <c r="S81" s="91"/>
+      <c r="T81" s="91"/>
+      <c r="U81" s="91"/>
+      <c r="V81" s="91"/>
+      <c r="W81" s="91"/>
+      <c r="X81" s="91"/>
+      <c r="Y81" s="91"/>
+      <c r="Z81" s="91"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="45" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B82" s="45" t="s">
-        <v>226</v>
-      </c>
-      <c r="C82" s="89" t="s">
-        <v>227</v>
+        <v>190</v>
+      </c>
+      <c r="C82" s="45" t="s">
+        <v>229</v>
       </c>
       <c r="D82" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="E82" s="94"/>
       <c r="F82" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G82" s="87"/>
-      <c r="H82" s="88"/>
-      <c r="I82" s="88"/>
-      <c r="J82" s="88"/>
-      <c r="K82" s="88"/>
-      <c r="L82" s="88"/>
-      <c r="M82" s="88"/>
-      <c r="N82" s="88"/>
-      <c r="O82" s="88"/>
-      <c r="P82" s="88"/>
-      <c r="Q82" s="88"/>
-      <c r="R82" s="88"/>
-      <c r="S82" s="88"/>
-      <c r="T82" s="88"/>
-      <c r="U82" s="88"/>
-      <c r="V82" s="88"/>
-      <c r="W82" s="88"/>
-      <c r="X82" s="88"/>
-      <c r="Y82" s="88"/>
-      <c r="Z82" s="88"/>
+        <v>107</v>
+      </c>
+      <c r="G82" s="90"/>
+      <c r="H82" s="91"/>
+      <c r="I82" s="91"/>
+      <c r="J82" s="91"/>
+      <c r="K82" s="91"/>
+      <c r="L82" s="91"/>
+      <c r="M82" s="91"/>
+      <c r="N82" s="91"/>
+      <c r="O82" s="91"/>
+      <c r="P82" s="91"/>
+      <c r="Q82" s="91"/>
+      <c r="R82" s="91"/>
+      <c r="S82" s="91"/>
+      <c r="T82" s="91"/>
+      <c r="U82" s="91"/>
+      <c r="V82" s="91"/>
+      <c r="W82" s="91"/>
+      <c r="X82" s="91"/>
+      <c r="Y82" s="91"/>
+      <c r="Z82" s="91"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="45" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B83" s="45" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C83" s="45" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D83" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E83" s="91"/>
+        <v>11</v>
+      </c>
+      <c r="E83" s="94"/>
       <c r="F83" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G83" s="87"/>
-      <c r="H83" s="88"/>
-      <c r="I83" s="88"/>
-      <c r="J83" s="88"/>
-      <c r="K83" s="88"/>
-      <c r="L83" s="88"/>
-      <c r="M83" s="88"/>
-      <c r="N83" s="88"/>
-      <c r="O83" s="88"/>
-      <c r="P83" s="88"/>
-      <c r="Q83" s="88"/>
-      <c r="R83" s="88"/>
-      <c r="S83" s="88"/>
-      <c r="T83" s="88"/>
-      <c r="U83" s="88"/>
-      <c r="V83" s="88"/>
-      <c r="W83" s="88"/>
-      <c r="X83" s="88"/>
-      <c r="Y83" s="88"/>
-      <c r="Z83" s="88"/>
+        <v>175</v>
+      </c>
+      <c r="G83" s="90"/>
+      <c r="H83" s="91"/>
+      <c r="I83" s="91"/>
+      <c r="J83" s="91"/>
+      <c r="K83" s="91"/>
+      <c r="L83" s="91"/>
+      <c r="M83" s="91"/>
+      <c r="N83" s="91"/>
+      <c r="O83" s="91"/>
+      <c r="P83" s="91"/>
+      <c r="Q83" s="91"/>
+      <c r="R83" s="91"/>
+      <c r="S83" s="91"/>
+      <c r="T83" s="91"/>
+      <c r="U83" s="91"/>
+      <c r="V83" s="91"/>
+      <c r="W83" s="91"/>
+      <c r="X83" s="91"/>
+      <c r="Y83" s="91"/>
+      <c r="Z83" s="91"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="45" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B84" s="45" t="s">
-        <v>232</v>
-      </c>
-      <c r="C84" s="89" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+      <c r="C84" s="92" t="s">
+        <v>235</v>
       </c>
       <c r="D84" s="45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E84" s="45"/>
       <c r="F84" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G84" s="87"/>
-      <c r="H84" s="88"/>
-      <c r="I84" s="88"/>
-      <c r="J84" s="88"/>
-      <c r="K84" s="88"/>
-      <c r="L84" s="88"/>
-      <c r="M84" s="88"/>
-      <c r="N84" s="88"/>
-      <c r="O84" s="88"/>
-      <c r="P84" s="88"/>
-      <c r="Q84" s="88"/>
-      <c r="R84" s="88"/>
-      <c r="S84" s="88"/>
-      <c r="T84" s="88"/>
-      <c r="U84" s="88"/>
-      <c r="V84" s="88"/>
-      <c r="W84" s="88"/>
-      <c r="X84" s="88"/>
-      <c r="Y84" s="88"/>
-      <c r="Z84" s="88"/>
+        <v>54</v>
+      </c>
+      <c r="G84" s="90"/>
+      <c r="H84" s="91"/>
+      <c r="I84" s="91"/>
+      <c r="J84" s="91"/>
+      <c r="K84" s="91"/>
+      <c r="L84" s="91"/>
+      <c r="M84" s="91"/>
+      <c r="N84" s="91"/>
+      <c r="O84" s="91"/>
+      <c r="P84" s="91"/>
+      <c r="Q84" s="91"/>
+      <c r="R84" s="91"/>
+      <c r="S84" s="91"/>
+      <c r="T84" s="91"/>
+      <c r="U84" s="91"/>
+      <c r="V84" s="91"/>
+      <c r="W84" s="91"/>
+      <c r="X84" s="91"/>
+      <c r="Y84" s="91"/>
+      <c r="Z84" s="91"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="45" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B85" s="45" t="s">
-        <v>109</v>
+        <v>237</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D85" s="45" t="s">
-        <v>236</v>
-      </c>
-      <c r="E85" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="E85" s="94"/>
       <c r="F85" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G85" s="87"/>
-      <c r="H85" s="88"/>
-      <c r="I85" s="88"/>
-      <c r="J85" s="88"/>
-      <c r="K85" s="88"/>
-      <c r="L85" s="88"/>
-      <c r="M85" s="88"/>
-      <c r="N85" s="88"/>
-      <c r="O85" s="88"/>
-      <c r="P85" s="88"/>
-      <c r="Q85" s="88"/>
-      <c r="R85" s="88"/>
-      <c r="S85" s="88"/>
-      <c r="T85" s="88"/>
-      <c r="U85" s="88"/>
-      <c r="V85" s="88"/>
-      <c r="W85" s="88"/>
-      <c r="X85" s="88"/>
-      <c r="Y85" s="88"/>
-      <c r="Z85" s="88"/>
+        <v>54</v>
+      </c>
+      <c r="G85" s="90"/>
+      <c r="H85" s="91"/>
+      <c r="I85" s="91"/>
+      <c r="J85" s="91"/>
+      <c r="K85" s="91"/>
+      <c r="L85" s="91"/>
+      <c r="M85" s="91"/>
+      <c r="N85" s="91"/>
+      <c r="O85" s="91"/>
+      <c r="P85" s="91"/>
+      <c r="Q85" s="91"/>
+      <c r="R85" s="91"/>
+      <c r="S85" s="91"/>
+      <c r="T85" s="91"/>
+      <c r="U85" s="91"/>
+      <c r="V85" s="91"/>
+      <c r="W85" s="91"/>
+      <c r="X85" s="91"/>
+      <c r="Y85" s="91"/>
+      <c r="Z85" s="91"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="45" t="s">
-        <v>163</v>
+        <v>239</v>
       </c>
       <c r="B86" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="C86" s="45" t="s">
-        <v>237</v>
+        <v>240</v>
+      </c>
+      <c r="C86" s="92" t="s">
+        <v>241</v>
       </c>
       <c r="D86" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E86" s="45"/>
       <c r="F86" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="G86" s="87"/>
-      <c r="H86" s="88"/>
-      <c r="I86" s="88"/>
-      <c r="J86" s="88"/>
-      <c r="K86" s="88"/>
-      <c r="L86" s="88"/>
-      <c r="M86" s="88"/>
-      <c r="N86" s="88"/>
-      <c r="O86" s="88"/>
-      <c r="P86" s="88"/>
-      <c r="Q86" s="88"/>
-      <c r="R86" s="88"/>
-      <c r="S86" s="88"/>
-      <c r="T86" s="88"/>
-      <c r="U86" s="88"/>
-      <c r="V86" s="88"/>
-      <c r="W86" s="88"/>
-      <c r="X86" s="88"/>
-      <c r="Y86" s="88"/>
-      <c r="Z86" s="88"/>
+        <v>107</v>
+      </c>
+      <c r="G86" s="90"/>
+      <c r="H86" s="91"/>
+      <c r="I86" s="91"/>
+      <c r="J86" s="91"/>
+      <c r="K86" s="91"/>
+      <c r="L86" s="91"/>
+      <c r="M86" s="91"/>
+      <c r="N86" s="91"/>
+      <c r="O86" s="91"/>
+      <c r="P86" s="91"/>
+      <c r="Q86" s="91"/>
+      <c r="R86" s="91"/>
+      <c r="S86" s="91"/>
+      <c r="T86" s="91"/>
+      <c r="U86" s="91"/>
+      <c r="V86" s="91"/>
+      <c r="W86" s="91"/>
+      <c r="X86" s="91"/>
+      <c r="Y86" s="91"/>
+      <c r="Z86" s="91"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="45" t="s">
-        <v>168</v>
+        <v>242</v>
       </c>
       <c r="B87" s="45" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="C87" s="45" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D87" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E87" s="91"/>
+        <v>244</v>
+      </c>
+      <c r="E87" s="45"/>
       <c r="F87" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="G87" s="87"/>
-      <c r="H87" s="88"/>
-      <c r="I87" s="88"/>
-      <c r="J87" s="88"/>
-      <c r="K87" s="88"/>
-      <c r="L87" s="88"/>
-      <c r="M87" s="88"/>
-      <c r="N87" s="88"/>
-      <c r="O87" s="88"/>
-      <c r="P87" s="88"/>
-      <c r="Q87" s="88"/>
-      <c r="R87" s="88"/>
-      <c r="S87" s="88"/>
-      <c r="T87" s="88"/>
-      <c r="U87" s="88"/>
-      <c r="V87" s="88"/>
-      <c r="W87" s="88"/>
-      <c r="X87" s="88"/>
-      <c r="Y87" s="88"/>
-      <c r="Z87" s="88"/>
+        <v>107</v>
+      </c>
+      <c r="G87" s="90"/>
+      <c r="H87" s="91"/>
+      <c r="I87" s="91"/>
+      <c r="J87" s="91"/>
+      <c r="K87" s="91"/>
+      <c r="L87" s="91"/>
+      <c r="M87" s="91"/>
+      <c r="N87" s="91"/>
+      <c r="O87" s="91"/>
+      <c r="P87" s="91"/>
+      <c r="Q87" s="91"/>
+      <c r="R87" s="91"/>
+      <c r="S87" s="91"/>
+      <c r="T87" s="91"/>
+      <c r="U87" s="91"/>
+      <c r="V87" s="91"/>
+      <c r="W87" s="91"/>
+      <c r="X87" s="91"/>
+      <c r="Y87" s="91"/>
+      <c r="Z87" s="91"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B88" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="B88" s="45" t="s">
-        <v>173</v>
-      </c>
       <c r="C88" s="45" t="s">
-        <v>174</v>
+        <v>245</v>
       </c>
       <c r="D88" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E88" s="45"/>
+      <c r="F88" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="G88" s="90"/>
+      <c r="H88" s="91"/>
+      <c r="I88" s="91"/>
+      <c r="J88" s="91"/>
+      <c r="K88" s="91"/>
+      <c r="L88" s="91"/>
+      <c r="M88" s="91"/>
+      <c r="N88" s="91"/>
+      <c r="O88" s="91"/>
+      <c r="P88" s="91"/>
+      <c r="Q88" s="91"/>
+      <c r="R88" s="91"/>
+      <c r="S88" s="91"/>
+      <c r="T88" s="91"/>
+      <c r="U88" s="91"/>
+      <c r="V88" s="91"/>
+      <c r="W88" s="91"/>
+      <c r="X88" s="91"/>
+      <c r="Y88" s="91"/>
+      <c r="Z88" s="91"/>
+    </row>
+    <row r="89" ht="15.75" customHeight="1">
+      <c r="A89" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="C89" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="E88" s="91"/>
-      <c r="F88" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="G88" s="87"/>
-      <c r="H88" s="88"/>
-      <c r="I88" s="88"/>
-      <c r="J88" s="88"/>
-      <c r="K88" s="88"/>
-      <c r="L88" s="88"/>
-      <c r="M88" s="88"/>
-      <c r="N88" s="88"/>
-      <c r="O88" s="88"/>
-      <c r="P88" s="88"/>
-      <c r="Q88" s="88"/>
-      <c r="R88" s="88"/>
-      <c r="S88" s="88"/>
-      <c r="T88" s="88"/>
-      <c r="U88" s="88"/>
-      <c r="V88" s="88"/>
-      <c r="W88" s="88"/>
-      <c r="X88" s="88"/>
-      <c r="Y88" s="88"/>
-      <c r="Z88" s="88"/>
-    </row>
-    <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="4"/>
-      <c r="G89" s="5"/>
+      <c r="E89" s="94"/>
+      <c r="F89" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="G89" s="90"/>
+      <c r="H89" s="91"/>
+      <c r="I89" s="91"/>
+      <c r="J89" s="91"/>
+      <c r="K89" s="91"/>
+      <c r="L89" s="91"/>
+      <c r="M89" s="91"/>
+      <c r="N89" s="91"/>
+      <c r="O89" s="91"/>
+      <c r="P89" s="91"/>
+      <c r="Q89" s="91"/>
+      <c r="R89" s="91"/>
+      <c r="S89" s="91"/>
+      <c r="T89" s="91"/>
+      <c r="U89" s="91"/>
+      <c r="V89" s="91"/>
+      <c r="W89" s="91"/>
+      <c r="X89" s="91"/>
+      <c r="Y89" s="91"/>
+      <c r="Z89" s="91"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="92"/>
-      <c r="G90" s="5"/>
+      <c r="A90" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="B90" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="D90" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E90" s="94"/>
+      <c r="F90" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="G90" s="90"/>
+      <c r="H90" s="91"/>
+      <c r="I90" s="91"/>
+      <c r="J90" s="91"/>
+      <c r="K90" s="91"/>
+      <c r="L90" s="91"/>
+      <c r="M90" s="91"/>
+      <c r="N90" s="91"/>
+      <c r="O90" s="91"/>
+      <c r="P90" s="91"/>
+      <c r="Q90" s="91"/>
+      <c r="R90" s="91"/>
+      <c r="S90" s="91"/>
+      <c r="T90" s="91"/>
+      <c r="U90" s="91"/>
+      <c r="V90" s="91"/>
+      <c r="W90" s="91"/>
+      <c r="X90" s="91"/>
+      <c r="Y90" s="91"/>
+      <c r="Z90" s="91"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
+      <c r="A91" s="4"/>
       <c r="G91" s="5"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
+      <c r="A92" s="95"/>
       <c r="G92" s="5"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
@@ -8703,6 +8821,12 @@
     </row>
     <row r="997" ht="15.75" customHeight="1">
       <c r="G997" s="5"/>
+    </row>
+    <row r="998" ht="15.75" customHeight="1">
+      <c r="G998" s="5"/>
+    </row>
+    <row r="999" ht="15.75" customHeight="1">
+      <c r="G999" s="5"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>

<commit_message>
State 6 Implementation v3.0.2 - navigation - Base View Abstraction
State 6 Implementation v3.0.2 - navigation - Base View Abstraction
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="pgWysHQ5Yo9Prt6sSqAqWa/b/LCqrBERFY36Uj/DZCU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="9RE5WWv/1Z/enEj8mWwpWuwrwng687r8dWKhSScwD+w="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="250">
   <si>
     <t>Waterfall Methodology</t>
   </si>
@@ -1694,7 +1694,24 @@
         <color rgb="FF156082"/>
         <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve"> •        Navigation and AppStatus</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <color rgb="FF156082"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">•	</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <b/>
+        <color rgb="FF156082"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Navigation and AppStatus</t>
     </r>
   </si>
   <si>
@@ -1723,6 +1740,48 @@
   </si>
   <si>
     <t>we had to adapt and change a lot the previous navigation controller</t>
+  </si>
+  <si>
+    <t>Create a BaseView that all Views will inherit for the communs utilities of views</t>
+  </si>
+  <si>
+    <t>BaseView Implemented and all view inherits from it</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Quattrocento Sans"/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Documentation according to client review and features implemented </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <b/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>to now:  AppStatus State Machinel, UML View Class Model</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Segoe UI"/>
+        <b/>
+        <color theme="4"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Sketch-View </t>
+    </r>
   </si>
   <si>
     <t>Implement the database</t>
@@ -2691,9 +2750,6 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="15" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -2716,6 +2772,9 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -4879,9 +4938,7 @@
       <c r="E51" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="F51" s="44" t="s">
-        <v>153</v>
-      </c>
+      <c r="F51" s="44"/>
       <c r="G51" s="74" t="s">
         <v>165</v>
       </c>
@@ -4906,135 +4963,141 @@
       <c r="Z51" s="18"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="76" t="s">
+      <c r="A52" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="F52" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G52" s="64"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="42"/>
+      <c r="J52" s="42"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
+      <c r="M52" s="42"/>
+      <c r="N52" s="42"/>
+      <c r="O52" s="42"/>
+      <c r="P52" s="42"/>
+      <c r="Q52" s="42"/>
+      <c r="R52" s="42"/>
+      <c r="S52" s="42"/>
+      <c r="T52" s="42"/>
+      <c r="U52" s="42"/>
+      <c r="V52" s="42"/>
+      <c r="W52" s="42"/>
+      <c r="X52" s="42"/>
+      <c r="Y52" s="42"/>
+      <c r="Z52" s="42"/>
+    </row>
+    <row r="53" ht="51.75" customHeight="1">
+      <c r="A53" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F53" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G53" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="18"/>
+      <c r="U53" s="18"/>
+      <c r="V53" s="18"/>
+      <c r="W53" s="18"/>
+      <c r="X53" s="18"/>
+      <c r="Y53" s="18"/>
+      <c r="Z53" s="18"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="76" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="76" t="s">
-        <v>166</v>
-      </c>
-      <c r="C52" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="D52" s="76" t="s">
+      <c r="B54" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C54" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="77"/>
-      <c r="F52" s="78" t="s">
+      <c r="E54" s="77"/>
+      <c r="F54" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="G52" s="79"/>
-      <c r="H52" s="80"/>
-      <c r="I52" s="80"/>
-      <c r="J52" s="80"/>
-      <c r="K52" s="80"/>
-      <c r="L52" s="80"/>
-      <c r="M52" s="80"/>
-      <c r="N52" s="80"/>
-      <c r="O52" s="80"/>
-      <c r="P52" s="80"/>
-      <c r="Q52" s="80"/>
-      <c r="R52" s="80"/>
-      <c r="S52" s="80"/>
-      <c r="T52" s="80"/>
-      <c r="U52" s="80"/>
-      <c r="V52" s="80"/>
-      <c r="W52" s="80"/>
-      <c r="X52" s="80"/>
-      <c r="Y52" s="80"/>
-      <c r="Z52" s="80"/>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="81"/>
-      <c r="F53" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G53" s="82"/>
-      <c r="H53" s="83"/>
-      <c r="I53" s="83"/>
-      <c r="J53" s="83"/>
-      <c r="K53" s="83"/>
-      <c r="L53" s="83"/>
-      <c r="M53" s="83"/>
-      <c r="N53" s="83"/>
-      <c r="O53" s="83"/>
-      <c r="P53" s="83"/>
-      <c r="Q53" s="83"/>
-      <c r="R53" s="83"/>
-      <c r="S53" s="83"/>
-      <c r="T53" s="83"/>
-      <c r="U53" s="83"/>
-      <c r="V53" s="83"/>
-      <c r="W53" s="83"/>
-      <c r="X53" s="83"/>
-      <c r="Y53" s="83"/>
-      <c r="Z53" s="83"/>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E54" s="81"/>
-      <c r="F54" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="G54" s="82"/>
-      <c r="H54" s="83"/>
-      <c r="I54" s="83"/>
-      <c r="J54" s="83"/>
-      <c r="K54" s="83"/>
-      <c r="L54" s="83"/>
-      <c r="M54" s="83"/>
-      <c r="N54" s="83"/>
-      <c r="O54" s="83"/>
-      <c r="P54" s="83"/>
-      <c r="Q54" s="83"/>
-      <c r="R54" s="83"/>
-      <c r="S54" s="83"/>
-      <c r="T54" s="83"/>
-      <c r="U54" s="83"/>
-      <c r="V54" s="83"/>
-      <c r="W54" s="83"/>
-      <c r="X54" s="83"/>
-      <c r="Y54" s="83"/>
-      <c r="Z54" s="83"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="80"/>
+      <c r="J54" s="80"/>
+      <c r="K54" s="80"/>
+      <c r="L54" s="80"/>
+      <c r="M54" s="80"/>
+      <c r="N54" s="80"/>
+      <c r="O54" s="80"/>
+      <c r="P54" s="80"/>
+      <c r="Q54" s="80"/>
+      <c r="R54" s="80"/>
+      <c r="S54" s="80"/>
+      <c r="T54" s="80"/>
+      <c r="U54" s="80"/>
+      <c r="V54" s="80"/>
+      <c r="W54" s="80"/>
+      <c r="X54" s="80"/>
+      <c r="Y54" s="80"/>
+      <c r="Z54" s="80"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="25" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E55" s="81"/>
       <c r="F55" s="28" t="s">
-        <v>179</v>
+        <v>107</v>
       </c>
       <c r="G55" s="82"/>
       <c r="H55" s="83"/>
@@ -5058,69 +5121,135 @@
       <c r="Z55" s="83"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="81"/>
+      <c r="F56" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="G56" s="82"/>
+      <c r="H56" s="83"/>
+      <c r="I56" s="83"/>
+      <c r="J56" s="83"/>
+      <c r="K56" s="83"/>
+      <c r="L56" s="83"/>
+      <c r="M56" s="83"/>
+      <c r="N56" s="83"/>
+      <c r="O56" s="83"/>
+      <c r="P56" s="83"/>
+      <c r="Q56" s="83"/>
+      <c r="R56" s="83"/>
+      <c r="S56" s="83"/>
+      <c r="T56" s="83"/>
+      <c r="U56" s="83"/>
+      <c r="V56" s="83"/>
+      <c r="W56" s="83"/>
+      <c r="X56" s="83"/>
+      <c r="Y56" s="83"/>
+      <c r="Z56" s="83"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B57" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="C57" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="D57" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="81"/>
+      <c r="F57" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="G57" s="82"/>
+      <c r="H57" s="83"/>
+      <c r="I57" s="83"/>
+      <c r="J57" s="83"/>
+      <c r="K57" s="83"/>
+      <c r="L57" s="83"/>
+      <c r="M57" s="83"/>
+      <c r="N57" s="83"/>
+      <c r="O57" s="83"/>
+      <c r="P57" s="83"/>
+      <c r="Q57" s="83"/>
+      <c r="R57" s="83"/>
+      <c r="S57" s="83"/>
+      <c r="T57" s="83"/>
+      <c r="U57" s="83"/>
+      <c r="V57" s="83"/>
+      <c r="W57" s="83"/>
+      <c r="X57" s="83"/>
+      <c r="Y57" s="83"/>
+      <c r="Z57" s="83"/>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="84"/>
-      <c r="F56" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="G56" s="85"/>
-      <c r="H56" s="86"/>
-      <c r="I56" s="86"/>
-      <c r="J56" s="86"/>
-      <c r="K56" s="86"/>
-      <c r="L56" s="86"/>
-      <c r="M56" s="86"/>
-      <c r="N56" s="86"/>
-      <c r="O56" s="86"/>
-      <c r="P56" s="86"/>
-      <c r="Q56" s="86"/>
-      <c r="R56" s="86"/>
-      <c r="S56" s="86"/>
-      <c r="T56" s="86"/>
-      <c r="U56" s="86"/>
-      <c r="V56" s="86"/>
-      <c r="W56" s="86"/>
-      <c r="X56" s="86"/>
-      <c r="Y56" s="86"/>
-      <c r="Z56" s="86"/>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="87"/>
-      <c r="B57" s="87"/>
-      <c r="C57" s="87"/>
-      <c r="D57" s="87"/>
-      <c r="E57" s="88"/>
-      <c r="F57" s="89"/>
-      <c r="G57" s="5"/>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="87"/>
-      <c r="B58" s="87"/>
-      <c r="C58" s="87"/>
-      <c r="D58" s="87"/>
-      <c r="E58" s="88"/>
-      <c r="F58" s="89"/>
-      <c r="G58" s="5"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G58" s="84"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
+      <c r="L58" s="85"/>
+      <c r="M58" s="85"/>
+      <c r="N58" s="85"/>
+      <c r="O58" s="85"/>
+      <c r="P58" s="85"/>
+      <c r="Q58" s="85"/>
+      <c r="R58" s="85"/>
+      <c r="S58" s="85"/>
+      <c r="T58" s="85"/>
+      <c r="U58" s="85"/>
+      <c r="V58" s="85"/>
+      <c r="W58" s="85"/>
+      <c r="X58" s="85"/>
+      <c r="Y58" s="85"/>
+      <c r="Z58" s="85"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="4"/>
+      <c r="A59" s="86"/>
+      <c r="B59" s="86"/>
+      <c r="C59" s="86"/>
+      <c r="D59" s="86"/>
+      <c r="E59" s="87"/>
+      <c r="F59" s="88"/>
       <c r="G59" s="5"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="1" t="s">
-        <v>183</v>
-      </c>
+      <c r="A60" s="86"/>
+      <c r="B60" s="86"/>
+      <c r="C60" s="86"/>
+      <c r="D60" s="86"/>
+      <c r="E60" s="87"/>
+      <c r="F60" s="88"/>
       <c r="G60" s="5"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
@@ -5128,989 +5257,993 @@
       <c r="G61" s="5"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="4"/>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B64" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D62" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F62" s="7" t="s">
+      <c r="D64" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F64" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G62" s="5"/>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="B63" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="D63" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E63" s="45"/>
-      <c r="F63" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="90"/>
-      <c r="H63" s="91"/>
-      <c r="I63" s="91"/>
-      <c r="J63" s="91"/>
-      <c r="K63" s="91"/>
-      <c r="L63" s="91"/>
-      <c r="M63" s="91"/>
-      <c r="N63" s="91"/>
-      <c r="O63" s="91"/>
-      <c r="P63" s="91"/>
-      <c r="Q63" s="91"/>
-      <c r="R63" s="91"/>
-      <c r="S63" s="91"/>
-      <c r="T63" s="91"/>
-      <c r="U63" s="91"/>
-      <c r="V63" s="91"/>
-      <c r="W63" s="91"/>
-      <c r="X63" s="91"/>
-      <c r="Y63" s="91"/>
-      <c r="Z63" s="91"/>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="B64" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="C64" s="92" t="s">
-        <v>191</v>
-      </c>
-      <c r="D64" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E64" s="45"/>
-      <c r="F64" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="G64" s="90"/>
-      <c r="H64" s="91"/>
-      <c r="I64" s="91"/>
-      <c r="J64" s="91"/>
-      <c r="K64" s="91"/>
-      <c r="L64" s="91"/>
-      <c r="M64" s="91"/>
-      <c r="N64" s="91"/>
-      <c r="O64" s="91"/>
-      <c r="P64" s="91"/>
-      <c r="Q64" s="91"/>
-      <c r="R64" s="91"/>
-      <c r="S64" s="91"/>
-      <c r="T64" s="91"/>
-      <c r="U64" s="91"/>
-      <c r="V64" s="91"/>
-      <c r="W64" s="91"/>
-      <c r="X64" s="91"/>
-      <c r="Y64" s="91"/>
-      <c r="Z64" s="91"/>
+      <c r="G64" s="5"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="45" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B65" s="45" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D65" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E65" s="45"/>
       <c r="F65" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="G65" s="90"/>
-      <c r="H65" s="91"/>
-      <c r="I65" s="91"/>
-      <c r="J65" s="91"/>
-      <c r="K65" s="91"/>
-      <c r="L65" s="91"/>
-      <c r="M65" s="91"/>
-      <c r="N65" s="91"/>
-      <c r="O65" s="91"/>
-      <c r="P65" s="91"/>
-      <c r="Q65" s="91"/>
-      <c r="R65" s="91"/>
-      <c r="S65" s="91"/>
-      <c r="T65" s="91"/>
-      <c r="U65" s="91"/>
-      <c r="V65" s="91"/>
-      <c r="W65" s="91"/>
-      <c r="X65" s="91"/>
-      <c r="Y65" s="91"/>
-      <c r="Z65" s="91"/>
+        <v>13</v>
+      </c>
+      <c r="G65" s="89"/>
+      <c r="H65" s="90"/>
+      <c r="I65" s="90"/>
+      <c r="J65" s="90"/>
+      <c r="K65" s="90"/>
+      <c r="L65" s="90"/>
+      <c r="M65" s="90"/>
+      <c r="N65" s="90"/>
+      <c r="O65" s="90"/>
+      <c r="P65" s="90"/>
+      <c r="Q65" s="90"/>
+      <c r="R65" s="90"/>
+      <c r="S65" s="90"/>
+      <c r="T65" s="90"/>
+      <c r="U65" s="90"/>
+      <c r="V65" s="90"/>
+      <c r="W65" s="90"/>
+      <c r="X65" s="90"/>
+      <c r="Y65" s="90"/>
+      <c r="Z65" s="90"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="45" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B66" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="C66" s="92" t="s">
-        <v>199</v>
+        <v>193</v>
+      </c>
+      <c r="C66" s="91" t="s">
+        <v>194</v>
       </c>
       <c r="D66" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E66" s="45"/>
       <c r="F66" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="G66" s="90"/>
-      <c r="H66" s="91"/>
-      <c r="I66" s="91"/>
-      <c r="J66" s="91"/>
-      <c r="K66" s="91"/>
-      <c r="L66" s="91"/>
-      <c r="M66" s="91"/>
-      <c r="N66" s="91"/>
-      <c r="O66" s="91"/>
-      <c r="P66" s="91"/>
-      <c r="Q66" s="91"/>
-      <c r="R66" s="91"/>
-      <c r="S66" s="91"/>
-      <c r="T66" s="91"/>
-      <c r="U66" s="91"/>
-      <c r="V66" s="91"/>
-      <c r="W66" s="91"/>
-      <c r="X66" s="91"/>
-      <c r="Y66" s="91"/>
-      <c r="Z66" s="91"/>
+        <v>195</v>
+      </c>
+      <c r="G66" s="89"/>
+      <c r="H66" s="90"/>
+      <c r="I66" s="90"/>
+      <c r="J66" s="90"/>
+      <c r="K66" s="90"/>
+      <c r="L66" s="90"/>
+      <c r="M66" s="90"/>
+      <c r="N66" s="90"/>
+      <c r="O66" s="90"/>
+      <c r="P66" s="90"/>
+      <c r="Q66" s="90"/>
+      <c r="R66" s="90"/>
+      <c r="S66" s="90"/>
+      <c r="T66" s="90"/>
+      <c r="U66" s="90"/>
+      <c r="V66" s="90"/>
+      <c r="W66" s="90"/>
+      <c r="X66" s="90"/>
+      <c r="Y66" s="90"/>
+      <c r="Z66" s="90"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="45" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B67" s="45" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D67" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E67" s="45"/>
       <c r="F67" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="G67" s="90"/>
-      <c r="H67" s="91"/>
-      <c r="I67" s="91"/>
-      <c r="J67" s="91"/>
-      <c r="K67" s="91"/>
-      <c r="L67" s="91"/>
-      <c r="M67" s="91"/>
-      <c r="N67" s="91"/>
-      <c r="O67" s="91"/>
-      <c r="P67" s="91"/>
-      <c r="Q67" s="91"/>
-      <c r="R67" s="91"/>
-      <c r="S67" s="91"/>
-      <c r="T67" s="91"/>
-      <c r="U67" s="91"/>
-      <c r="V67" s="91"/>
-      <c r="W67" s="91"/>
-      <c r="X67" s="91"/>
-      <c r="Y67" s="91"/>
-      <c r="Z67" s="91"/>
+        <v>199</v>
+      </c>
+      <c r="G67" s="89"/>
+      <c r="H67" s="90"/>
+      <c r="I67" s="90"/>
+      <c r="J67" s="90"/>
+      <c r="K67" s="90"/>
+      <c r="L67" s="90"/>
+      <c r="M67" s="90"/>
+      <c r="N67" s="90"/>
+      <c r="O67" s="90"/>
+      <c r="P67" s="90"/>
+      <c r="Q67" s="90"/>
+      <c r="R67" s="90"/>
+      <c r="S67" s="90"/>
+      <c r="T67" s="90"/>
+      <c r="U67" s="90"/>
+      <c r="V67" s="90"/>
+      <c r="W67" s="90"/>
+      <c r="X67" s="90"/>
+      <c r="Y67" s="90"/>
+      <c r="Z67" s="90"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="C68" s="91" t="s">
         <v>202</v>
-      </c>
-      <c r="B68" s="45" t="s">
-        <v>203</v>
-      </c>
-      <c r="C68" s="92" t="s">
-        <v>204</v>
       </c>
       <c r="D68" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E68" s="45"/>
       <c r="F68" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="G68" s="90"/>
-      <c r="H68" s="91"/>
-      <c r="I68" s="91"/>
-      <c r="J68" s="91"/>
-      <c r="K68" s="91"/>
-      <c r="L68" s="91"/>
-      <c r="M68" s="91"/>
-      <c r="N68" s="91"/>
-      <c r="O68" s="91"/>
-      <c r="P68" s="91"/>
-      <c r="Q68" s="91"/>
-      <c r="R68" s="91"/>
-      <c r="S68" s="91"/>
-      <c r="T68" s="91"/>
-      <c r="U68" s="91"/>
-      <c r="V68" s="91"/>
-      <c r="W68" s="91"/>
-      <c r="X68" s="91"/>
-      <c r="Y68" s="91"/>
-      <c r="Z68" s="91"/>
+        <v>195</v>
+      </c>
+      <c r="G68" s="89"/>
+      <c r="H68" s="90"/>
+      <c r="I68" s="90"/>
+      <c r="J68" s="90"/>
+      <c r="K68" s="90"/>
+      <c r="L68" s="90"/>
+      <c r="M68" s="90"/>
+      <c r="N68" s="90"/>
+      <c r="O68" s="90"/>
+      <c r="P68" s="90"/>
+      <c r="Q68" s="90"/>
+      <c r="R68" s="90"/>
+      <c r="S68" s="90"/>
+      <c r="T68" s="90"/>
+      <c r="U68" s="90"/>
+      <c r="V68" s="90"/>
+      <c r="W68" s="90"/>
+      <c r="X68" s="90"/>
+      <c r="Y68" s="90"/>
+      <c r="Z68" s="90"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="45" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B69" s="45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D69" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E69" s="45"/>
       <c r="F69" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G69" s="90"/>
-      <c r="H69" s="91"/>
-      <c r="I69" s="91"/>
-      <c r="J69" s="91"/>
-      <c r="K69" s="91"/>
-      <c r="L69" s="91"/>
-      <c r="M69" s="91"/>
-      <c r="N69" s="91"/>
-      <c r="O69" s="91"/>
-      <c r="P69" s="91"/>
-      <c r="Q69" s="91"/>
-      <c r="R69" s="91"/>
-      <c r="S69" s="91"/>
-      <c r="T69" s="91"/>
-      <c r="U69" s="91"/>
-      <c r="V69" s="91"/>
-      <c r="W69" s="91"/>
-      <c r="X69" s="91"/>
-      <c r="Y69" s="91"/>
-      <c r="Z69" s="91"/>
+        <v>199</v>
+      </c>
+      <c r="G69" s="89"/>
+      <c r="H69" s="90"/>
+      <c r="I69" s="90"/>
+      <c r="J69" s="90"/>
+      <c r="K69" s="90"/>
+      <c r="L69" s="90"/>
+      <c r="M69" s="90"/>
+      <c r="N69" s="90"/>
+      <c r="O69" s="90"/>
+      <c r="P69" s="90"/>
+      <c r="Q69" s="90"/>
+      <c r="R69" s="90"/>
+      <c r="S69" s="90"/>
+      <c r="T69" s="90"/>
+      <c r="U69" s="90"/>
+      <c r="V69" s="90"/>
+      <c r="W69" s="90"/>
+      <c r="X69" s="90"/>
+      <c r="Y69" s="90"/>
+      <c r="Z69" s="90"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="C70" s="91" t="s">
         <v>207</v>
-      </c>
-      <c r="B70" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="C70" s="93" t="s">
-        <v>209</v>
       </c>
       <c r="D70" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E70" s="45"/>
       <c r="F70" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="G70" s="90"/>
-      <c r="H70" s="91"/>
-      <c r="I70" s="91"/>
-      <c r="J70" s="91"/>
-      <c r="K70" s="91"/>
-      <c r="L70" s="91"/>
-      <c r="M70" s="91"/>
-      <c r="N70" s="91"/>
-      <c r="O70" s="91"/>
-      <c r="P70" s="91"/>
-      <c r="Q70" s="91"/>
-      <c r="R70" s="91"/>
-      <c r="S70" s="91"/>
-      <c r="T70" s="91"/>
-      <c r="U70" s="91"/>
-      <c r="V70" s="91"/>
-      <c r="W70" s="91"/>
-      <c r="X70" s="91"/>
-      <c r="Y70" s="91"/>
-      <c r="Z70" s="91"/>
+        <v>195</v>
+      </c>
+      <c r="G70" s="89"/>
+      <c r="H70" s="90"/>
+      <c r="I70" s="90"/>
+      <c r="J70" s="90"/>
+      <c r="K70" s="90"/>
+      <c r="L70" s="90"/>
+      <c r="M70" s="90"/>
+      <c r="N70" s="90"/>
+      <c r="O70" s="90"/>
+      <c r="P70" s="90"/>
+      <c r="Q70" s="90"/>
+      <c r="R70" s="90"/>
+      <c r="S70" s="90"/>
+      <c r="T70" s="90"/>
+      <c r="U70" s="90"/>
+      <c r="V70" s="90"/>
+      <c r="W70" s="90"/>
+      <c r="X70" s="90"/>
+      <c r="Y70" s="90"/>
+      <c r="Z70" s="90"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="45" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C71" s="45" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D71" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E71" s="45"/>
       <c r="F71" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G71" s="90"/>
-      <c r="H71" s="91"/>
-      <c r="I71" s="91"/>
-      <c r="J71" s="91"/>
-      <c r="K71" s="91"/>
-      <c r="L71" s="91"/>
-      <c r="M71" s="91"/>
-      <c r="N71" s="91"/>
-      <c r="O71" s="91"/>
-      <c r="P71" s="91"/>
-      <c r="Q71" s="91"/>
-      <c r="R71" s="91"/>
-      <c r="S71" s="91"/>
-      <c r="T71" s="91"/>
-      <c r="U71" s="91"/>
-      <c r="V71" s="91"/>
-      <c r="W71" s="91"/>
-      <c r="X71" s="91"/>
-      <c r="Y71" s="91"/>
-      <c r="Z71" s="91"/>
+        <v>178</v>
+      </c>
+      <c r="G71" s="89"/>
+      <c r="H71" s="90"/>
+      <c r="I71" s="90"/>
+      <c r="J71" s="90"/>
+      <c r="K71" s="90"/>
+      <c r="L71" s="90"/>
+      <c r="M71" s="90"/>
+      <c r="N71" s="90"/>
+      <c r="O71" s="90"/>
+      <c r="P71" s="90"/>
+      <c r="Q71" s="90"/>
+      <c r="R71" s="90"/>
+      <c r="S71" s="90"/>
+      <c r="T71" s="90"/>
+      <c r="U71" s="90"/>
+      <c r="V71" s="90"/>
+      <c r="W71" s="90"/>
+      <c r="X71" s="90"/>
+      <c r="Y71" s="90"/>
+      <c r="Z71" s="90"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="B72" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="B72" s="45" t="s">
+      <c r="C72" s="92" t="s">
         <v>212</v>
-      </c>
-      <c r="C72" s="93" t="s">
-        <v>213</v>
       </c>
       <c r="D72" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E72" s="45"/>
       <c r="F72" s="44" t="s">
-        <v>214</v>
-      </c>
-      <c r="G72" s="90"/>
-      <c r="H72" s="91"/>
-      <c r="I72" s="91"/>
-      <c r="J72" s="91"/>
-      <c r="K72" s="91"/>
-      <c r="L72" s="91"/>
-      <c r="M72" s="91"/>
-      <c r="N72" s="91"/>
-      <c r="O72" s="91"/>
-      <c r="P72" s="91"/>
-      <c r="Q72" s="91"/>
-      <c r="R72" s="91"/>
-      <c r="S72" s="91"/>
-      <c r="T72" s="91"/>
-      <c r="U72" s="91"/>
-      <c r="V72" s="91"/>
-      <c r="W72" s="91"/>
-      <c r="X72" s="91"/>
-      <c r="Y72" s="91"/>
-      <c r="Z72" s="91"/>
+        <v>195</v>
+      </c>
+      <c r="G72" s="89"/>
+      <c r="H72" s="90"/>
+      <c r="I72" s="90"/>
+      <c r="J72" s="90"/>
+      <c r="K72" s="90"/>
+      <c r="L72" s="90"/>
+      <c r="M72" s="90"/>
+      <c r="N72" s="90"/>
+      <c r="O72" s="90"/>
+      <c r="P72" s="90"/>
+      <c r="Q72" s="90"/>
+      <c r="R72" s="90"/>
+      <c r="S72" s="90"/>
+      <c r="T72" s="90"/>
+      <c r="U72" s="90"/>
+      <c r="V72" s="90"/>
+      <c r="W72" s="90"/>
+      <c r="X72" s="90"/>
+      <c r="Y72" s="90"/>
+      <c r="Z72" s="90"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="45" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="B73" s="45" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="D73" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E73" s="45"/>
       <c r="F73" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="G73" s="90"/>
-      <c r="H73" s="91"/>
-      <c r="I73" s="91"/>
-      <c r="J73" s="91"/>
-      <c r="K73" s="91"/>
-      <c r="L73" s="91"/>
-      <c r="M73" s="91"/>
-      <c r="N73" s="91"/>
-      <c r="O73" s="91"/>
-      <c r="P73" s="91"/>
-      <c r="Q73" s="91"/>
-      <c r="R73" s="91"/>
-      <c r="S73" s="91"/>
-      <c r="T73" s="91"/>
-      <c r="U73" s="91"/>
-      <c r="V73" s="91"/>
-      <c r="W73" s="91"/>
-      <c r="X73" s="91"/>
-      <c r="Y73" s="91"/>
-      <c r="Z73" s="91"/>
+        <v>178</v>
+      </c>
+      <c r="G73" s="89"/>
+      <c r="H73" s="90"/>
+      <c r="I73" s="90"/>
+      <c r="J73" s="90"/>
+      <c r="K73" s="90"/>
+      <c r="L73" s="90"/>
+      <c r="M73" s="90"/>
+      <c r="N73" s="90"/>
+      <c r="O73" s="90"/>
+      <c r="P73" s="90"/>
+      <c r="Q73" s="90"/>
+      <c r="R73" s="90"/>
+      <c r="S73" s="90"/>
+      <c r="T73" s="90"/>
+      <c r="U73" s="90"/>
+      <c r="V73" s="90"/>
+      <c r="W73" s="90"/>
+      <c r="X73" s="90"/>
+      <c r="Y73" s="90"/>
+      <c r="Z73" s="90"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="45" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="B74" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="C74" s="45" t="s">
-        <v>182</v>
+        <v>215</v>
+      </c>
+      <c r="C74" s="92" t="s">
+        <v>216</v>
       </c>
       <c r="D74" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E74" s="45"/>
       <c r="F74" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="G74" s="89"/>
+      <c r="H74" s="90"/>
+      <c r="I74" s="90"/>
+      <c r="J74" s="90"/>
+      <c r="K74" s="90"/>
+      <c r="L74" s="90"/>
+      <c r="M74" s="90"/>
+      <c r="N74" s="90"/>
+      <c r="O74" s="90"/>
+      <c r="P74" s="90"/>
+      <c r="Q74" s="90"/>
+      <c r="R74" s="90"/>
+      <c r="S74" s="90"/>
+      <c r="T74" s="90"/>
+      <c r="U74" s="90"/>
+      <c r="V74" s="90"/>
+      <c r="W74" s="90"/>
+      <c r="X74" s="90"/>
+      <c r="Y74" s="90"/>
+      <c r="Z74" s="90"/>
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="A75" s="45" t="s">
         <v>179</v>
       </c>
-      <c r="G74" s="90"/>
-      <c r="H74" s="91"/>
-      <c r="I74" s="91"/>
-      <c r="J74" s="91"/>
-      <c r="K74" s="91"/>
-      <c r="L74" s="91"/>
-      <c r="M74" s="91"/>
-      <c r="N74" s="91"/>
-      <c r="O74" s="91"/>
-      <c r="P74" s="91"/>
-      <c r="Q74" s="91"/>
-      <c r="R74" s="91"/>
-      <c r="S74" s="91"/>
-      <c r="T74" s="91"/>
-      <c r="U74" s="91"/>
-      <c r="V74" s="91"/>
-      <c r="W74" s="91"/>
-      <c r="X74" s="91"/>
-      <c r="Y74" s="91"/>
-      <c r="Z74" s="91"/>
-    </row>
-    <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="4"/>
-      <c r="G75" s="5"/>
+      <c r="B75" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="D75" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E75" s="45"/>
+      <c r="F75" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G75" s="89"/>
+      <c r="H75" s="90"/>
+      <c r="I75" s="90"/>
+      <c r="J75" s="90"/>
+      <c r="K75" s="90"/>
+      <c r="L75" s="90"/>
+      <c r="M75" s="90"/>
+      <c r="N75" s="90"/>
+      <c r="O75" s="90"/>
+      <c r="P75" s="90"/>
+      <c r="Q75" s="90"/>
+      <c r="R75" s="90"/>
+      <c r="S75" s="90"/>
+      <c r="T75" s="90"/>
+      <c r="U75" s="90"/>
+      <c r="V75" s="90"/>
+      <c r="W75" s="90"/>
+      <c r="X75" s="90"/>
+      <c r="Y75" s="90"/>
+      <c r="Z75" s="90"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G76" s="5"/>
+      <c r="A76" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B76" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C76" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="D76" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E76" s="45"/>
+      <c r="F76" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G76" s="89"/>
+      <c r="H76" s="90"/>
+      <c r="I76" s="90"/>
+      <c r="J76" s="90"/>
+      <c r="K76" s="90"/>
+      <c r="L76" s="90"/>
+      <c r="M76" s="90"/>
+      <c r="N76" s="90"/>
+      <c r="O76" s="90"/>
+      <c r="P76" s="90"/>
+      <c r="Q76" s="90"/>
+      <c r="R76" s="90"/>
+      <c r="S76" s="90"/>
+      <c r="T76" s="90"/>
+      <c r="U76" s="90"/>
+      <c r="V76" s="90"/>
+      <c r="W76" s="90"/>
+      <c r="X76" s="90"/>
+      <c r="Y76" s="90"/>
+      <c r="Z76" s="90"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="4"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G78" s="5"/>
+    </row>
+    <row r="79" ht="15.75" customHeight="1">
+      <c r="A79" s="4"/>
+      <c r="G79" s="5"/>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B80" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C80" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F78" s="7" t="s">
+      <c r="D80" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G78" s="5"/>
-    </row>
-    <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="B79" s="45" t="s">
-        <v>217</v>
-      </c>
-      <c r="C79" s="92" t="s">
-        <v>218</v>
-      </c>
-      <c r="D79" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E79" s="45"/>
-      <c r="F79" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G79" s="90"/>
-      <c r="H79" s="91"/>
-      <c r="I79" s="91"/>
-      <c r="J79" s="91"/>
-      <c r="K79" s="91"/>
-      <c r="L79" s="91"/>
-      <c r="M79" s="91"/>
-      <c r="N79" s="91"/>
-      <c r="O79" s="91"/>
-      <c r="P79" s="91"/>
-      <c r="Q79" s="91"/>
-      <c r="R79" s="91"/>
-      <c r="S79" s="91"/>
-      <c r="T79" s="91"/>
-      <c r="U79" s="91"/>
-      <c r="V79" s="91"/>
-      <c r="W79" s="91"/>
-      <c r="X79" s="91"/>
-      <c r="Y79" s="91"/>
-      <c r="Z79" s="91"/>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="B80" s="45" t="s">
-        <v>220</v>
-      </c>
-      <c r="C80" s="92" t="s">
-        <v>221</v>
-      </c>
-      <c r="D80" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="45"/>
-      <c r="F80" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G80" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="H80" s="91"/>
-      <c r="I80" s="91"/>
-      <c r="J80" s="91"/>
-      <c r="K80" s="91"/>
-      <c r="L80" s="91"/>
-      <c r="M80" s="91"/>
-      <c r="N80" s="91"/>
-      <c r="O80" s="91"/>
-      <c r="P80" s="91"/>
-      <c r="Q80" s="91"/>
-      <c r="R80" s="91"/>
-      <c r="S80" s="91"/>
-      <c r="T80" s="91"/>
-      <c r="U80" s="91"/>
-      <c r="V80" s="91"/>
-      <c r="W80" s="91"/>
-      <c r="X80" s="91"/>
-      <c r="Y80" s="91"/>
-      <c r="Z80" s="91"/>
+      <c r="G80" s="5"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="45" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B81" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C81" s="92" t="s">
-        <v>224</v>
+        <v>220</v>
+      </c>
+      <c r="C81" s="91" t="s">
+        <v>221</v>
       </c>
       <c r="D81" s="45" t="s">
-        <v>225</v>
-      </c>
-      <c r="E81" s="45"/>
+        <v>16</v>
+      </c>
+      <c r="E81" s="93"/>
       <c r="F81" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="G81" s="45" t="s">
-        <v>227</v>
-      </c>
-      <c r="H81" s="91"/>
-      <c r="I81" s="91"/>
-      <c r="J81" s="91"/>
-      <c r="K81" s="91"/>
-      <c r="L81" s="91"/>
-      <c r="M81" s="91"/>
-      <c r="N81" s="91"/>
-      <c r="O81" s="91"/>
-      <c r="P81" s="91"/>
-      <c r="Q81" s="91"/>
-      <c r="R81" s="91"/>
-      <c r="S81" s="91"/>
-      <c r="T81" s="91"/>
-      <c r="U81" s="91"/>
-      <c r="V81" s="91"/>
-      <c r="W81" s="91"/>
-      <c r="X81" s="91"/>
-      <c r="Y81" s="91"/>
-      <c r="Z81" s="91"/>
+        <v>13</v>
+      </c>
+      <c r="G81" s="89"/>
+      <c r="H81" s="90"/>
+      <c r="I81" s="90"/>
+      <c r="J81" s="90"/>
+      <c r="K81" s="90"/>
+      <c r="L81" s="90"/>
+      <c r="M81" s="90"/>
+      <c r="N81" s="90"/>
+      <c r="O81" s="90"/>
+      <c r="P81" s="90"/>
+      <c r="Q81" s="90"/>
+      <c r="R81" s="90"/>
+      <c r="S81" s="90"/>
+      <c r="T81" s="90"/>
+      <c r="U81" s="90"/>
+      <c r="V81" s="90"/>
+      <c r="W81" s="90"/>
+      <c r="X81" s="90"/>
+      <c r="Y81" s="90"/>
+      <c r="Z81" s="90"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="45" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B82" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="C82" s="45" t="s">
-        <v>229</v>
+        <v>223</v>
+      </c>
+      <c r="C82" s="91" t="s">
+        <v>224</v>
       </c>
       <c r="D82" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E82" s="94"/>
+        <v>11</v>
+      </c>
+      <c r="E82" s="45"/>
       <c r="F82" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G82" s="90"/>
-      <c r="H82" s="91"/>
-      <c r="I82" s="91"/>
-      <c r="J82" s="91"/>
-      <c r="K82" s="91"/>
-      <c r="L82" s="91"/>
-      <c r="M82" s="91"/>
-      <c r="N82" s="91"/>
-      <c r="O82" s="91"/>
-      <c r="P82" s="91"/>
-      <c r="Q82" s="91"/>
-      <c r="R82" s="91"/>
-      <c r="S82" s="91"/>
-      <c r="T82" s="91"/>
-      <c r="U82" s="91"/>
-      <c r="V82" s="91"/>
-      <c r="W82" s="91"/>
-      <c r="X82" s="91"/>
-      <c r="Y82" s="91"/>
-      <c r="Z82" s="91"/>
+        <v>13</v>
+      </c>
+      <c r="G82" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="H82" s="90"/>
+      <c r="I82" s="90"/>
+      <c r="J82" s="90"/>
+      <c r="K82" s="90"/>
+      <c r="L82" s="90"/>
+      <c r="M82" s="90"/>
+      <c r="N82" s="90"/>
+      <c r="O82" s="90"/>
+      <c r="P82" s="90"/>
+      <c r="Q82" s="90"/>
+      <c r="R82" s="90"/>
+      <c r="S82" s="90"/>
+      <c r="T82" s="90"/>
+      <c r="U82" s="90"/>
+      <c r="V82" s="90"/>
+      <c r="W82" s="90"/>
+      <c r="X82" s="90"/>
+      <c r="Y82" s="90"/>
+      <c r="Z82" s="90"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="B83" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" s="91" t="s">
+        <v>227</v>
+      </c>
+      <c r="D83" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="E83" s="45"/>
+      <c r="F83" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="G83" s="45" t="s">
         <v>230</v>
       </c>
-      <c r="B83" s="45" t="s">
-        <v>231</v>
-      </c>
-      <c r="C83" s="45" t="s">
-        <v>232</v>
-      </c>
-      <c r="D83" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="94"/>
-      <c r="F83" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G83" s="90"/>
-      <c r="H83" s="91"/>
-      <c r="I83" s="91"/>
-      <c r="J83" s="91"/>
-      <c r="K83" s="91"/>
-      <c r="L83" s="91"/>
-      <c r="M83" s="91"/>
-      <c r="N83" s="91"/>
-      <c r="O83" s="91"/>
-      <c r="P83" s="91"/>
-      <c r="Q83" s="91"/>
-      <c r="R83" s="91"/>
-      <c r="S83" s="91"/>
-      <c r="T83" s="91"/>
-      <c r="U83" s="91"/>
-      <c r="V83" s="91"/>
-      <c r="W83" s="91"/>
-      <c r="X83" s="91"/>
-      <c r="Y83" s="91"/>
-      <c r="Z83" s="91"/>
+      <c r="H83" s="90"/>
+      <c r="I83" s="90"/>
+      <c r="J83" s="90"/>
+      <c r="K83" s="90"/>
+      <c r="L83" s="90"/>
+      <c r="M83" s="90"/>
+      <c r="N83" s="90"/>
+      <c r="O83" s="90"/>
+      <c r="P83" s="90"/>
+      <c r="Q83" s="90"/>
+      <c r="R83" s="90"/>
+      <c r="S83" s="90"/>
+      <c r="T83" s="90"/>
+      <c r="U83" s="90"/>
+      <c r="V83" s="90"/>
+      <c r="W83" s="90"/>
+      <c r="X83" s="90"/>
+      <c r="Y83" s="90"/>
+      <c r="Z83" s="90"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="45" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B84" s="45" t="s">
-        <v>234</v>
-      </c>
-      <c r="C84" s="92" t="s">
-        <v>235</v>
+        <v>193</v>
+      </c>
+      <c r="C84" s="45" t="s">
+        <v>232</v>
       </c>
       <c r="D84" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="E84" s="94"/>
       <c r="F84" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G84" s="90"/>
-      <c r="H84" s="91"/>
-      <c r="I84" s="91"/>
-      <c r="J84" s="91"/>
-      <c r="K84" s="91"/>
-      <c r="L84" s="91"/>
-      <c r="M84" s="91"/>
-      <c r="N84" s="91"/>
-      <c r="O84" s="91"/>
-      <c r="P84" s="91"/>
-      <c r="Q84" s="91"/>
-      <c r="R84" s="91"/>
-      <c r="S84" s="91"/>
-      <c r="T84" s="91"/>
-      <c r="U84" s="91"/>
-      <c r="V84" s="91"/>
-      <c r="W84" s="91"/>
-      <c r="X84" s="91"/>
-      <c r="Y84" s="91"/>
-      <c r="Z84" s="91"/>
+        <v>107</v>
+      </c>
+      <c r="G84" s="89"/>
+      <c r="H84" s="90"/>
+      <c r="I84" s="90"/>
+      <c r="J84" s="90"/>
+      <c r="K84" s="90"/>
+      <c r="L84" s="90"/>
+      <c r="M84" s="90"/>
+      <c r="N84" s="90"/>
+      <c r="O84" s="90"/>
+      <c r="P84" s="90"/>
+      <c r="Q84" s="90"/>
+      <c r="R84" s="90"/>
+      <c r="S84" s="90"/>
+      <c r="T84" s="90"/>
+      <c r="U84" s="90"/>
+      <c r="V84" s="90"/>
+      <c r="W84" s="90"/>
+      <c r="X84" s="90"/>
+      <c r="Y84" s="90"/>
+      <c r="Z84" s="90"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="45" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B85" s="45" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D85" s="45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E85" s="94"/>
       <c r="F85" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G85" s="90"/>
-      <c r="H85" s="91"/>
-      <c r="I85" s="91"/>
-      <c r="J85" s="91"/>
-      <c r="K85" s="91"/>
-      <c r="L85" s="91"/>
-      <c r="M85" s="91"/>
-      <c r="N85" s="91"/>
-      <c r="O85" s="91"/>
-      <c r="P85" s="91"/>
-      <c r="Q85" s="91"/>
-      <c r="R85" s="91"/>
-      <c r="S85" s="91"/>
-      <c r="T85" s="91"/>
-      <c r="U85" s="91"/>
-      <c r="V85" s="91"/>
-      <c r="W85" s="91"/>
-      <c r="X85" s="91"/>
-      <c r="Y85" s="91"/>
-      <c r="Z85" s="91"/>
+        <v>178</v>
+      </c>
+      <c r="G85" s="89"/>
+      <c r="H85" s="90"/>
+      <c r="I85" s="90"/>
+      <c r="J85" s="90"/>
+      <c r="K85" s="90"/>
+      <c r="L85" s="90"/>
+      <c r="M85" s="90"/>
+      <c r="N85" s="90"/>
+      <c r="O85" s="90"/>
+      <c r="P85" s="90"/>
+      <c r="Q85" s="90"/>
+      <c r="R85" s="90"/>
+      <c r="S85" s="90"/>
+      <c r="T85" s="90"/>
+      <c r="U85" s="90"/>
+      <c r="V85" s="90"/>
+      <c r="W85" s="90"/>
+      <c r="X85" s="90"/>
+      <c r="Y85" s="90"/>
+      <c r="Z85" s="90"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="45" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B86" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="C86" s="92" t="s">
-        <v>241</v>
+        <v>237</v>
+      </c>
+      <c r="C86" s="91" t="s">
+        <v>238</v>
       </c>
       <c r="D86" s="45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E86" s="45"/>
       <c r="F86" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G86" s="90"/>
-      <c r="H86" s="91"/>
-      <c r="I86" s="91"/>
-      <c r="J86" s="91"/>
-      <c r="K86" s="91"/>
-      <c r="L86" s="91"/>
-      <c r="M86" s="91"/>
-      <c r="N86" s="91"/>
-      <c r="O86" s="91"/>
-      <c r="P86" s="91"/>
-      <c r="Q86" s="91"/>
-      <c r="R86" s="91"/>
-      <c r="S86" s="91"/>
-      <c r="T86" s="91"/>
-      <c r="U86" s="91"/>
-      <c r="V86" s="91"/>
-      <c r="W86" s="91"/>
-      <c r="X86" s="91"/>
-      <c r="Y86" s="91"/>
-      <c r="Z86" s="91"/>
+        <v>54</v>
+      </c>
+      <c r="G86" s="89"/>
+      <c r="H86" s="90"/>
+      <c r="I86" s="90"/>
+      <c r="J86" s="90"/>
+      <c r="K86" s="90"/>
+      <c r="L86" s="90"/>
+      <c r="M86" s="90"/>
+      <c r="N86" s="90"/>
+      <c r="O86" s="90"/>
+      <c r="P86" s="90"/>
+      <c r="Q86" s="90"/>
+      <c r="R86" s="90"/>
+      <c r="S86" s="90"/>
+      <c r="T86" s="90"/>
+      <c r="U86" s="90"/>
+      <c r="V86" s="90"/>
+      <c r="W86" s="90"/>
+      <c r="X86" s="90"/>
+      <c r="Y86" s="90"/>
+      <c r="Z86" s="90"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="45" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B87" s="45" t="s">
-        <v>109</v>
+        <v>240</v>
       </c>
       <c r="C87" s="45" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D87" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="E87" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="E87" s="94"/>
       <c r="F87" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G87" s="90"/>
-      <c r="H87" s="91"/>
-      <c r="I87" s="91"/>
-      <c r="J87" s="91"/>
-      <c r="K87" s="91"/>
-      <c r="L87" s="91"/>
-      <c r="M87" s="91"/>
-      <c r="N87" s="91"/>
-      <c r="O87" s="91"/>
-      <c r="P87" s="91"/>
-      <c r="Q87" s="91"/>
-      <c r="R87" s="91"/>
-      <c r="S87" s="91"/>
-      <c r="T87" s="91"/>
-      <c r="U87" s="91"/>
-      <c r="V87" s="91"/>
-      <c r="W87" s="91"/>
-      <c r="X87" s="91"/>
-      <c r="Y87" s="91"/>
-      <c r="Z87" s="91"/>
+        <v>54</v>
+      </c>
+      <c r="G87" s="89"/>
+      <c r="H87" s="90"/>
+      <c r="I87" s="90"/>
+      <c r="J87" s="90"/>
+      <c r="K87" s="90"/>
+      <c r="L87" s="90"/>
+      <c r="M87" s="90"/>
+      <c r="N87" s="90"/>
+      <c r="O87" s="90"/>
+      <c r="P87" s="90"/>
+      <c r="Q87" s="90"/>
+      <c r="R87" s="90"/>
+      <c r="S87" s="90"/>
+      <c r="T87" s="90"/>
+      <c r="U87" s="90"/>
+      <c r="V87" s="90"/>
+      <c r="W87" s="90"/>
+      <c r="X87" s="90"/>
+      <c r="Y87" s="90"/>
+      <c r="Z87" s="90"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="45" t="s">
-        <v>171</v>
+        <v>242</v>
       </c>
       <c r="B88" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C88" s="45" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+      <c r="C88" s="91" t="s">
+        <v>244</v>
       </c>
       <c r="D88" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E88" s="45"/>
       <c r="F88" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G88" s="90"/>
-      <c r="H88" s="91"/>
-      <c r="I88" s="91"/>
-      <c r="J88" s="91"/>
-      <c r="K88" s="91"/>
-      <c r="L88" s="91"/>
-      <c r="M88" s="91"/>
-      <c r="N88" s="91"/>
-      <c r="O88" s="91"/>
-      <c r="P88" s="91"/>
-      <c r="Q88" s="91"/>
-      <c r="R88" s="91"/>
-      <c r="S88" s="91"/>
-      <c r="T88" s="91"/>
-      <c r="U88" s="91"/>
-      <c r="V88" s="91"/>
-      <c r="W88" s="91"/>
-      <c r="X88" s="91"/>
-      <c r="Y88" s="91"/>
-      <c r="Z88" s="91"/>
+        <v>107</v>
+      </c>
+      <c r="G88" s="89"/>
+      <c r="H88" s="90"/>
+      <c r="I88" s="90"/>
+      <c r="J88" s="90"/>
+      <c r="K88" s="90"/>
+      <c r="L88" s="90"/>
+      <c r="M88" s="90"/>
+      <c r="N88" s="90"/>
+      <c r="O88" s="90"/>
+      <c r="P88" s="90"/>
+      <c r="Q88" s="90"/>
+      <c r="R88" s="90"/>
+      <c r="S88" s="90"/>
+      <c r="T88" s="90"/>
+      <c r="U88" s="90"/>
+      <c r="V88" s="90"/>
+      <c r="W88" s="90"/>
+      <c r="X88" s="90"/>
+      <c r="Y88" s="90"/>
+      <c r="Z88" s="90"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="45" t="s">
-        <v>176</v>
+        <v>245</v>
       </c>
       <c r="B89" s="45" t="s">
-        <v>177</v>
+        <v>109</v>
       </c>
       <c r="C89" s="45" t="s">
         <v>246</v>
       </c>
       <c r="D89" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E89" s="94"/>
+        <v>247</v>
+      </c>
+      <c r="E89" s="45"/>
       <c r="F89" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="G89" s="90"/>
-      <c r="H89" s="91"/>
-      <c r="I89" s="91"/>
-      <c r="J89" s="91"/>
-      <c r="K89" s="91"/>
-      <c r="L89" s="91"/>
-      <c r="M89" s="91"/>
-      <c r="N89" s="91"/>
-      <c r="O89" s="91"/>
-      <c r="P89" s="91"/>
-      <c r="Q89" s="91"/>
-      <c r="R89" s="91"/>
-      <c r="S89" s="91"/>
-      <c r="T89" s="91"/>
-      <c r="U89" s="91"/>
-      <c r="V89" s="91"/>
-      <c r="W89" s="91"/>
-      <c r="X89" s="91"/>
-      <c r="Y89" s="91"/>
-      <c r="Z89" s="91"/>
+        <v>107</v>
+      </c>
+      <c r="G89" s="89"/>
+      <c r="H89" s="90"/>
+      <c r="I89" s="90"/>
+      <c r="J89" s="90"/>
+      <c r="K89" s="90"/>
+      <c r="L89" s="90"/>
+      <c r="M89" s="90"/>
+      <c r="N89" s="90"/>
+      <c r="O89" s="90"/>
+      <c r="P89" s="90"/>
+      <c r="Q89" s="90"/>
+      <c r="R89" s="90"/>
+      <c r="S89" s="90"/>
+      <c r="T89" s="90"/>
+      <c r="U89" s="90"/>
+      <c r="V89" s="90"/>
+      <c r="W89" s="90"/>
+      <c r="X89" s="90"/>
+      <c r="Y89" s="90"/>
+      <c r="Z89" s="90"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="D90" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E90" s="45"/>
+      <c r="F90" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="G90" s="89"/>
+      <c r="H90" s="90"/>
+      <c r="I90" s="90"/>
+      <c r="J90" s="90"/>
+      <c r="K90" s="90"/>
+      <c r="L90" s="90"/>
+      <c r="M90" s="90"/>
+      <c r="N90" s="90"/>
+      <c r="O90" s="90"/>
+      <c r="P90" s="90"/>
+      <c r="Q90" s="90"/>
+      <c r="R90" s="90"/>
+      <c r="S90" s="90"/>
+      <c r="T90" s="90"/>
+      <c r="U90" s="90"/>
+      <c r="V90" s="90"/>
+      <c r="W90" s="90"/>
+      <c r="X90" s="90"/>
+      <c r="Y90" s="90"/>
+      <c r="Z90" s="90"/>
+    </row>
+    <row r="91" ht="15.75" customHeight="1">
+      <c r="A91" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="B90" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="C90" s="45" t="s">
+      <c r="C91" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="D91" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E91" s="94"/>
+      <c r="F91" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="D90" s="45" t="s">
+      <c r="G91" s="89"/>
+      <c r="H91" s="90"/>
+      <c r="I91" s="90"/>
+      <c r="J91" s="90"/>
+      <c r="K91" s="90"/>
+      <c r="L91" s="90"/>
+      <c r="M91" s="90"/>
+      <c r="N91" s="90"/>
+      <c r="O91" s="90"/>
+      <c r="P91" s="90"/>
+      <c r="Q91" s="90"/>
+      <c r="R91" s="90"/>
+      <c r="S91" s="90"/>
+      <c r="T91" s="90"/>
+      <c r="U91" s="90"/>
+      <c r="V91" s="90"/>
+      <c r="W91" s="90"/>
+      <c r="X91" s="90"/>
+      <c r="Y91" s="90"/>
+      <c r="Z91" s="90"/>
+    </row>
+    <row r="92" ht="15.75" customHeight="1">
+      <c r="A92" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C92" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="D92" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="E90" s="94"/>
-      <c r="F90" s="44" t="s">
-        <v>179</v>
-      </c>
-      <c r="G90" s="90"/>
-      <c r="H90" s="91"/>
-      <c r="I90" s="91"/>
-      <c r="J90" s="91"/>
-      <c r="K90" s="91"/>
-      <c r="L90" s="91"/>
-      <c r="M90" s="91"/>
-      <c r="N90" s="91"/>
-      <c r="O90" s="91"/>
-      <c r="P90" s="91"/>
-      <c r="Q90" s="91"/>
-      <c r="R90" s="91"/>
-      <c r="S90" s="91"/>
-      <c r="T90" s="91"/>
-      <c r="U90" s="91"/>
-      <c r="V90" s="91"/>
-      <c r="W90" s="91"/>
-      <c r="X90" s="91"/>
-      <c r="Y90" s="91"/>
-      <c r="Z90" s="91"/>
-    </row>
-    <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="4"/>
-      <c r="G91" s="5"/>
-    </row>
-    <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="95"/>
-      <c r="G92" s="5"/>
+      <c r="E92" s="94"/>
+      <c r="F92" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G92" s="89"/>
+      <c r="H92" s="90"/>
+      <c r="I92" s="90"/>
+      <c r="J92" s="90"/>
+      <c r="K92" s="90"/>
+      <c r="L92" s="90"/>
+      <c r="M92" s="90"/>
+      <c r="N92" s="90"/>
+      <c r="O92" s="90"/>
+      <c r="P92" s="90"/>
+      <c r="Q92" s="90"/>
+      <c r="R92" s="90"/>
+      <c r="S92" s="90"/>
+      <c r="T92" s="90"/>
+      <c r="U92" s="90"/>
+      <c r="V92" s="90"/>
+      <c r="W92" s="90"/>
+      <c r="X92" s="90"/>
+      <c r="Y92" s="90"/>
+      <c r="Z92" s="90"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
+      <c r="A93" s="4"/>
       <c r="G93" s="5"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
+      <c r="A94" s="95"/>
       <c r="G94" s="5"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
@@ -8827,6 +8960,12 @@
     </row>
     <row r="999" ht="15.75" customHeight="1">
       <c r="G999" s="5"/>
+    </row>
+    <row r="1000" ht="15.75" customHeight="1">
+      <c r="G1000" s="5"/>
+    </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="G1001" s="5"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>

<commit_message>
State 6 Implementation v5.0.0- scoring
State 6 Implementation v5.0.0- scoring
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SERVERMS30\usuarios$\secundaria\nicolas.philippe\Documents\GitHub\internal-java\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CB050D-3AF1-4A26-A371-F9A0CD039840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A464B9E-3D15-4F3D-87F0-802F7D6CB436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="259">
   <si>
     <t>Waterfall Methodology</t>
   </si>
@@ -2301,6 +2301,24 @@
   </si>
   <si>
     <t>04/27/2025</t>
+  </si>
+  <si>
+    <t>Implement Chekers Logic</t>
+  </si>
+  <si>
+    <t>5/27/2025</t>
+  </si>
+  <si>
+    <t>Working Checkers Game</t>
+  </si>
+  <si>
+    <t>Implement Scoring</t>
+  </si>
+  <si>
+    <t>Scoring implemented</t>
+  </si>
+  <si>
+    <t>20 mn</t>
   </si>
 </sst>
 </file>
@@ -2862,13 +2880,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3089,10 +3107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5165,136 +5183,100 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="75" t="s">
+    <row r="55" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="C55" s="96" t="s">
+        <v>255</v>
+      </c>
+      <c r="D55" s="96" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="97" t="s">
+        <v>254</v>
+      </c>
+      <c r="F55" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="94" t="s">
+        <v>256</v>
+      </c>
+      <c r="C56" s="96" t="s">
+        <v>257</v>
+      </c>
+      <c r="D56" s="96" t="s">
+        <v>258</v>
+      </c>
+      <c r="E56" s="97" t="s">
+        <v>254</v>
+      </c>
+      <c r="F56" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="B55" s="75" t="s">
+      <c r="B57" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="C55" s="75" t="s">
+      <c r="C57" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="D55" s="75" t="s">
+      <c r="D57" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="76"/>
-      <c r="F55" s="77" t="s">
+      <c r="E57" s="76"/>
+      <c r="F57" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="G55" s="78"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
-      <c r="M55" s="79"/>
-      <c r="N55" s="79"/>
-      <c r="O55" s="79"/>
-      <c r="P55" s="79"/>
-      <c r="Q55" s="79"/>
-      <c r="R55" s="79"/>
-      <c r="S55" s="79"/>
-      <c r="T55" s="79"/>
-      <c r="U55" s="79"/>
-      <c r="V55" s="79"/>
-      <c r="W55" s="79"/>
-      <c r="X55" s="79"/>
-      <c r="Y55" s="79"/>
-      <c r="Z55" s="79"/>
-    </row>
-    <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C56" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E56" s="80"/>
-      <c r="F56" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G56" s="81"/>
-      <c r="H56" s="82"/>
-      <c r="I56" s="82"/>
-      <c r="J56" s="82"/>
-      <c r="K56" s="82"/>
-      <c r="L56" s="82"/>
-      <c r="M56" s="82"/>
-      <c r="N56" s="82"/>
-      <c r="O56" s="82"/>
-      <c r="P56" s="82"/>
-      <c r="Q56" s="82"/>
-      <c r="R56" s="82"/>
-      <c r="S56" s="82"/>
-      <c r="T56" s="82"/>
-      <c r="U56" s="82"/>
-      <c r="V56" s="82"/>
-      <c r="W56" s="82"/>
-      <c r="X56" s="82"/>
-      <c r="Y56" s="82"/>
-      <c r="Z56" s="82"/>
-    </row>
-    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="E57" s="80"/>
-      <c r="F57" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="G57" s="81"/>
-      <c r="H57" s="82"/>
-      <c r="I57" s="82"/>
-      <c r="J57" s="82"/>
-      <c r="K57" s="82"/>
-      <c r="L57" s="82"/>
-      <c r="M57" s="82"/>
-      <c r="N57" s="82"/>
-      <c r="O57" s="82"/>
-      <c r="P57" s="82"/>
-      <c r="Q57" s="82"/>
-      <c r="R57" s="82"/>
-      <c r="S57" s="82"/>
-      <c r="T57" s="82"/>
-      <c r="U57" s="82"/>
-      <c r="V57" s="82"/>
-      <c r="W57" s="82"/>
-      <c r="X57" s="82"/>
-      <c r="Y57" s="82"/>
-      <c r="Z57" s="82"/>
+      <c r="G57" s="78"/>
+      <c r="H57" s="79"/>
+      <c r="I57" s="79"/>
+      <c r="J57" s="79"/>
+      <c r="K57" s="79"/>
+      <c r="L57" s="79"/>
+      <c r="M57" s="79"/>
+      <c r="N57" s="79"/>
+      <c r="O57" s="79"/>
+      <c r="P57" s="79"/>
+      <c r="Q57" s="79"/>
+      <c r="R57" s="79"/>
+      <c r="S57" s="79"/>
+      <c r="T57" s="79"/>
+      <c r="U57" s="79"/>
+      <c r="V57" s="79"/>
+      <c r="W57" s="79"/>
+      <c r="X57" s="79"/>
+      <c r="Y57" s="79"/>
+      <c r="Z57" s="79"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E58" s="80"/>
       <c r="F58" s="28" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="G58" s="81"/>
       <c r="H58" s="82"/>
@@ -5318,69 +5300,135 @@
       <c r="Z58" s="82"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="E59" s="80"/>
+      <c r="F59" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="G59" s="81"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="82"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="82"/>
+      <c r="L59" s="82"/>
+      <c r="M59" s="82"/>
+      <c r="N59" s="82"/>
+      <c r="O59" s="82"/>
+      <c r="P59" s="82"/>
+      <c r="Q59" s="82"/>
+      <c r="R59" s="82"/>
+      <c r="S59" s="82"/>
+      <c r="T59" s="82"/>
+      <c r="U59" s="82"/>
+      <c r="V59" s="82"/>
+      <c r="W59" s="82"/>
+      <c r="X59" s="82"/>
+      <c r="Y59" s="82"/>
+      <c r="Z59" s="82"/>
+    </row>
+    <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E60" s="80"/>
+      <c r="F60" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="G60" s="81"/>
+      <c r="H60" s="82"/>
+      <c r="I60" s="82"/>
+      <c r="J60" s="82"/>
+      <c r="K60" s="82"/>
+      <c r="L60" s="82"/>
+      <c r="M60" s="82"/>
+      <c r="N60" s="82"/>
+      <c r="O60" s="82"/>
+      <c r="P60" s="82"/>
+      <c r="Q60" s="82"/>
+      <c r="R60" s="82"/>
+      <c r="S60" s="82"/>
+      <c r="T60" s="82"/>
+      <c r="U60" s="82"/>
+      <c r="V60" s="82"/>
+      <c r="W60" s="82"/>
+      <c r="X60" s="82"/>
+      <c r="Y60" s="82"/>
+      <c r="Z60" s="82"/>
+    </row>
+    <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B61" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C61" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D61" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E59" s="9"/>
-      <c r="F59" s="10" t="s">
+      <c r="E61" s="9"/>
+      <c r="F61" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G59" s="83"/>
-      <c r="H59" s="84"/>
-      <c r="I59" s="84"/>
-      <c r="J59" s="84"/>
-      <c r="K59" s="84"/>
-      <c r="L59" s="84"/>
-      <c r="M59" s="84"/>
-      <c r="N59" s="84"/>
-      <c r="O59" s="84"/>
-      <c r="P59" s="84"/>
-      <c r="Q59" s="84"/>
-      <c r="R59" s="84"/>
-      <c r="S59" s="84"/>
-      <c r="T59" s="84"/>
-      <c r="U59" s="84"/>
-      <c r="V59" s="84"/>
-      <c r="W59" s="84"/>
-      <c r="X59" s="84"/>
-      <c r="Y59" s="84"/>
-      <c r="Z59" s="84"/>
-    </row>
-    <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="85"/>
-      <c r="B60" s="85"/>
-      <c r="C60" s="85"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="86"/>
-      <c r="F60" s="87"/>
-      <c r="G60" s="5"/>
-    </row>
-    <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="85"/>
-      <c r="B61" s="85"/>
-      <c r="C61" s="85"/>
-      <c r="D61" s="85"/>
-      <c r="E61" s="86"/>
-      <c r="F61" s="87"/>
-      <c r="G61" s="5"/>
+      <c r="G61" s="83"/>
+      <c r="H61" s="84"/>
+      <c r="I61" s="84"/>
+      <c r="J61" s="84"/>
+      <c r="K61" s="84"/>
+      <c r="L61" s="84"/>
+      <c r="M61" s="84"/>
+      <c r="N61" s="84"/>
+      <c r="O61" s="84"/>
+      <c r="P61" s="84"/>
+      <c r="Q61" s="84"/>
+      <c r="R61" s="84"/>
+      <c r="S61" s="84"/>
+      <c r="T61" s="84"/>
+      <c r="U61" s="84"/>
+      <c r="V61" s="84"/>
+      <c r="W61" s="84"/>
+      <c r="X61" s="84"/>
+      <c r="Y61" s="84"/>
+      <c r="Z61" s="84"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
+      <c r="A62" s="85"/>
+      <c r="B62" s="85"/>
+      <c r="C62" s="85"/>
+      <c r="D62" s="85"/>
+      <c r="E62" s="86"/>
+      <c r="F62" s="87"/>
       <c r="G62" s="5"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="A63" s="85"/>
+      <c r="B63" s="85"/>
+      <c r="C63" s="85"/>
+      <c r="D63" s="85"/>
+      <c r="E63" s="86"/>
+      <c r="F63" s="87"/>
       <c r="G63" s="5"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5388,118 +5436,52 @@
       <c r="G64" s="5"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G65" s="5"/>
+    </row>
+    <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="G66" s="5"/>
+    </row>
+    <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B67" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C67" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D67" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E67" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F67" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G65" s="5"/>
-    </row>
-    <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="B66" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="C66" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="D66" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E66" s="45"/>
-      <c r="F66" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G66" s="88"/>
-      <c r="H66" s="89"/>
-      <c r="I66" s="89"/>
-      <c r="J66" s="89"/>
-      <c r="K66" s="89"/>
-      <c r="L66" s="89"/>
-      <c r="M66" s="89"/>
-      <c r="N66" s="89"/>
-      <c r="O66" s="89"/>
-      <c r="P66" s="89"/>
-      <c r="Q66" s="89"/>
-      <c r="R66" s="89"/>
-      <c r="S66" s="89"/>
-      <c r="T66" s="89"/>
-      <c r="U66" s="89"/>
-      <c r="V66" s="89"/>
-      <c r="W66" s="89"/>
-      <c r="X66" s="89"/>
-      <c r="Y66" s="89"/>
-      <c r="Z66" s="89"/>
-    </row>
-    <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="B67" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="C67" s="90" t="s">
-        <v>194</v>
-      </c>
-      <c r="D67" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E67" s="45"/>
-      <c r="F67" s="44" t="s">
-        <v>195</v>
-      </c>
-      <c r="G67" s="88"/>
-      <c r="H67" s="89"/>
-      <c r="I67" s="89"/>
-      <c r="J67" s="89"/>
-      <c r="K67" s="89"/>
-      <c r="L67" s="89"/>
-      <c r="M67" s="89"/>
-      <c r="N67" s="89"/>
-      <c r="O67" s="89"/>
-      <c r="P67" s="89"/>
-      <c r="Q67" s="89"/>
-      <c r="R67" s="89"/>
-      <c r="S67" s="89"/>
-      <c r="T67" s="89"/>
-      <c r="U67" s="89"/>
-      <c r="V67" s="89"/>
-      <c r="W67" s="89"/>
-      <c r="X67" s="89"/>
-      <c r="Y67" s="89"/>
-      <c r="Z67" s="89"/>
+      <c r="G67" s="5"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="45" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B68" s="45" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D68" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E68" s="45"/>
       <c r="F68" s="44" t="s">
-        <v>199</v>
+        <v>13</v>
       </c>
       <c r="G68" s="88"/>
       <c r="H68" s="89"/>
@@ -5524,13 +5506,13 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="45" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B69" s="45" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C69" s="90" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D69" s="45" t="s">
         <v>30</v>
@@ -5565,10 +5547,10 @@
         <v>196</v>
       </c>
       <c r="B70" s="45" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D70" s="45" t="s">
         <v>86</v>
@@ -5600,13 +5582,13 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="45" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C71" s="90" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D71" s="45" t="s">
         <v>30</v>
@@ -5641,17 +5623,17 @@
         <v>196</v>
       </c>
       <c r="B72" s="45" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C72" s="45" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D72" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E72" s="45"/>
       <c r="F72" s="44" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="G72" s="88"/>
       <c r="H72" s="89"/>
@@ -5676,13 +5658,13 @@
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="45" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B73" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="C73" s="91" t="s">
-        <v>212</v>
+        <v>206</v>
+      </c>
+      <c r="C73" s="90" t="s">
+        <v>207</v>
       </c>
       <c r="D73" s="45" t="s">
         <v>30</v>
@@ -5717,7 +5699,7 @@
         <v>196</v>
       </c>
       <c r="B74" s="45" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C74" s="45" t="s">
         <v>209</v>
@@ -5752,20 +5734,20 @@
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B75" s="45" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C75" s="91" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D75" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E75" s="45"/>
       <c r="F75" s="44" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="G75" s="88"/>
       <c r="H75" s="89"/>
@@ -5790,20 +5772,20 @@
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="45" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B76" s="45" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="C76" s="45" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="D76" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E76" s="45"/>
       <c r="F76" s="44" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G76" s="88"/>
       <c r="H76" s="89"/>
@@ -5828,20 +5810,20 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="45" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="B77" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="C77" s="45" t="s">
-        <v>185</v>
+        <v>215</v>
+      </c>
+      <c r="C77" s="91" t="s">
+        <v>216</v>
       </c>
       <c r="D77" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E77" s="45"/>
       <c r="F77" s="44" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="G77" s="88"/>
       <c r="H77" s="89"/>
@@ -5865,138 +5847,134 @@
       <c r="Z77" s="89"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="G78" s="5"/>
+      <c r="A78" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="D78" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E78" s="45"/>
+      <c r="F78" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G78" s="88"/>
+      <c r="H78" s="89"/>
+      <c r="I78" s="89"/>
+      <c r="J78" s="89"/>
+      <c r="K78" s="89"/>
+      <c r="L78" s="89"/>
+      <c r="M78" s="89"/>
+      <c r="N78" s="89"/>
+      <c r="O78" s="89"/>
+      <c r="P78" s="89"/>
+      <c r="Q78" s="89"/>
+      <c r="R78" s="89"/>
+      <c r="S78" s="89"/>
+      <c r="T78" s="89"/>
+      <c r="U78" s="89"/>
+      <c r="V78" s="89"/>
+      <c r="W78" s="89"/>
+      <c r="X78" s="89"/>
+      <c r="Y78" s="89"/>
+      <c r="Z78" s="89"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G79" s="5"/>
+      <c r="A79" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B79" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C79" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="D79" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" s="45"/>
+      <c r="F79" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G79" s="88"/>
+      <c r="H79" s="89"/>
+      <c r="I79" s="89"/>
+      <c r="J79" s="89"/>
+      <c r="K79" s="89"/>
+      <c r="L79" s="89"/>
+      <c r="M79" s="89"/>
+      <c r="N79" s="89"/>
+      <c r="O79" s="89"/>
+      <c r="P79" s="89"/>
+      <c r="Q79" s="89"/>
+      <c r="R79" s="89"/>
+      <c r="S79" s="89"/>
+      <c r="T79" s="89"/>
+      <c r="U79" s="89"/>
+      <c r="V79" s="89"/>
+      <c r="W79" s="89"/>
+      <c r="X79" s="89"/>
+      <c r="Y79" s="89"/>
+      <c r="Z79" s="89"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="G80" s="5"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+      <c r="A81" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G81" s="5"/>
+    </row>
+    <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="G82" s="5"/>
+    </row>
+    <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B83" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C83" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D83" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E83" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F83" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G81" s="5"/>
-    </row>
-    <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="B82" s="45" t="s">
-        <v>220</v>
-      </c>
-      <c r="C82" s="90" t="s">
-        <v>221</v>
-      </c>
-      <c r="D82" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E82" s="45"/>
-      <c r="F82" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G82" s="88"/>
-      <c r="H82" s="89"/>
-      <c r="I82" s="89"/>
-      <c r="J82" s="89"/>
-      <c r="K82" s="89"/>
-      <c r="L82" s="89"/>
-      <c r="M82" s="89"/>
-      <c r="N82" s="89"/>
-      <c r="O82" s="89"/>
-      <c r="P82" s="89"/>
-      <c r="Q82" s="89"/>
-      <c r="R82" s="89"/>
-      <c r="S82" s="89"/>
-      <c r="T82" s="89"/>
-      <c r="U82" s="89"/>
-      <c r="V82" s="89"/>
-      <c r="W82" s="89"/>
-      <c r="X82" s="89"/>
-      <c r="Y82" s="89"/>
-      <c r="Z82" s="89"/>
-    </row>
-    <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="B83" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="C83" s="90" t="s">
-        <v>224</v>
-      </c>
-      <c r="D83" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="45"/>
-      <c r="F83" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G83" s="45" t="s">
-        <v>225</v>
-      </c>
-      <c r="H83" s="89"/>
-      <c r="I83" s="89"/>
-      <c r="J83" s="89"/>
-      <c r="K83" s="89"/>
-      <c r="L83" s="89"/>
-      <c r="M83" s="89"/>
-      <c r="N83" s="89"/>
-      <c r="O83" s="89"/>
-      <c r="P83" s="89"/>
-      <c r="Q83" s="89"/>
-      <c r="R83" s="89"/>
-      <c r="S83" s="89"/>
-      <c r="T83" s="89"/>
-      <c r="U83" s="89"/>
-      <c r="V83" s="89"/>
-      <c r="W83" s="89"/>
-      <c r="X83" s="89"/>
-      <c r="Y83" s="89"/>
-      <c r="Z83" s="89"/>
+      <c r="G83" s="5"/>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="45" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B84" s="45" t="s">
-        <v>28</v>
+        <v>220</v>
       </c>
       <c r="C84" s="90" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D84" s="45" t="s">
-        <v>228</v>
+        <v>16</v>
       </c>
       <c r="E84" s="45"/>
       <c r="F84" s="44" t="s">
-        <v>229</v>
-      </c>
-      <c r="G84" s="45" t="s">
-        <v>230</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G84" s="88"/>
       <c r="H84" s="89"/>
       <c r="I84" s="89"/>
       <c r="J84" s="89"/>
@@ -6019,22 +5997,24 @@
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="45" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B85" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="C85" s="45" t="s">
-        <v>232</v>
+        <v>223</v>
+      </c>
+      <c r="C85" s="90" t="s">
+        <v>224</v>
       </c>
       <c r="D85" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E85" s="92"/>
+        <v>11</v>
+      </c>
+      <c r="E85" s="45"/>
       <c r="F85" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G85" s="88"/>
+        <v>13</v>
+      </c>
+      <c r="G85" s="45" t="s">
+        <v>225</v>
+      </c>
       <c r="H85" s="89"/>
       <c r="I85" s="89"/>
       <c r="J85" s="89"/>
@@ -6057,22 +6037,24 @@
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="45" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B86" s="45" t="s">
-        <v>234</v>
-      </c>
-      <c r="C86" s="45" t="s">
-        <v>235</v>
+        <v>28</v>
+      </c>
+      <c r="C86" s="90" t="s">
+        <v>227</v>
       </c>
       <c r="D86" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" s="92"/>
+        <v>228</v>
+      </c>
+      <c r="E86" s="45"/>
       <c r="F86" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="G86" s="88"/>
+        <v>229</v>
+      </c>
+      <c r="G86" s="45" t="s">
+        <v>230</v>
+      </c>
       <c r="H86" s="89"/>
       <c r="I86" s="89"/>
       <c r="J86" s="89"/>
@@ -6095,20 +6077,20 @@
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="45" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B87" s="45" t="s">
-        <v>237</v>
-      </c>
-      <c r="C87" s="90" t="s">
-        <v>238</v>
+        <v>193</v>
+      </c>
+      <c r="C87" s="45" t="s">
+        <v>232</v>
       </c>
       <c r="D87" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="E87" s="92"/>
       <c r="F87" s="44" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="G87" s="88"/>
       <c r="H87" s="89"/>
@@ -6133,20 +6115,20 @@
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="45" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B88" s="45" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C88" s="45" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D88" s="45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E88" s="92"/>
       <c r="F88" s="44" t="s">
-        <v>54</v>
+        <v>178</v>
       </c>
       <c r="G88" s="88"/>
       <c r="H88" s="89"/>
@@ -6171,20 +6153,20 @@
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="45" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B89" s="45" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C89" s="90" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D89" s="45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E89" s="45"/>
       <c r="F89" s="44" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="G89" s="88"/>
       <c r="H89" s="89"/>
@@ -6209,20 +6191,20 @@
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="45" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B90" s="45" t="s">
-        <v>109</v>
+        <v>240</v>
       </c>
       <c r="C90" s="45" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D90" s="45" t="s">
-        <v>247</v>
-      </c>
-      <c r="E90" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="E90" s="92"/>
       <c r="F90" s="44" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="G90" s="88"/>
       <c r="H90" s="89"/>
@@ -6247,20 +6229,20 @@
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="45" t="s">
-        <v>174</v>
+        <v>242</v>
       </c>
       <c r="B91" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="C91" s="45" t="s">
-        <v>248</v>
+        <v>243</v>
+      </c>
+      <c r="C91" s="90" t="s">
+        <v>244</v>
       </c>
       <c r="D91" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E91" s="45"/>
       <c r="F91" s="44" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
       <c r="G91" s="88"/>
       <c r="H91" s="89"/>
@@ -6285,20 +6267,20 @@
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="45" t="s">
-        <v>179</v>
+        <v>245</v>
       </c>
       <c r="B92" s="45" t="s">
-        <v>180</v>
+        <v>109</v>
       </c>
       <c r="C92" s="45" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D92" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E92" s="92"/>
+        <v>247</v>
+      </c>
+      <c r="E92" s="45"/>
       <c r="F92" s="44" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="G92" s="88"/>
       <c r="H92" s="89"/>
@@ -6323,20 +6305,20 @@
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="45" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B93" s="45" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C93" s="45" t="s">
-        <v>185</v>
+        <v>248</v>
       </c>
       <c r="D93" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E93" s="92"/>
+        <v>30</v>
+      </c>
+      <c r="E93" s="45"/>
       <c r="F93" s="44" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G93" s="88"/>
       <c r="H93" s="89"/>
@@ -6360,62 +6342,132 @@
       <c r="Z93" s="89"/>
     </row>
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="G94" s="5"/>
+      <c r="A94" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="D94" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" s="92"/>
+      <c r="F94" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G94" s="88"/>
+      <c r="H94" s="89"/>
+      <c r="I94" s="89"/>
+      <c r="J94" s="89"/>
+      <c r="K94" s="89"/>
+      <c r="L94" s="89"/>
+      <c r="M94" s="89"/>
+      <c r="N94" s="89"/>
+      <c r="O94" s="89"/>
+      <c r="P94" s="89"/>
+      <c r="Q94" s="89"/>
+      <c r="R94" s="89"/>
+      <c r="S94" s="89"/>
+      <c r="T94" s="89"/>
+      <c r="U94" s="89"/>
+      <c r="V94" s="89"/>
+      <c r="W94" s="89"/>
+      <c r="X94" s="89"/>
+      <c r="Y94" s="89"/>
+      <c r="Z94" s="89"/>
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="93"/>
-      <c r="G95" s="5"/>
+      <c r="A95" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B95" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C95" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="D95" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E95" s="92"/>
+      <c r="F95" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G95" s="88"/>
+      <c r="H95" s="89"/>
+      <c r="I95" s="89"/>
+      <c r="J95" s="89"/>
+      <c r="K95" s="89"/>
+      <c r="L95" s="89"/>
+      <c r="M95" s="89"/>
+      <c r="N95" s="89"/>
+      <c r="O95" s="89"/>
+      <c r="P95" s="89"/>
+      <c r="Q95" s="89"/>
+      <c r="R95" s="89"/>
+      <c r="S95" s="89"/>
+      <c r="T95" s="89"/>
+      <c r="U95" s="89"/>
+      <c r="V95" s="89"/>
+      <c r="W95" s="89"/>
+      <c r="X95" s="89"/>
+      <c r="Y95" s="89"/>
+      <c r="Z95" s="89"/>
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="93"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G112" s="5"/>
     </row>
     <row r="113" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9087,6 +9139,12 @@
     </row>
     <row r="1002" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1002" s="5"/>
+    </row>
+    <row r="1003" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1003" s="5"/>
+    </row>
+    <row r="1004" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1004" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
v6.0.0 Database Development- Defining the interface, Implementing the mysql Db
v6.0.0 Database Integration - Defining the interface, Implementing the mysql Db:
- interface create in Java abstracting the mockup
- mysql installed
- physical schema added
- default initial data script added
- sql statements created
</commit_message>
<xml_diff>
--- a/documentation/Record Of Tasks.xlsx
+++ b/documentation/Record Of Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SERVERMS30\usuarios$\secundaria\nicolas.philippe\Documents\GitHub\internal-java\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A464B9E-3D15-4F3D-87F0-802F7D6CB436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F97DF48-617C-4FAF-8C02-702FA0C9309D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="264">
   <si>
     <t>Waterfall Methodology</t>
   </si>
@@ -1746,42 +1746,6 @@
     <t>BaseView Implemented and all view inherits from it</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Quattrocento Sans"/>
-      </rPr>
-      <t xml:space="preserve">Documentation according to client review and features implemented </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Segoe UI"/>
-      </rPr>
-      <t>to now:  AppStatus State Machinel, UML View Class Model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Segoe UI"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Segoe UI"/>
-      </rPr>
-      <t xml:space="preserve">Sketch-View </t>
-    </r>
-  </si>
-  <si>
     <t>Implement the database</t>
   </si>
   <si>
@@ -2303,22 +2267,116 @@
     <t>04/27/2025</t>
   </si>
   <si>
-    <t>Implement Chekers Logic</t>
-  </si>
-  <si>
-    <t>5/27/2025</t>
-  </si>
-  <si>
-    <t>Working Checkers Game</t>
-  </si>
-  <si>
-    <t>Implement Scoring</t>
-  </si>
-  <si>
-    <t>Scoring implemented</t>
-  </si>
-  <si>
-    <t>20 mn</t>
+    <t>Install mysql</t>
+  </si>
+  <si>
+    <t>sql installed and running</t>
+  </si>
+  <si>
+    <t>05/27/2025</t>
+  </si>
+  <si>
+    <t>Create physical database model</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documentation according to client review and features implemented </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+      </rPr>
+      <t>to now:  AppStatus State Machine, UML View Class Model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+      </rPr>
+      <t xml:space="preserve">Sketch-View </t>
+    </r>
+  </si>
+  <si>
+    <t>importing physical database model and some initial data</t>
+  </si>
+  <si>
+    <t>07/27/2025</t>
+  </si>
+  <si>
+    <t>create the interface and the required sql statement</t>
+  </si>
+  <si>
+    <t>Using the mockup, we extract its interface to create the db interface, and we created all the required sql statements</t>
+  </si>
+  <si>
+    <t>08/27/2025</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Quattrocento Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>Script for generating scheme, script for inserting default data, script for selecting the data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Quattrocento Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Quattrocento Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>Physical DB entity mode</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Quattrocento Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Quattrocento Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> using https://sqldbm.com/
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2328,7 +2386,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2499,6 +2557,27 @@
       <name val="Quattrocento Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Quattrocento Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Quattrocento Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2631,7 +2710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2892,6 +2971,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3107,10 +3187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5129,7 +5209,7 @@
         <v>150</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>168</v>
+        <v>256</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>46</v>
@@ -5168,53 +5248,71 @@
         <v>108</v>
       </c>
       <c r="B54" s="94" t="s">
+        <v>249</v>
+      </c>
+      <c r="C54" s="96" t="s">
         <v>250</v>
-      </c>
-      <c r="C54" s="96" t="s">
-        <v>251</v>
       </c>
       <c r="D54" s="96" t="s">
         <v>42</v>
       </c>
       <c r="E54" s="97" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F54" s="41" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B55" s="94" t="s">
-        <v>253</v>
-      </c>
-      <c r="C55" s="96" t="s">
-        <v>255</v>
-      </c>
-      <c r="D55" s="96" t="s">
-        <v>16</v>
-      </c>
-      <c r="E55" s="97" t="s">
-        <v>254</v>
-      </c>
-      <c r="F55" s="41" t="s">
+    <row r="55" spans="1:26" ht="39.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="D55" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="76"/>
+      <c r="F55" s="77" t="s">
         <v>107</v>
       </c>
+      <c r="G55" s="78"/>
+      <c r="H55" s="79"/>
+      <c r="I55" s="79"/>
+      <c r="J55" s="79"/>
+      <c r="K55" s="79"/>
+      <c r="L55" s="79"/>
+      <c r="M55" s="79"/>
+      <c r="N55" s="79"/>
+      <c r="O55" s="79"/>
+      <c r="P55" s="79"/>
+      <c r="Q55" s="79"/>
+      <c r="R55" s="79"/>
+      <c r="S55" s="79"/>
+      <c r="T55" s="79"/>
+      <c r="U55" s="79"/>
+      <c r="V55" s="79"/>
+      <c r="W55" s="79"/>
+      <c r="X55" s="79"/>
+      <c r="Y55" s="79"/>
+      <c r="Z55" s="79"/>
     </row>
     <row r="56" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B56" s="94" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C56" s="96" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D56" s="96" t="s">
-        <v>258</v>
+        <v>72</v>
       </c>
       <c r="E56" s="97" t="s">
         <v>254</v>
@@ -5223,98 +5321,62 @@
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="B57" s="75" t="s">
-        <v>169</v>
-      </c>
-      <c r="C57" s="75" t="s">
+    <row r="57" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="94" t="s">
+        <v>255</v>
+      </c>
+      <c r="C57" s="96" t="s">
+        <v>263</v>
+      </c>
+      <c r="D57" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="97" t="s">
+        <v>254</v>
+      </c>
+      <c r="F57" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="C58" s="96" t="s">
+        <v>262</v>
+      </c>
+      <c r="D58" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="F58" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="D57" s="75" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="76"/>
-      <c r="F57" s="77" t="s">
-        <v>107</v>
-      </c>
-      <c r="G57" s="78"/>
-      <c r="H57" s="79"/>
-      <c r="I57" s="79"/>
-      <c r="J57" s="79"/>
-      <c r="K57" s="79"/>
-      <c r="L57" s="79"/>
-      <c r="M57" s="79"/>
-      <c r="N57" s="79"/>
-      <c r="O57" s="79"/>
-      <c r="P57" s="79"/>
-      <c r="Q57" s="79"/>
-      <c r="R57" s="79"/>
-      <c r="S57" s="79"/>
-      <c r="T57" s="79"/>
-      <c r="U57" s="79"/>
-      <c r="V57" s="79"/>
-      <c r="W57" s="79"/>
-      <c r="X57" s="79"/>
-      <c r="Y57" s="79"/>
-      <c r="Z57" s="79"/>
-    </row>
-    <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
+      <c r="B59" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="C59" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="C58" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="D58" s="25" t="s">
+      <c r="D59" s="25" t="s">
         <v>30</v>
-      </c>
-      <c r="E58" s="80"/>
-      <c r="F58" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G58" s="81"/>
-      <c r="H58" s="82"/>
-      <c r="I58" s="82"/>
-      <c r="J58" s="82"/>
-      <c r="K58" s="82"/>
-      <c r="L58" s="82"/>
-      <c r="M58" s="82"/>
-      <c r="N58" s="82"/>
-      <c r="O58" s="82"/>
-      <c r="P58" s="82"/>
-      <c r="Q58" s="82"/>
-      <c r="R58" s="82"/>
-      <c r="S58" s="82"/>
-      <c r="T58" s="82"/>
-      <c r="U58" s="82"/>
-      <c r="V58" s="82"/>
-      <c r="W58" s="82"/>
-      <c r="X58" s="82"/>
-      <c r="Y58" s="82"/>
-      <c r="Z58" s="82"/>
-    </row>
-    <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="C59" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>177</v>
       </c>
       <c r="E59" s="80"/>
       <c r="F59" s="28" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
       <c r="G59" s="81"/>
       <c r="H59" s="82"/>
@@ -5337,108 +5399,150 @@
       <c r="Y59" s="82"/>
       <c r="Z59" s="82"/>
     </row>
-    <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="25" t="s">
+    <row r="60" spans="1:26" s="98" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C60" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="D60" s="98" t="s">
+        <v>46</v>
+      </c>
+      <c r="E60" s="97" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="E61" s="80"/>
+      <c r="F61" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="G61" s="81"/>
+      <c r="H61" s="82"/>
+      <c r="I61" s="82"/>
+      <c r="J61" s="82"/>
+      <c r="K61" s="82"/>
+      <c r="L61" s="82"/>
+      <c r="M61" s="82"/>
+      <c r="N61" s="82"/>
+      <c r="O61" s="82"/>
+      <c r="P61" s="82"/>
+      <c r="Q61" s="82"/>
+      <c r="R61" s="82"/>
+      <c r="S61" s="82"/>
+      <c r="T61" s="82"/>
+      <c r="U61" s="82"/>
+      <c r="V61" s="82"/>
+      <c r="W61" s="82"/>
+      <c r="X61" s="82"/>
+      <c r="Y61" s="82"/>
+      <c r="Z61" s="82"/>
+    </row>
+    <row r="62" spans="1:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B62" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="B60" s="25" t="s">
+      <c r="C62" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="D62" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62" s="80"/>
+      <c r="F62" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="D60" s="25" t="s">
+      <c r="G62" s="81"/>
+      <c r="H62" s="82"/>
+      <c r="I62" s="82"/>
+      <c r="J62" s="82"/>
+      <c r="K62" s="82"/>
+      <c r="L62" s="82"/>
+      <c r="M62" s="82"/>
+      <c r="N62" s="82"/>
+      <c r="O62" s="82"/>
+      <c r="P62" s="82"/>
+      <c r="Q62" s="82"/>
+      <c r="R62" s="82"/>
+      <c r="S62" s="82"/>
+      <c r="T62" s="82"/>
+      <c r="U62" s="82"/>
+      <c r="V62" s="82"/>
+      <c r="W62" s="82"/>
+      <c r="X62" s="82"/>
+      <c r="Y62" s="82"/>
+      <c r="Z62" s="82"/>
+    </row>
+    <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D63" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E60" s="80"/>
-      <c r="F60" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="G60" s="81"/>
-      <c r="H60" s="82"/>
-      <c r="I60" s="82"/>
-      <c r="J60" s="82"/>
-      <c r="K60" s="82"/>
-      <c r="L60" s="82"/>
-      <c r="M60" s="82"/>
-      <c r="N60" s="82"/>
-      <c r="O60" s="82"/>
-      <c r="P60" s="82"/>
-      <c r="Q60" s="82"/>
-      <c r="R60" s="82"/>
-      <c r="S60" s="82"/>
-      <c r="T60" s="82"/>
-      <c r="U60" s="82"/>
-      <c r="V60" s="82"/>
-      <c r="W60" s="82"/>
-      <c r="X60" s="82"/>
-      <c r="Y60" s="82"/>
-      <c r="Z60" s="82"/>
-    </row>
-    <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E61" s="9"/>
-      <c r="F61" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="G61" s="83"/>
-      <c r="H61" s="84"/>
-      <c r="I61" s="84"/>
-      <c r="J61" s="84"/>
-      <c r="K61" s="84"/>
-      <c r="L61" s="84"/>
-      <c r="M61" s="84"/>
-      <c r="N61" s="84"/>
-      <c r="O61" s="84"/>
-      <c r="P61" s="84"/>
-      <c r="Q61" s="84"/>
-      <c r="R61" s="84"/>
-      <c r="S61" s="84"/>
-      <c r="T61" s="84"/>
-      <c r="U61" s="84"/>
-      <c r="V61" s="84"/>
-      <c r="W61" s="84"/>
-      <c r="X61" s="84"/>
-      <c r="Y61" s="84"/>
-      <c r="Z61" s="84"/>
-    </row>
-    <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="85"/>
-      <c r="B62" s="85"/>
-      <c r="C62" s="85"/>
-      <c r="D62" s="85"/>
-      <c r="E62" s="86"/>
-      <c r="F62" s="87"/>
-      <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="85"/>
-      <c r="B63" s="85"/>
-      <c r="C63" s="85"/>
-      <c r="D63" s="85"/>
-      <c r="E63" s="86"/>
-      <c r="F63" s="87"/>
-      <c r="G63" s="5"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G63" s="83"/>
+      <c r="H63" s="84"/>
+      <c r="I63" s="84"/>
+      <c r="J63" s="84"/>
+      <c r="K63" s="84"/>
+      <c r="L63" s="84"/>
+      <c r="M63" s="84"/>
+      <c r="N63" s="84"/>
+      <c r="O63" s="84"/>
+      <c r="P63" s="84"/>
+      <c r="Q63" s="84"/>
+      <c r="R63" s="84"/>
+      <c r="S63" s="84"/>
+      <c r="T63" s="84"/>
+      <c r="U63" s="84"/>
+      <c r="V63" s="84"/>
+      <c r="W63" s="84"/>
+      <c r="X63" s="84"/>
+      <c r="Y63" s="84"/>
+      <c r="Z63" s="84"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
+      <c r="A64" s="85"/>
+      <c r="B64" s="85"/>
+      <c r="C64" s="85"/>
+      <c r="D64" s="85"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="87"/>
       <c r="G64" s="5"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="A65" s="85"/>
+      <c r="B65" s="85"/>
+      <c r="C65" s="85"/>
+      <c r="D65" s="85"/>
+      <c r="E65" s="86"/>
+      <c r="F65" s="87"/>
       <c r="G65" s="5"/>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5446,118 +5550,52 @@
       <c r="G66" s="5"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G67" s="5"/>
+    </row>
+    <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="G68" s="5"/>
+    </row>
+    <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B69" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D69" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E67" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F67" s="7" t="s">
+      <c r="F69" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G67" s="5"/>
-    </row>
-    <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="B68" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="C68" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="D68" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68" s="45"/>
-      <c r="F68" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="88"/>
-      <c r="H68" s="89"/>
-      <c r="I68" s="89"/>
-      <c r="J68" s="89"/>
-      <c r="K68" s="89"/>
-      <c r="L68" s="89"/>
-      <c r="M68" s="89"/>
-      <c r="N68" s="89"/>
-      <c r="O68" s="89"/>
-      <c r="P68" s="89"/>
-      <c r="Q68" s="89"/>
-      <c r="R68" s="89"/>
-      <c r="S68" s="89"/>
-      <c r="T68" s="89"/>
-      <c r="U68" s="89"/>
-      <c r="V68" s="89"/>
-      <c r="W68" s="89"/>
-      <c r="X68" s="89"/>
-      <c r="Y68" s="89"/>
-      <c r="Z68" s="89"/>
-    </row>
-    <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="B69" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="C69" s="90" t="s">
-        <v>194</v>
-      </c>
-      <c r="D69" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E69" s="45"/>
-      <c r="F69" s="44" t="s">
-        <v>195</v>
-      </c>
-      <c r="G69" s="88"/>
-      <c r="H69" s="89"/>
-      <c r="I69" s="89"/>
-      <c r="J69" s="89"/>
-      <c r="K69" s="89"/>
-      <c r="L69" s="89"/>
-      <c r="M69" s="89"/>
-      <c r="N69" s="89"/>
-      <c r="O69" s="89"/>
-      <c r="P69" s="89"/>
-      <c r="Q69" s="89"/>
-      <c r="R69" s="89"/>
-      <c r="S69" s="89"/>
-      <c r="T69" s="89"/>
-      <c r="U69" s="89"/>
-      <c r="V69" s="89"/>
-      <c r="W69" s="89"/>
-      <c r="X69" s="89"/>
-      <c r="Y69" s="89"/>
-      <c r="Z69" s="89"/>
+      <c r="G69" s="5"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="45" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B70" s="45" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D70" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E70" s="45"/>
       <c r="F70" s="44" t="s">
-        <v>199</v>
+        <v>13</v>
       </c>
       <c r="G70" s="88"/>
       <c r="H70" s="89"/>
@@ -5582,20 +5620,20 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="45" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C71" s="90" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D71" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E71" s="45"/>
       <c r="F71" s="44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G71" s="88"/>
       <c r="H71" s="89"/>
@@ -5620,20 +5658,20 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B72" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="B72" s="45" t="s">
-        <v>203</v>
-      </c>
       <c r="C72" s="45" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D72" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E72" s="45"/>
       <c r="F72" s="44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G72" s="88"/>
       <c r="H72" s="89"/>
@@ -5658,20 +5696,20 @@
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="45" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B73" s="45" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C73" s="90" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D73" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E73" s="45"/>
       <c r="F73" s="44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G73" s="88"/>
       <c r="H73" s="89"/>
@@ -5696,20 +5734,20 @@
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B74" s="45" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C74" s="45" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D74" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E74" s="45"/>
       <c r="F74" s="44" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="G74" s="88"/>
       <c r="H74" s="89"/>
@@ -5734,20 +5772,20 @@
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B75" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="C75" s="91" t="s">
-        <v>212</v>
+        <v>205</v>
+      </c>
+      <c r="C75" s="90" t="s">
+        <v>206</v>
       </c>
       <c r="D75" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E75" s="45"/>
       <c r="F75" s="44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G75" s="88"/>
       <c r="H75" s="89"/>
@@ -5772,20 +5810,20 @@
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B76" s="45" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C76" s="45" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D76" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E76" s="45"/>
       <c r="F76" s="44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G76" s="88"/>
       <c r="H76" s="89"/>
@@ -5810,20 +5848,20 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="45" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B77" s="45" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C77" s="91" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D77" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E77" s="45"/>
       <c r="F77" s="44" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="G77" s="88"/>
       <c r="H77" s="89"/>
@@ -5848,20 +5886,20 @@
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="45" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B78" s="45" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="C78" s="45" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="D78" s="45" t="s">
         <v>86</v>
       </c>
       <c r="E78" s="45"/>
       <c r="F78" s="44" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G78" s="88"/>
       <c r="H78" s="89"/>
@@ -5886,20 +5924,20 @@
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="45" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
       <c r="B79" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="C79" s="45" t="s">
-        <v>185</v>
+        <v>214</v>
+      </c>
+      <c r="C79" s="91" t="s">
+        <v>215</v>
       </c>
       <c r="D79" s="45" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="E79" s="45"/>
       <c r="F79" s="44" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="G79" s="88"/>
       <c r="H79" s="89"/>
@@ -5923,138 +5961,134 @@
       <c r="Z79" s="89"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="G80" s="5"/>
+      <c r="A80" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="C80" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="D80" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" s="45"/>
+      <c r="F80" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="G80" s="88"/>
+      <c r="H80" s="89"/>
+      <c r="I80" s="89"/>
+      <c r="J80" s="89"/>
+      <c r="K80" s="89"/>
+      <c r="L80" s="89"/>
+      <c r="M80" s="89"/>
+      <c r="N80" s="89"/>
+      <c r="O80" s="89"/>
+      <c r="P80" s="89"/>
+      <c r="Q80" s="89"/>
+      <c r="R80" s="89"/>
+      <c r="S80" s="89"/>
+      <c r="T80" s="89"/>
+      <c r="U80" s="89"/>
+      <c r="V80" s="89"/>
+      <c r="W80" s="89"/>
+      <c r="X80" s="89"/>
+      <c r="Y80" s="89"/>
+      <c r="Z80" s="89"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G81" s="5"/>
+      <c r="A81" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="C81" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="D81" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" s="45"/>
+      <c r="F81" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="G81" s="88"/>
+      <c r="H81" s="89"/>
+      <c r="I81" s="89"/>
+      <c r="J81" s="89"/>
+      <c r="K81" s="89"/>
+      <c r="L81" s="89"/>
+      <c r="M81" s="89"/>
+      <c r="N81" s="89"/>
+      <c r="O81" s="89"/>
+      <c r="P81" s="89"/>
+      <c r="Q81" s="89"/>
+      <c r="R81" s="89"/>
+      <c r="S81" s="89"/>
+      <c r="T81" s="89"/>
+      <c r="U81" s="89"/>
+      <c r="V81" s="89"/>
+      <c r="W81" s="89"/>
+      <c r="X81" s="89"/>
+      <c r="Y81" s="89"/>
+      <c r="Z81" s="89"/>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="G82" s="5"/>
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G83" s="5"/>
+    </row>
+    <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="G84" s="5"/>
+    </row>
+    <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B85" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D85" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E85" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E83" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F83" s="7" t="s">
+      <c r="F85" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G83" s="5"/>
-    </row>
-    <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="B84" s="45" t="s">
-        <v>220</v>
-      </c>
-      <c r="C84" s="90" t="s">
-        <v>221</v>
-      </c>
-      <c r="D84" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E84" s="45"/>
-      <c r="F84" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G84" s="88"/>
-      <c r="H84" s="89"/>
-      <c r="I84" s="89"/>
-      <c r="J84" s="89"/>
-      <c r="K84" s="89"/>
-      <c r="L84" s="89"/>
-      <c r="M84" s="89"/>
-      <c r="N84" s="89"/>
-      <c r="O84" s="89"/>
-      <c r="P84" s="89"/>
-      <c r="Q84" s="89"/>
-      <c r="R84" s="89"/>
-      <c r="S84" s="89"/>
-      <c r="T84" s="89"/>
-      <c r="U84" s="89"/>
-      <c r="V84" s="89"/>
-      <c r="W84" s="89"/>
-      <c r="X84" s="89"/>
-      <c r="Y84" s="89"/>
-      <c r="Z84" s="89"/>
-    </row>
-    <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="B85" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="C85" s="90" t="s">
-        <v>224</v>
-      </c>
-      <c r="D85" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E85" s="45"/>
-      <c r="F85" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G85" s="45" t="s">
-        <v>225</v>
-      </c>
-      <c r="H85" s="89"/>
-      <c r="I85" s="89"/>
-      <c r="J85" s="89"/>
-      <c r="K85" s="89"/>
-      <c r="L85" s="89"/>
-      <c r="M85" s="89"/>
-      <c r="N85" s="89"/>
-      <c r="O85" s="89"/>
-      <c r="P85" s="89"/>
-      <c r="Q85" s="89"/>
-      <c r="R85" s="89"/>
-      <c r="S85" s="89"/>
-      <c r="T85" s="89"/>
-      <c r="U85" s="89"/>
-      <c r="V85" s="89"/>
-      <c r="W85" s="89"/>
-      <c r="X85" s="89"/>
-      <c r="Y85" s="89"/>
-      <c r="Z85" s="89"/>
+      <c r="G85" s="5"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="45" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B86" s="45" t="s">
-        <v>28</v>
+        <v>219</v>
       </c>
       <c r="C86" s="90" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D86" s="45" t="s">
-        <v>228</v>
+        <v>16</v>
       </c>
       <c r="E86" s="45"/>
       <c r="F86" s="44" t="s">
-        <v>229</v>
-      </c>
-      <c r="G86" s="45" t="s">
-        <v>230</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G86" s="88"/>
       <c r="H86" s="89"/>
       <c r="I86" s="89"/>
       <c r="J86" s="89"/>
@@ -6077,22 +6111,24 @@
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="45" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B87" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="C87" s="45" t="s">
-        <v>232</v>
+        <v>222</v>
+      </c>
+      <c r="C87" s="90" t="s">
+        <v>223</v>
       </c>
       <c r="D87" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E87" s="92"/>
+        <v>11</v>
+      </c>
+      <c r="E87" s="45"/>
       <c r="F87" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G87" s="88"/>
+        <v>13</v>
+      </c>
+      <c r="G87" s="45" t="s">
+        <v>224</v>
+      </c>
       <c r="H87" s="89"/>
       <c r="I87" s="89"/>
       <c r="J87" s="89"/>
@@ -6115,22 +6151,24 @@
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="45" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B88" s="45" t="s">
-        <v>234</v>
-      </c>
-      <c r="C88" s="45" t="s">
-        <v>235</v>
+        <v>28</v>
+      </c>
+      <c r="C88" s="90" t="s">
+        <v>226</v>
       </c>
       <c r="D88" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" s="92"/>
+        <v>227</v>
+      </c>
+      <c r="E88" s="45"/>
       <c r="F88" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="G88" s="88"/>
+        <v>228</v>
+      </c>
+      <c r="G88" s="45" t="s">
+        <v>229</v>
+      </c>
       <c r="H88" s="89"/>
       <c r="I88" s="89"/>
       <c r="J88" s="89"/>
@@ -6153,20 +6191,20 @@
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="45" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B89" s="45" t="s">
-        <v>237</v>
-      </c>
-      <c r="C89" s="90" t="s">
-        <v>238</v>
+        <v>192</v>
+      </c>
+      <c r="C89" s="45" t="s">
+        <v>231</v>
       </c>
       <c r="D89" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E89" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="E89" s="92"/>
       <c r="F89" s="44" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="G89" s="88"/>
       <c r="H89" s="89"/>
@@ -6191,20 +6229,20 @@
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="45" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B90" s="45" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C90" s="45" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D90" s="45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E90" s="92"/>
       <c r="F90" s="44" t="s">
-        <v>54</v>
+        <v>177</v>
       </c>
       <c r="G90" s="88"/>
       <c r="H90" s="89"/>
@@ -6229,20 +6267,20 @@
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="45" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B91" s="45" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C91" s="90" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D91" s="45" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E91" s="45"/>
       <c r="F91" s="44" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="G91" s="88"/>
       <c r="H91" s="89"/>
@@ -6267,20 +6305,20 @@
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="45" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B92" s="45" t="s">
-        <v>109</v>
+        <v>239</v>
       </c>
       <c r="C92" s="45" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D92" s="45" t="s">
-        <v>247</v>
-      </c>
-      <c r="E92" s="45"/>
+        <v>30</v>
+      </c>
+      <c r="E92" s="92"/>
       <c r="F92" s="44" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="G92" s="88"/>
       <c r="H92" s="89"/>
@@ -6305,20 +6343,20 @@
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="45" t="s">
-        <v>174</v>
+        <v>241</v>
       </c>
       <c r="B93" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="C93" s="45" t="s">
-        <v>248</v>
+        <v>242</v>
+      </c>
+      <c r="C93" s="90" t="s">
+        <v>243</v>
       </c>
       <c r="D93" s="45" t="s">
         <v>30</v>
       </c>
       <c r="E93" s="45"/>
       <c r="F93" s="44" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
       <c r="G93" s="88"/>
       <c r="H93" s="89"/>
@@ -6343,20 +6381,20 @@
     </row>
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="45" t="s">
-        <v>179</v>
+        <v>244</v>
       </c>
       <c r="B94" s="45" t="s">
-        <v>180</v>
+        <v>109</v>
       </c>
       <c r="C94" s="45" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D94" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E94" s="92"/>
+        <v>246</v>
+      </c>
+      <c r="E94" s="45"/>
       <c r="F94" s="44" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="G94" s="88"/>
       <c r="H94" s="89"/>
@@ -6381,20 +6419,20 @@
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="45" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B95" s="45" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>185</v>
+        <v>247</v>
       </c>
       <c r="D95" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E95" s="92"/>
+        <v>30</v>
+      </c>
+      <c r="E95" s="45"/>
       <c r="F95" s="44" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G95" s="88"/>
       <c r="H95" s="89"/>
@@ -6418,56 +6456,126 @@
       <c r="Z95" s="89"/>
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="G96" s="5"/>
-    </row>
-    <row r="97" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="93"/>
-      <c r="G97" s="5"/>
-    </row>
-    <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B96" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="C96" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="D96" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E96" s="92"/>
+      <c r="F96" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="G96" s="88"/>
+      <c r="H96" s="89"/>
+      <c r="I96" s="89"/>
+      <c r="J96" s="89"/>
+      <c r="K96" s="89"/>
+      <c r="L96" s="89"/>
+      <c r="M96" s="89"/>
+      <c r="N96" s="89"/>
+      <c r="O96" s="89"/>
+      <c r="P96" s="89"/>
+      <c r="Q96" s="89"/>
+      <c r="R96" s="89"/>
+      <c r="S96" s="89"/>
+      <c r="T96" s="89"/>
+      <c r="U96" s="89"/>
+      <c r="V96" s="89"/>
+      <c r="W96" s="89"/>
+      <c r="X96" s="89"/>
+      <c r="Y96" s="89"/>
+      <c r="Z96" s="89"/>
+    </row>
+    <row r="97" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="B97" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="C97" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="D97" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E97" s="92"/>
+      <c r="F97" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="G97" s="88"/>
+      <c r="H97" s="89"/>
+      <c r="I97" s="89"/>
+      <c r="J97" s="89"/>
+      <c r="K97" s="89"/>
+      <c r="L97" s="89"/>
+      <c r="M97" s="89"/>
+      <c r="N97" s="89"/>
+      <c r="O97" s="89"/>
+      <c r="P97" s="89"/>
+      <c r="Q97" s="89"/>
+      <c r="R97" s="89"/>
+      <c r="S97" s="89"/>
+      <c r="T97" s="89"/>
+      <c r="U97" s="89"/>
+      <c r="V97" s="89"/>
+      <c r="W97" s="89"/>
+      <c r="X97" s="89"/>
+      <c r="Y97" s="89"/>
+      <c r="Z97" s="89"/>
+    </row>
+    <row r="98" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="93"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G101" s="5"/>
     </row>
-    <row r="102" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G102" s="5"/>
     </row>
-    <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G103" s="5"/>
     </row>
-    <row r="104" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G104" s="5"/>
     </row>
-    <row r="105" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G112" s="5"/>
     </row>
     <row r="113" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9145,6 +9253,12 @@
     </row>
     <row r="1004" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1004" s="5"/>
+    </row>
+    <row r="1005" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1005" s="5"/>
+    </row>
+    <row r="1006" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1006" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>